<commit_message>
047 Week 6/5 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="112">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -648,10 +648,10 @@
     <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1127,7 +1127,9 @@
       <c r="G6" s="12">
         <v>30.0</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="13">
+        <v>28.0</v>
+      </c>
       <c r="I6" s="15"/>
       <c r="J6" s="14"/>
       <c r="K6" s="15"/>
@@ -1148,7 +1150,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>158</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7">
@@ -1170,7 +1172,9 @@
       <c r="G7" s="12">
         <v>25.0</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="13">
+        <v>24.0</v>
+      </c>
       <c r="I7" s="15"/>
       <c r="J7" s="14"/>
       <c r="K7" s="15"/>
@@ -1191,7 +1195,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>138</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8">
@@ -1213,7 +1217,9 @@
       <c r="G8" s="12">
         <v>42.0</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="13">
+        <v>28.0</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="14"/>
       <c r="K8" s="15"/>
@@ -1234,7 +1240,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>165</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9">
@@ -1256,7 +1262,9 @@
       <c r="G9" s="12">
         <v>27.0</v>
       </c>
-      <c r="H9" s="14"/>
+      <c r="H9" s="13">
+        <v>34.0</v>
+      </c>
       <c r="I9" s="15"/>
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
@@ -1277,7 +1285,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10">
@@ -1297,7 +1305,9 @@
       <c r="G10" s="12">
         <v>39.0</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="13">
+        <v>30.0</v>
+      </c>
       <c r="I10" s="15"/>
       <c r="J10" s="14"/>
       <c r="K10" s="15"/>
@@ -1318,7 +1328,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11">
@@ -1373,7 +1383,9 @@
       <c r="G12" s="12">
         <v>19.0</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="13">
+        <v>29.0</v>
+      </c>
       <c r="I12" s="15"/>
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
@@ -1394,7 +1406,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>138</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13">
@@ -1412,7 +1424,9 @@
         <v>26.0</v>
       </c>
       <c r="G13" s="15"/>
-      <c r="H13" s="14"/>
+      <c r="H13" s="13">
+        <v>32.0</v>
+      </c>
       <c r="I13" s="15"/>
       <c r="J13" s="14"/>
       <c r="K13" s="15"/>
@@ -1433,7 +1447,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14">
@@ -1535,7 +1549,9 @@
       <c r="G16" s="12">
         <v>36.0</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="13">
+        <v>9.0</v>
+      </c>
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
       <c r="K16" s="15"/>
@@ -1556,7 +1572,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17">
@@ -1578,7 +1594,9 @@
       <c r="G17" s="12">
         <v>34.0</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="13">
+        <v>33.0</v>
+      </c>
       <c r="I17" s="15"/>
       <c r="J17" s="14"/>
       <c r="K17" s="15"/>
@@ -1599,7 +1617,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>158</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18">
@@ -1621,7 +1639,9 @@
       <c r="G18" s="12">
         <v>34.0</v>
       </c>
-      <c r="H18" s="14"/>
+      <c r="H18" s="13">
+        <v>34.0</v>
+      </c>
       <c r="I18" s="15"/>
       <c r="J18" s="14"/>
       <c r="K18" s="15"/>
@@ -1642,7 +1662,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19">
@@ -1662,7 +1682,9 @@
       <c r="G19" s="12">
         <v>30.0</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="13">
+        <v>27.0</v>
+      </c>
       <c r="I19" s="15"/>
       <c r="J19" s="14"/>
       <c r="K19" s="15"/>
@@ -1683,7 +1705,7 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20">
@@ -1703,7 +1725,9 @@
       <c r="G20" s="12">
         <v>39.0</v>
       </c>
-      <c r="H20" s="14"/>
+      <c r="H20" s="13">
+        <v>31.0</v>
+      </c>
       <c r="I20" s="15"/>
       <c r="J20" s="14"/>
       <c r="K20" s="15"/>
@@ -1724,7 +1748,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>142</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21">
@@ -1744,7 +1768,9 @@
       <c r="G21" s="12">
         <v>35.0</v>
       </c>
-      <c r="H21" s="14"/>
+      <c r="H21" s="13">
+        <v>35.0</v>
+      </c>
       <c r="I21" s="15"/>
       <c r="J21" s="14"/>
       <c r="K21" s="15"/>
@@ -1765,7 +1791,7 @@
       <c r="Z21" s="16"/>
       <c r="AA21" s="14">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22">
@@ -1787,7 +1813,9 @@
       <c r="G22" s="12">
         <v>37.0</v>
       </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="13">
+        <v>35.0</v>
+      </c>
       <c r="I22" s="15"/>
       <c r="J22" s="14"/>
       <c r="K22" s="15"/>
@@ -1808,7 +1836,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -1856,7 +1884,9 @@
       <c r="G24" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="21" t="s">
+        <v>68</v>
+      </c>
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
@@ -1896,7 +1926,9 @@
       <c r="G25" s="24">
         <v>42.0</v>
       </c>
-      <c r="H25" s="24"/>
+      <c r="H25" s="24">
+        <v>35.0</v>
+      </c>
       <c r="I25" s="24"/>
       <c r="J25" s="24"/>
       <c r="K25" s="24"/>
@@ -2116,7 +2148,9 @@
       <c r="F5" s="13">
         <v>33.0</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="12">
+        <v>28.0</v>
+      </c>
       <c r="H5" s="14"/>
       <c r="I5" s="15"/>
       <c r="J5" s="14"/>
@@ -2138,7 +2172,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>114</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6">
@@ -2155,7 +2189,9 @@
         <v>33.0</v>
       </c>
       <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
+      <c r="G6" s="12">
+        <v>29.0</v>
+      </c>
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
       <c r="J6" s="14"/>
@@ -2177,7 +2213,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7">
@@ -2194,7 +2230,9 @@
       <c r="F7" s="13">
         <v>31.0</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="12">
+        <v>29.0</v>
+      </c>
       <c r="H7" s="14"/>
       <c r="I7" s="15"/>
       <c r="J7" s="14"/>
@@ -2216,7 +2254,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
@@ -2235,7 +2273,9 @@
       <c r="F8" s="13">
         <v>31.0</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="12">
+        <v>31.0</v>
+      </c>
       <c r="H8" s="14"/>
       <c r="I8" s="15"/>
       <c r="J8" s="14"/>
@@ -2257,7 +2297,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>127</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9">
@@ -2276,7 +2316,9 @@
       <c r="F9" s="13">
         <v>30.0</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="12">
+        <v>33.0</v>
+      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
       <c r="J9" s="14"/>
@@ -2298,7 +2340,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10">
@@ -2315,7 +2357,9 @@
         <v>33.0</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="12">
+        <v>38.0</v>
+      </c>
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
       <c r="J10" s="14"/>
@@ -2337,7 +2381,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11">
@@ -2352,7 +2396,9 @@
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="12">
+        <v>31.0</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
       <c r="J11" s="14"/>
@@ -2374,7 +2420,7 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12">
@@ -2393,7 +2439,9 @@
       <c r="F12" s="13">
         <v>38.0</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="12">
+        <v>34.0</v>
+      </c>
       <c r="H12" s="14"/>
       <c r="I12" s="15"/>
       <c r="J12" s="14"/>
@@ -2415,7 +2463,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13">
@@ -2434,7 +2482,9 @@
       <c r="F13" s="13">
         <v>27.0</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="12">
+        <v>35.0</v>
+      </c>
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
       <c r="J13" s="14"/>
@@ -2456,7 +2506,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14">
@@ -2549,7 +2599,9 @@
       <c r="F16" s="13">
         <v>27.0</v>
       </c>
-      <c r="G16" s="15"/>
+      <c r="G16" s="12">
+        <v>26.0</v>
+      </c>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
@@ -2571,7 +2623,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17">
@@ -2588,7 +2640,9 @@
       <c r="F17" s="13">
         <v>34.0</v>
       </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="12">
+        <v>29.0</v>
+      </c>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
       <c r="J17" s="14"/>
@@ -2610,7 +2664,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18">
@@ -2625,7 +2679,9 @@
       <c r="F18" s="12">
         <v>27.0</v>
       </c>
-      <c r="G18" s="15"/>
+      <c r="G18" s="12">
+        <v>26.0</v>
+      </c>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
       <c r="J18" s="15"/>
@@ -2647,7 +2703,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -2692,7 +2748,9 @@
       <c r="F20" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="G20" s="21"/>
+      <c r="G20" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
@@ -2730,7 +2788,9 @@
       <c r="F21" s="24">
         <v>38.0</v>
       </c>
-      <c r="G21" s="24"/>
+      <c r="G21" s="24">
+        <v>38.0</v>
+      </c>
       <c r="H21" s="24"/>
       <c r="I21" s="24"/>
       <c r="J21" s="24"/>
@@ -2787,10 +2847,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="31">
+        <v>14.0</v>
+      </c>
+      <c r="C2" s="32">
         <v>13.0</v>
-      </c>
-      <c r="C2" s="32">
-        <v>12.0</v>
       </c>
     </row>
     <row r="3">
@@ -2809,7 +2869,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="31">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="C4" s="32">
         <v>18.0</v>
@@ -2823,7 +2883,7 @@
         <v>15.0</v>
       </c>
       <c r="C5" s="32">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="6">
@@ -2831,10 +2891,10 @@
         <v>55</v>
       </c>
       <c r="B6" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="32">
         <v>-1.0</v>
-      </c>
-      <c r="C6" s="32">
-        <v>-2.0</v>
       </c>
     </row>
     <row r="7">
@@ -2922,7 +2982,7 @@
         <v>14.0</v>
       </c>
       <c r="C14" s="32">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="15">
@@ -2930,10 +2990,10 @@
         <v>64</v>
       </c>
       <c r="B15" s="31">
-        <v>33.0</v>
+        <v>32.0</v>
       </c>
       <c r="C15" s="32">
-        <v>31.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="16">
@@ -2952,7 +3012,7 @@
         <v>66</v>
       </c>
       <c r="B17" s="31">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C17" s="32">
         <v>7.0</v>
@@ -2963,7 +3023,7 @@
         <v>67</v>
       </c>
       <c r="B18" s="31">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="C18" s="32">
         <v>7.0</v>
@@ -2985,10 +3045,10 @@
         <v>101</v>
       </c>
       <c r="B20" s="31">
+        <v>21.0</v>
+      </c>
+      <c r="C20" s="32">
         <v>20.0</v>
-      </c>
-      <c r="C20" s="32">
-        <v>19.0</v>
       </c>
     </row>
     <row r="21">
@@ -3018,10 +3078,10 @@
         <v>97</v>
       </c>
       <c r="B23" s="31">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="C23" s="32">
-        <v>28.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="24">
@@ -3029,10 +3089,10 @@
         <v>100</v>
       </c>
       <c r="B24" s="34">
+        <v>27.0</v>
+      </c>
+      <c r="C24" s="35">
         <v>25.0</v>
-      </c>
-      <c r="C24" s="35">
-        <v>24.0</v>
       </c>
     </row>
     <row r="25">
@@ -7005,43 +7065,47 @@
       <c r="B6" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="43"/>
+      <c r="C6" s="42" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="13">
         <v>6.0</v>
       </c>
-      <c r="B7" s="41"/>
+      <c r="B7" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="C7" s="42"/>
     </row>
     <row r="8">
       <c r="A8" s="13">
         <v>7.0</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
     </row>
     <row r="9">
       <c r="A9" s="13">
         <v>8.0</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="43"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
     </row>
     <row r="10">
       <c r="A10" s="13">
         <v>9.0</v>
       </c>
       <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
+      <c r="C10" s="44"/>
       <c r="G10" s="14"/>
     </row>
     <row r="11">
       <c r="A11" s="13">
         <v>10.0</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="43"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
     </row>
     <row r="12">
       <c r="A12" s="13">
@@ -7062,14 +7126,14 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="41"/>
-      <c r="C14" s="43"/>
+      <c r="C14" s="44"/>
     </row>
     <row r="15">
       <c r="A15" s="13">
         <v>14.0</v>
       </c>
       <c r="B15" s="41"/>
-      <c r="C15" s="43"/>
+      <c r="C15" s="44"/>
     </row>
     <row r="16">
       <c r="A16" s="13">
@@ -7090,14 +7154,14 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="41"/>
-      <c r="C18" s="43"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19">
       <c r="A19" s="13">
         <v>18.0</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
     </row>
     <row r="20">
       <c r="A20" s="13">
@@ -7110,28 +7174,28 @@
       <c r="A21" s="13">
         <v>20.0</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
     </row>
     <row r="22">
       <c r="A22" s="13">
         <v>21.0</v>
       </c>
-      <c r="B22" s="44"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="42"/>
     </row>
     <row r="23">
       <c r="A23" s="13">
         <v>22.0</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
     </row>
     <row r="24">
       <c r="A24" s="13">
         <v>23.0</v>
       </c>
-      <c r="B24" s="44"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="42"/>
     </row>
     <row r="25">
@@ -12129,7 +12193,14 @@
         <f>'SUNDAY SINGLES'!G25</f>
         <v>42</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="49" t="str">
+        <f>'THURSDAY SINGLES'!G20</f>
+        <v>KEN PEEL</v>
+      </c>
+      <c r="E6" s="48">
+        <f>'THURSDAY SINGLES'!G21</f>
+        <v>38</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="13">
@@ -12137,13 +12208,20 @@
       </c>
       <c r="B7" s="48" t="str">
         <f>'SUNDAY SINGLES'!H24</f>
+        <v>ANDY THOMPSON</v>
+      </c>
+      <c r="C7" s="48">
+        <f>'SUNDAY SINGLES'!H25</f>
+        <v>35</v>
+      </c>
+      <c r="D7" s="49" t="str">
+        <f>'THURSDAY SINGLES'!H20</f>
         <v/>
       </c>
-      <c r="C7" s="48" t="str">
-        <f>'SUNDAY SINGLES'!H25</f>
+      <c r="E7" s="48" t="str">
+        <f>'THURSDAY SINGLES'!H21</f>
         <v/>
       </c>
-      <c r="D7" s="49"/>
     </row>
     <row r="8">
       <c r="A8" s="13">

</xml_diff>

<commit_message>
049 Week 7/6 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -305,9 +305,6 @@
     <t>25th Sept 25</t>
   </si>
   <si>
-    <t>STEW TAYLOR</t>
-  </si>
-  <si>
     <t>STEVE CONNOR</t>
   </si>
   <si>
@@ -339,6 +336,9 @@
   </si>
   <si>
     <t>MARTIN BROCKLEY</t>
+  </si>
+  <si>
+    <t>STEW LAWSON</t>
   </si>
   <si>
     <t>SUNDAY</t>
@@ -648,10 +648,10 @@
     <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1085,7 +1085,9 @@
         <v>24.0</v>
       </c>
       <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
+      <c r="I5" s="12">
+        <v>31.0</v>
+      </c>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
       <c r="L5" s="14"/>
@@ -1105,7 +1107,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>136</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6">
@@ -1130,7 +1132,9 @@
       <c r="H6" s="13">
         <v>28.0</v>
       </c>
-      <c r="I6" s="15"/>
+      <c r="I6" s="12">
+        <v>32.0</v>
+      </c>
       <c r="J6" s="14"/>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
@@ -1150,7 +1154,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>186</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7">
@@ -1175,7 +1179,9 @@
       <c r="H7" s="13">
         <v>24.0</v>
       </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="12">
+        <v>23.0</v>
+      </c>
       <c r="J7" s="14"/>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
@@ -1195,7 +1201,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>162</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8">
@@ -1220,7 +1226,9 @@
       <c r="H8" s="13">
         <v>28.0</v>
       </c>
-      <c r="I8" s="15"/>
+      <c r="I8" s="12">
+        <v>26.0</v>
+      </c>
       <c r="J8" s="14"/>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
@@ -1240,7 +1248,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9">
@@ -1386,7 +1394,9 @@
       <c r="H12" s="13">
         <v>29.0</v>
       </c>
-      <c r="I12" s="15"/>
+      <c r="I12" s="12">
+        <v>29.0</v>
+      </c>
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
@@ -1406,7 +1416,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>167</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13">
@@ -1597,7 +1607,9 @@
       <c r="H17" s="13">
         <v>33.0</v>
       </c>
-      <c r="I17" s="15"/>
+      <c r="I17" s="12">
+        <v>28.0</v>
+      </c>
       <c r="J17" s="14"/>
       <c r="K17" s="15"/>
       <c r="L17" s="14"/>
@@ -1617,7 +1629,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18">
@@ -1642,7 +1654,9 @@
       <c r="H18" s="13">
         <v>34.0</v>
       </c>
-      <c r="I18" s="15"/>
+      <c r="I18" s="12">
+        <v>28.0</v>
+      </c>
       <c r="J18" s="14"/>
       <c r="K18" s="15"/>
       <c r="L18" s="14"/>
@@ -1662,7 +1676,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>194</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19">
@@ -1685,7 +1699,9 @@
       <c r="H19" s="13">
         <v>27.0</v>
       </c>
-      <c r="I19" s="15"/>
+      <c r="I19" s="12">
+        <v>29.0</v>
+      </c>
       <c r="J19" s="14"/>
       <c r="K19" s="15"/>
       <c r="L19" s="14"/>
@@ -1705,7 +1721,7 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20">
@@ -1771,7 +1787,9 @@
       <c r="H21" s="13">
         <v>35.0</v>
       </c>
-      <c r="I21" s="15"/>
+      <c r="I21" s="12">
+        <v>34.0</v>
+      </c>
       <c r="J21" s="14"/>
       <c r="K21" s="15"/>
       <c r="L21" s="14"/>
@@ -1791,7 +1809,7 @@
       <c r="Z21" s="16"/>
       <c r="AA21" s="14">
         <f t="shared" si="1"/>
-        <v>161</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22">
@@ -1816,7 +1834,9 @@
       <c r="H22" s="13">
         <v>35.0</v>
       </c>
-      <c r="I22" s="15"/>
+      <c r="I22" s="12">
+        <v>28.0</v>
+      </c>
       <c r="J22" s="14"/>
       <c r="K22" s="15"/>
       <c r="L22" s="14"/>
@@ -1836,7 +1856,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>182</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -1887,7 +1907,9 @@
       <c r="H24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="I24" s="21"/>
+      <c r="I24" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
@@ -1929,7 +1951,9 @@
       <c r="H25" s="24">
         <v>35.0</v>
       </c>
-      <c r="I25" s="24"/>
+      <c r="I25" s="24">
+        <v>34.0</v>
+      </c>
       <c r="J25" s="24"/>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
@@ -2151,7 +2175,9 @@
       <c r="G5" s="12">
         <v>28.0</v>
       </c>
-      <c r="H5" s="14"/>
+      <c r="H5" s="13">
+        <v>37.0</v>
+      </c>
       <c r="I5" s="15"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
@@ -2172,7 +2198,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>142</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6">
@@ -2192,7 +2218,9 @@
       <c r="G6" s="12">
         <v>29.0</v>
       </c>
-      <c r="H6" s="14"/>
+      <c r="H6" s="13">
+        <v>34.0</v>
+      </c>
       <c r="I6" s="15"/>
       <c r="J6" s="14"/>
       <c r="K6" s="15"/>
@@ -2213,12 +2241,12 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="C7" s="12">
         <v>33.0</v>
@@ -2233,7 +2261,9 @@
       <c r="G7" s="12">
         <v>29.0</v>
       </c>
-      <c r="H7" s="14"/>
+      <c r="H7" s="13">
+        <v>33.0</v>
+      </c>
       <c r="I7" s="15"/>
       <c r="J7" s="14"/>
       <c r="K7" s="15"/>
@@ -2254,7 +2284,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>124</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8">
@@ -2276,7 +2306,9 @@
       <c r="G8" s="12">
         <v>31.0</v>
       </c>
-      <c r="H8" s="14"/>
+      <c r="H8" s="13">
+        <v>27.0</v>
+      </c>
       <c r="I8" s="15"/>
       <c r="J8" s="14"/>
       <c r="K8" s="15"/>
@@ -2297,7 +2329,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>158</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9">
@@ -2319,7 +2351,9 @@
       <c r="G9" s="12">
         <v>33.0</v>
       </c>
-      <c r="H9" s="14"/>
+      <c r="H9" s="13">
+        <v>35.0</v>
+      </c>
       <c r="I9" s="15"/>
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
@@ -2340,7 +2374,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>143</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10">
@@ -2360,7 +2394,9 @@
       <c r="G10" s="12">
         <v>38.0</v>
       </c>
-      <c r="H10" s="14"/>
+      <c r="H10" s="13">
+        <v>34.0</v>
+      </c>
       <c r="I10" s="15"/>
       <c r="J10" s="14"/>
       <c r="K10" s="15"/>
@@ -2381,12 +2417,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="12">
         <v>22.0</v>
@@ -2399,7 +2435,9 @@
       <c r="G11" s="12">
         <v>31.0</v>
       </c>
-      <c r="H11" s="14"/>
+      <c r="H11" s="13">
+        <v>31.0</v>
+      </c>
       <c r="I11" s="15"/>
       <c r="J11" s="14"/>
       <c r="K11" s="15"/>
@@ -2420,12 +2458,12 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="12">
         <v>28.0</v>
@@ -2442,7 +2480,9 @@
       <c r="G12" s="12">
         <v>34.0</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="13">
+        <v>31.0</v>
+      </c>
       <c r="I12" s="15"/>
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
@@ -2463,12 +2503,12 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="12">
         <v>31.0</v>
@@ -2485,7 +2525,9 @@
       <c r="G13" s="12">
         <v>35.0</v>
       </c>
-      <c r="H13" s="14"/>
+      <c r="H13" s="13">
+        <v>35.0</v>
+      </c>
       <c r="I13" s="15"/>
       <c r="J13" s="14"/>
       <c r="K13" s="15"/>
@@ -2506,7 +2548,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>161</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14">
@@ -2559,7 +2601,9 @@
         <v>33.0</v>
       </c>
       <c r="G15" s="15"/>
-      <c r="H15" s="14"/>
+      <c r="H15" s="13">
+        <v>28.0</v>
+      </c>
       <c r="I15" s="15"/>
       <c r="J15" s="14"/>
       <c r="K15" s="15"/>
@@ -2580,12 +2624,12 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" s="12">
         <v>32.0</v>
@@ -2643,7 +2687,9 @@
       <c r="G17" s="12">
         <v>29.0</v>
       </c>
-      <c r="H17" s="14"/>
+      <c r="H17" s="13">
+        <v>34.0</v>
+      </c>
       <c r="I17" s="15"/>
       <c r="J17" s="14"/>
       <c r="K17" s="15"/>
@@ -2664,12 +2710,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="12">
         <v>27.0</v>
@@ -2743,15 +2789,17 @@
         <v>56</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H20" s="21"/>
+      <c r="H20" s="21" t="s">
+        <v>51</v>
+      </c>
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
@@ -2791,7 +2839,9 @@
       <c r="G21" s="24">
         <v>38.0</v>
       </c>
-      <c r="H21" s="24"/>
+      <c r="H21" s="24">
+        <v>37.0</v>
+      </c>
       <c r="I21" s="24"/>
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
@@ -2836,10 +2886,10 @@
         <v>25</v>
       </c>
       <c r="B1" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>102</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2">
@@ -2847,10 +2897,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="31">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="C2" s="32">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="3">
@@ -2869,10 +2919,10 @@
         <v>53</v>
       </c>
       <c r="B4" s="31">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="C4" s="32">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="5">
@@ -2927,12 +2977,12 @@
         <v>19.0</v>
       </c>
       <c r="C9" s="32">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="B10" s="31">
         <v>7.0</v>
@@ -2946,10 +2996,10 @@
         <v>60</v>
       </c>
       <c r="B11" s="31">
+        <v>10.0</v>
+      </c>
+      <c r="C11" s="32">
         <v>9.0</v>
-      </c>
-      <c r="C11" s="32">
-        <v>8.0</v>
       </c>
     </row>
     <row r="12">
@@ -3012,10 +3062,10 @@
         <v>66</v>
       </c>
       <c r="B17" s="31">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="C17" s="32">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="18">
@@ -3042,7 +3092,7 @@
     </row>
     <row r="20">
       <c r="A20" s="33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="31">
         <v>21.0</v>
@@ -3053,7 +3103,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="31">
         <v>16.0</v>
@@ -3064,29 +3114,29 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B22" s="31">
         <v>15.0</v>
       </c>
       <c r="C22" s="32">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="31">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="C23" s="32">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="34">
         <v>27.0</v>
@@ -7005,13 +7055,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>105</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2">
@@ -7041,7 +7091,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>51</v>
@@ -7055,7 +7105,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6">
@@ -7066,7 +7116,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7">
@@ -7076,36 +7126,40 @@
       <c r="B7" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="42" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="13">
         <v>7.0</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="43"/>
     </row>
     <row r="9">
       <c r="A9" s="13">
         <v>8.0</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="43"/>
     </row>
     <row r="10">
       <c r="A10" s="13">
         <v>9.0</v>
       </c>
       <c r="B10" s="41"/>
-      <c r="C10" s="44"/>
+      <c r="C10" s="43"/>
       <c r="G10" s="14"/>
     </row>
     <row r="11">
       <c r="A11" s="13">
         <v>10.0</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="43"/>
     </row>
     <row r="12">
       <c r="A12" s="13">
@@ -7126,14 +7180,14 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="41"/>
-      <c r="C14" s="44"/>
+      <c r="C14" s="43"/>
     </row>
     <row r="15">
       <c r="A15" s="13">
         <v>14.0</v>
       </c>
       <c r="B15" s="41"/>
-      <c r="C15" s="44"/>
+      <c r="C15" s="43"/>
     </row>
     <row r="16">
       <c r="A16" s="13">
@@ -7154,14 +7208,14 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="41"/>
-      <c r="C18" s="44"/>
+      <c r="C18" s="43"/>
     </row>
     <row r="19">
       <c r="A19" s="13">
         <v>18.0</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="43"/>
     </row>
     <row r="20">
       <c r="A20" s="13">
@@ -7174,28 +7228,28 @@
       <c r="A21" s="13">
         <v>20.0</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="43"/>
     </row>
     <row r="22">
       <c r="A22" s="13">
         <v>21.0</v>
       </c>
-      <c r="B22" s="43"/>
+      <c r="B22" s="44"/>
       <c r="C22" s="42"/>
     </row>
     <row r="23">
       <c r="A23" s="13">
         <v>22.0</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="43"/>
     </row>
     <row r="24">
       <c r="A24" s="13">
         <v>23.0</v>
       </c>
-      <c r="B24" s="43"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="42"/>
     </row>
     <row r="25">
@@ -12082,7 +12136,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>108</v>
@@ -12216,11 +12270,11 @@
       </c>
       <c r="D7" s="49" t="str">
         <f>'THURSDAY SINGLES'!H20</f>
-        <v/>
-      </c>
-      <c r="E7" s="48" t="str">
+        <v>BAZ MASON</v>
+      </c>
+      <c r="E7" s="48">
         <f>'THURSDAY SINGLES'!H21</f>
-        <v/>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
@@ -12229,11 +12283,11 @@
       </c>
       <c r="B8" s="48" t="str">
         <f>'SUNDAY SINGLES'!I24</f>
-        <v/>
-      </c>
-      <c r="C8" s="48" t="str">
+        <v>SCOTT LEONARDE</v>
+      </c>
+      <c r="C8" s="48">
         <f>'SUNDAY SINGLES'!I25</f>
-        <v/>
+        <v>34</v>
       </c>
       <c r="D8" s="49"/>
     </row>

</xml_diff>

<commit_message>
050 Week 8/7 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>WEEKLY WINNER</t>
+  </si>
+  <si>
+    <t>FRED HOLINGWORTH</t>
   </si>
   <si>
     <t>WINNERS SCORE</t>
@@ -1088,7 +1091,9 @@
       <c r="I5" s="12">
         <v>31.0</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="J5" s="13">
+        <v>27.0</v>
+      </c>
       <c r="K5" s="15"/>
       <c r="L5" s="14"/>
       <c r="M5" s="15"/>
@@ -1107,7 +1112,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>167</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6">
@@ -1135,7 +1140,9 @@
       <c r="I6" s="12">
         <v>32.0</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="13">
+        <v>31.0</v>
+      </c>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
       <c r="M6" s="15"/>
@@ -1154,7 +1161,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>218</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7">
@@ -1229,7 +1236,9 @@
       <c r="I8" s="12">
         <v>26.0</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="13">
+        <v>30.0</v>
+      </c>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
       <c r="M8" s="15"/>
@@ -1248,7 +1257,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>219</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9">
@@ -1397,7 +1406,9 @@
       <c r="I12" s="12">
         <v>29.0</v>
       </c>
-      <c r="J12" s="14"/>
+      <c r="J12" s="13">
+        <v>31.0</v>
+      </c>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
       <c r="M12" s="15"/>
@@ -1416,7 +1427,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>196</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13">
@@ -1438,7 +1449,9 @@
         <v>32.0</v>
       </c>
       <c r="I13" s="15"/>
-      <c r="J13" s="14"/>
+      <c r="J13" s="13">
+        <v>26.0</v>
+      </c>
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
       <c r="M13" s="15"/>
@@ -1457,7 +1470,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14">
@@ -1477,7 +1490,9 @@
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="14"/>
+      <c r="J14" s="13">
+        <v>34.0</v>
+      </c>
       <c r="K14" s="15"/>
       <c r="L14" s="14"/>
       <c r="M14" s="15"/>
@@ -1496,7 +1511,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15">
@@ -1610,7 +1625,9 @@
       <c r="I17" s="12">
         <v>28.0</v>
       </c>
-      <c r="J17" s="14"/>
+      <c r="J17" s="13">
+        <v>33.0</v>
+      </c>
       <c r="K17" s="15"/>
       <c r="L17" s="14"/>
       <c r="M17" s="15"/>
@@ -1629,7 +1646,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>219</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18">
@@ -1657,7 +1674,9 @@
       <c r="I18" s="12">
         <v>28.0</v>
       </c>
-      <c r="J18" s="14"/>
+      <c r="J18" s="13">
+        <v>31.0</v>
+      </c>
       <c r="K18" s="15"/>
       <c r="L18" s="14"/>
       <c r="M18" s="15"/>
@@ -1676,7 +1695,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>222</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19">
@@ -1702,7 +1721,9 @@
       <c r="I19" s="12">
         <v>29.0</v>
       </c>
-      <c r="J19" s="14"/>
+      <c r="J19" s="13">
+        <v>31.0</v>
+      </c>
       <c r="K19" s="15"/>
       <c r="L19" s="14"/>
       <c r="M19" s="15"/>
@@ -1721,7 +1742,7 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>179</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20">
@@ -1745,7 +1766,9 @@
         <v>31.0</v>
       </c>
       <c r="I20" s="15"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="13">
+        <v>35.0</v>
+      </c>
       <c r="K20" s="15"/>
       <c r="L20" s="14"/>
       <c r="M20" s="15"/>
@@ -1764,7 +1787,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21">
@@ -1790,7 +1813,9 @@
       <c r="I21" s="12">
         <v>34.0</v>
       </c>
-      <c r="J21" s="14"/>
+      <c r="J21" s="13">
+        <v>29.0</v>
+      </c>
       <c r="K21" s="15"/>
       <c r="L21" s="14"/>
       <c r="M21" s="15"/>
@@ -1809,7 +1834,7 @@
       <c r="Z21" s="16"/>
       <c r="AA21" s="14">
         <f t="shared" si="1"/>
-        <v>195</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22">
@@ -1837,7 +1862,9 @@
       <c r="I22" s="12">
         <v>28.0</v>
       </c>
-      <c r="J22" s="14"/>
+      <c r="J22" s="13">
+        <v>34.0</v>
+      </c>
       <c r="K22" s="15"/>
       <c r="L22" s="14"/>
       <c r="M22" s="15"/>
@@ -1856,7 +1883,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -1910,7 +1937,9 @@
       <c r="I24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="J24" s="21"/>
+      <c r="J24" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
@@ -1931,7 +1960,7 @@
     </row>
     <row r="25">
       <c r="B25" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" s="24">
         <v>35.0</v>
@@ -1954,7 +1983,9 @@
       <c r="I25" s="24">
         <v>34.0</v>
       </c>
-      <c r="J25" s="24"/>
+      <c r="J25" s="24">
+        <v>35.0</v>
+      </c>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
@@ -1996,83 +2027,83 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AA3" s="6"/>
     </row>
@@ -2178,7 +2209,9 @@
       <c r="H5" s="13">
         <v>37.0</v>
       </c>
-      <c r="I5" s="15"/>
+      <c r="I5" s="12">
+        <v>32.0</v>
+      </c>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
       <c r="L5" s="14"/>
@@ -2198,7 +2231,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>179</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
@@ -2221,7 +2254,9 @@
       <c r="H6" s="13">
         <v>34.0</v>
       </c>
-      <c r="I6" s="15"/>
+      <c r="I6" s="12">
+        <v>29.0</v>
+      </c>
       <c r="J6" s="14"/>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
@@ -2241,7 +2276,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>166</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7">
@@ -2264,7 +2299,9 @@
       <c r="H7" s="13">
         <v>33.0</v>
       </c>
-      <c r="I7" s="15"/>
+      <c r="I7" s="12">
+        <v>32.0</v>
+      </c>
       <c r="J7" s="14"/>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
@@ -2284,7 +2321,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>157</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8">
@@ -2309,7 +2346,9 @@
       <c r="H8" s="13">
         <v>27.0</v>
       </c>
-      <c r="I8" s="15"/>
+      <c r="I8" s="12">
+        <v>35.0</v>
+      </c>
       <c r="J8" s="14"/>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
@@ -2329,7 +2368,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>185</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9">
@@ -2397,7 +2436,9 @@
       <c r="H10" s="13">
         <v>34.0</v>
       </c>
-      <c r="I10" s="15"/>
+      <c r="I10" s="12">
+        <v>42.0</v>
+      </c>
       <c r="J10" s="14"/>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
@@ -2417,12 +2458,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>174</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C11" s="12">
         <v>22.0</v>
@@ -2438,7 +2479,9 @@
       <c r="H11" s="13">
         <v>31.0</v>
       </c>
-      <c r="I11" s="15"/>
+      <c r="I11" s="12">
+        <v>29.0</v>
+      </c>
       <c r="J11" s="14"/>
       <c r="K11" s="15"/>
       <c r="L11" s="14"/>
@@ -2458,12 +2501,12 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C12" s="12">
         <v>28.0</v>
@@ -2483,7 +2526,9 @@
       <c r="H12" s="13">
         <v>31.0</v>
       </c>
-      <c r="I12" s="15"/>
+      <c r="I12" s="12">
+        <v>30.0</v>
+      </c>
       <c r="J12" s="14"/>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
@@ -2503,12 +2548,12 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>190</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C13" s="12">
         <v>31.0</v>
@@ -2561,7 +2606,9 @@
       <c r="F14" s="14"/>
       <c r="G14" s="15"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="12">
+        <v>27.0</v>
+      </c>
       <c r="J14" s="14"/>
       <c r="K14" s="15"/>
       <c r="L14" s="14"/>
@@ -2581,7 +2628,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15">
@@ -2629,7 +2676,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C16" s="12">
         <v>32.0</v>
@@ -2647,7 +2694,9 @@
         <v>26.0</v>
       </c>
       <c r="H16" s="14"/>
-      <c r="I16" s="15"/>
+      <c r="I16" s="12">
+        <v>21.0</v>
+      </c>
       <c r="J16" s="14"/>
       <c r="K16" s="15"/>
       <c r="L16" s="14"/>
@@ -2667,7 +2716,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17">
@@ -2690,7 +2739,9 @@
       <c r="H17" s="13">
         <v>34.0</v>
       </c>
-      <c r="I17" s="15"/>
+      <c r="I17" s="12">
+        <v>38.0</v>
+      </c>
       <c r="J17" s="14"/>
       <c r="K17" s="15"/>
       <c r="L17" s="14"/>
@@ -2710,12 +2761,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>162</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="26" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C18" s="12">
         <v>27.0</v>
@@ -2729,7 +2780,9 @@
         <v>26.0</v>
       </c>
       <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
+      <c r="I18" s="12">
+        <v>39.0</v>
+      </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
       <c r="L18" s="15"/>
@@ -2749,7 +2802,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -2789,10 +2842,10 @@
         <v>56</v>
       </c>
       <c r="E20" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>97</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>64</v>
@@ -2800,7 +2853,9 @@
       <c r="H20" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="21"/>
+      <c r="I20" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="J20" s="21"/>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
@@ -2822,7 +2877,7 @@
     </row>
     <row r="21">
       <c r="B21" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C21" s="24">
         <v>40.0</v>
@@ -2842,7 +2897,9 @@
       <c r="H21" s="24">
         <v>37.0</v>
       </c>
-      <c r="I21" s="24"/>
+      <c r="I21" s="24">
+        <v>42.0</v>
+      </c>
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
@@ -2886,10 +2943,10 @@
         <v>25</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2">
@@ -2897,7 +2954,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="31">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="C2" s="32">
         <v>12.0</v>
@@ -2930,7 +2987,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="31">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="C5" s="32">
         <v>14.0</v>
@@ -2985,10 +3042,10 @@
         <v>59</v>
       </c>
       <c r="B10" s="31">
+        <v>8.0</v>
+      </c>
+      <c r="C10" s="32">
         <v>7.0</v>
-      </c>
-      <c r="C10" s="32">
-        <v>6.0</v>
       </c>
     </row>
     <row r="11">
@@ -2996,10 +3053,10 @@
         <v>60</v>
       </c>
       <c r="B11" s="31">
+        <v>11.0</v>
+      </c>
+      <c r="C11" s="32">
         <v>10.0</v>
-      </c>
-      <c r="C11" s="32">
-        <v>9.0</v>
       </c>
     </row>
     <row r="12">
@@ -3029,7 +3086,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="31">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="C14" s="32">
         <v>13.0</v>
@@ -3040,10 +3097,10 @@
         <v>64</v>
       </c>
       <c r="B15" s="31">
-        <v>32.0</v>
+        <v>31.0</v>
       </c>
       <c r="C15" s="32">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="16">
@@ -3092,18 +3149,18 @@
     </row>
     <row r="20">
       <c r="A20" s="33" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B20" s="31">
-        <v>21.0</v>
+        <v>18.0</v>
       </c>
       <c r="C20" s="32">
-        <v>20.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B21" s="31">
         <v>16.0</v>
@@ -3114,7 +3171,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B22" s="31">
         <v>15.0</v>
@@ -3125,7 +3182,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B23" s="31">
         <v>29.0</v>
@@ -3136,7 +3193,7 @@
     </row>
     <row r="24">
       <c r="A24" s="18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B24" s="34">
         <v>27.0</v>
@@ -7055,13 +7112,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
@@ -7105,7 +7162,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6">
@@ -7116,7 +7173,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
@@ -7135,15 +7192,19 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="43"/>
+        <v>108</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="13">
         <v>8.0</v>
       </c>
-      <c r="B9" s="44"/>
+      <c r="B9" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="C9" s="43"/>
     </row>
     <row r="10">
@@ -12136,19 +12197,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2">
@@ -12289,7 +12350,14 @@
         <f>'SUNDAY SINGLES'!I25</f>
         <v>34</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="49" t="str">
+        <f>'THURSDAY SINGLES'!I20</f>
+        <v>KEN PEEL</v>
+      </c>
+      <c r="E8" s="48">
+        <f>'THURSDAY SINGLES'!I$21</f>
+        <v>42</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="13">
@@ -12297,13 +12365,20 @@
       </c>
       <c r="B9" s="48" t="str">
         <f>'SUNDAY SINGLES'!J24</f>
+        <v>FRED HOLINGWORTH</v>
+      </c>
+      <c r="C9" s="48">
+        <f>'SUNDAY SINGLES'!J25</f>
+        <v>35</v>
+      </c>
+      <c r="D9" s="49" t="str">
+        <f>'THURSDAY SINGLES'!J20</f>
         <v/>
       </c>
-      <c r="C9" s="48" t="str">
-        <f>'SUNDAY SINGLES'!J25</f>
+      <c r="E9" s="48" t="str">
+        <f>'THURSDAY SINGLES'!J$21</f>
         <v/>
       </c>
-      <c r="D9" s="49"/>
     </row>
     <row r="10">
       <c r="A10" s="13">
@@ -12318,6 +12393,10 @@
         <v/>
       </c>
       <c r="D10" s="49"/>
+      <c r="E10" s="48" t="str">
+        <f>'THURSDAY SINGLES'!J$21</f>
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="13">
@@ -12332,18 +12411,30 @@
         <v/>
       </c>
       <c r="D11" s="49"/>
+      <c r="E11" s="48" t="str">
+        <f>'THURSDAY SINGLES'!J$21</f>
+        <v/>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="13">
         <v>11.0</v>
       </c>
       <c r="D12" s="49"/>
+      <c r="E12" s="48" t="str">
+        <f>'THURSDAY SINGLES'!J$21</f>
+        <v/>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="13">
         <v>12.0</v>
       </c>
       <c r="D13" s="49"/>
+      <c r="E13" s="48" t="str">
+        <f>'THURSDAY SINGLES'!J$21</f>
+        <v/>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="13">

</xml_diff>

<commit_message>
051 Week 9/8 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="114">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>STEW LAWSON</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>SUNDAY</t>
@@ -1094,7 +1097,9 @@
       <c r="J5" s="13">
         <v>27.0</v>
       </c>
-      <c r="K5" s="15"/>
+      <c r="K5" s="12">
+        <v>31.0</v>
+      </c>
       <c r="L5" s="14"/>
       <c r="M5" s="15"/>
       <c r="N5" s="14"/>
@@ -1112,7 +1117,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>194</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6">
@@ -1143,7 +1148,9 @@
       <c r="J6" s="13">
         <v>31.0</v>
       </c>
-      <c r="K6" s="15"/>
+      <c r="K6" s="12">
+        <v>30.0</v>
+      </c>
       <c r="L6" s="14"/>
       <c r="M6" s="15"/>
       <c r="N6" s="14"/>
@@ -1161,7 +1168,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>249</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7">
@@ -1190,7 +1197,9 @@
         <v>23.0</v>
       </c>
       <c r="J7" s="14"/>
-      <c r="K7" s="15"/>
+      <c r="K7" s="12">
+        <v>26.0</v>
+      </c>
       <c r="L7" s="14"/>
       <c r="M7" s="15"/>
       <c r="N7" s="14"/>
@@ -1208,7 +1217,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>185</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8">
@@ -1327,7 +1336,9 @@
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
+      <c r="K10" s="12">
+        <v>39.0</v>
+      </c>
       <c r="L10" s="14"/>
       <c r="M10" s="15"/>
       <c r="N10" s="14"/>
@@ -1345,7 +1356,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>167</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11">
@@ -1360,7 +1371,9 @@
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="15"/>
+      <c r="K11" s="12">
+        <v>32.0</v>
+      </c>
       <c r="L11" s="14"/>
       <c r="M11" s="15"/>
       <c r="N11" s="14"/>
@@ -1378,7 +1391,7 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -1409,7 +1422,9 @@
       <c r="J12" s="13">
         <v>31.0</v>
       </c>
-      <c r="K12" s="15"/>
+      <c r="K12" s="12">
+        <v>31.0</v>
+      </c>
       <c r="L12" s="14"/>
       <c r="M12" s="15"/>
       <c r="N12" s="14"/>
@@ -1427,7 +1442,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>227</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13">
@@ -1452,7 +1467,9 @@
       <c r="J13" s="13">
         <v>26.0</v>
       </c>
-      <c r="K13" s="15"/>
+      <c r="K13" s="12">
+        <v>32.0</v>
+      </c>
       <c r="L13" s="14"/>
       <c r="M13" s="15"/>
       <c r="N13" s="14"/>
@@ -1470,7 +1487,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14">
@@ -1493,7 +1510,9 @@
       <c r="J14" s="13">
         <v>34.0</v>
       </c>
-      <c r="K14" s="15"/>
+      <c r="K14" s="12">
+        <v>36.0</v>
+      </c>
       <c r="L14" s="14"/>
       <c r="M14" s="15"/>
       <c r="N14" s="14"/>
@@ -1511,7 +1530,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15">
@@ -1628,7 +1647,9 @@
       <c r="J17" s="13">
         <v>33.0</v>
       </c>
-      <c r="K17" s="15"/>
+      <c r="K17" s="12">
+        <v>35.0</v>
+      </c>
       <c r="L17" s="14"/>
       <c r="M17" s="15"/>
       <c r="N17" s="14"/>
@@ -1646,7 +1667,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>252</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18">
@@ -1677,7 +1698,9 @@
       <c r="J18" s="13">
         <v>31.0</v>
       </c>
-      <c r="K18" s="15"/>
+      <c r="K18" s="12">
+        <v>29.0</v>
+      </c>
       <c r="L18" s="14"/>
       <c r="M18" s="15"/>
       <c r="N18" s="14"/>
@@ -1695,7 +1718,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>253</v>
+        <v>282</v>
       </c>
     </row>
     <row r="19">
@@ -1769,7 +1792,9 @@
       <c r="J20" s="13">
         <v>35.0</v>
       </c>
-      <c r="K20" s="15"/>
+      <c r="K20" s="12">
+        <v>32.0</v>
+      </c>
       <c r="L20" s="14"/>
       <c r="M20" s="15"/>
       <c r="N20" s="14"/>
@@ -1787,7 +1812,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21">
@@ -1865,7 +1890,9 @@
       <c r="J22" s="13">
         <v>34.0</v>
       </c>
-      <c r="K22" s="15"/>
+      <c r="K22" s="12">
+        <v>31.0</v>
+      </c>
       <c r="L22" s="14"/>
       <c r="M22" s="15"/>
       <c r="N22" s="14"/>
@@ -1883,7 +1910,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>244</v>
+        <v>275</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -1940,7 +1967,9 @@
       <c r="J24" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="K24" s="21"/>
+      <c r="K24" s="21" t="s">
+        <v>56</v>
+      </c>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
@@ -1986,7 +2015,9 @@
       <c r="J25" s="24">
         <v>35.0</v>
       </c>
-      <c r="K25" s="24"/>
+      <c r="K25" s="24">
+        <v>39.0</v>
+      </c>
       <c r="L25" s="24"/>
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
@@ -2257,7 +2288,9 @@
       <c r="I6" s="12">
         <v>29.0</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="13">
+        <v>30.0</v>
+      </c>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
       <c r="M6" s="15"/>
@@ -2276,7 +2309,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>195</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7">
@@ -2302,7 +2335,9 @@
       <c r="I7" s="12">
         <v>32.0</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="13">
+        <v>32.0</v>
+      </c>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
       <c r="M7" s="15"/>
@@ -2321,7 +2356,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>189</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8">
@@ -2349,7 +2384,9 @@
       <c r="I8" s="12">
         <v>35.0</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="13">
+        <v>31.0</v>
+      </c>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
       <c r="M8" s="15"/>
@@ -2368,7 +2405,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9">
@@ -2439,7 +2476,9 @@
       <c r="I10" s="12">
         <v>42.0</v>
       </c>
-      <c r="J10" s="14"/>
+      <c r="J10" s="13">
+        <v>27.0</v>
+      </c>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
       <c r="M10" s="15"/>
@@ -2458,7 +2497,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>216</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11">
@@ -2529,7 +2568,9 @@
       <c r="I12" s="12">
         <v>30.0</v>
       </c>
-      <c r="J12" s="14"/>
+      <c r="J12" s="13">
+        <v>29.0</v>
+      </c>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
       <c r="M12" s="15"/>
@@ -2548,7 +2589,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13">
@@ -2609,7 +2650,9 @@
       <c r="I14" s="12">
         <v>27.0</v>
       </c>
-      <c r="J14" s="14"/>
+      <c r="J14" s="13">
+        <v>28.0</v>
+      </c>
       <c r="K14" s="15"/>
       <c r="L14" s="14"/>
       <c r="M14" s="15"/>
@@ -2628,7 +2671,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
@@ -2652,7 +2695,9 @@
         <v>28.0</v>
       </c>
       <c r="I15" s="15"/>
-      <c r="J15" s="14"/>
+      <c r="J15" s="13">
+        <v>32.0</v>
+      </c>
       <c r="K15" s="15"/>
       <c r="L15" s="14"/>
       <c r="M15" s="15"/>
@@ -2671,7 +2716,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>148</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16">
@@ -2697,7 +2742,9 @@
       <c r="I16" s="12">
         <v>21.0</v>
       </c>
-      <c r="J16" s="14"/>
+      <c r="J16" s="13">
+        <v>32.0</v>
+      </c>
       <c r="K16" s="15"/>
       <c r="L16" s="14"/>
       <c r="M16" s="15"/>
@@ -2716,7 +2763,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>161</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17">
@@ -2742,7 +2789,9 @@
       <c r="I17" s="12">
         <v>38.0</v>
       </c>
-      <c r="J17" s="14"/>
+      <c r="J17" s="13">
+        <v>32.0</v>
+      </c>
       <c r="K17" s="15"/>
       <c r="L17" s="14"/>
       <c r="M17" s="15"/>
@@ -2761,7 +2810,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18">
@@ -2856,7 +2905,9 @@
       <c r="I20" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="J20" s="21"/>
+      <c r="J20" s="21" t="s">
+        <v>100</v>
+      </c>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
@@ -2900,7 +2951,9 @@
       <c r="I21" s="24">
         <v>42.0</v>
       </c>
-      <c r="J21" s="24"/>
+      <c r="J21" s="24">
+        <v>32.0</v>
+      </c>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
@@ -3119,7 +3172,7 @@
         <v>66</v>
       </c>
       <c r="B17" s="31">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C17" s="32">
         <v>6.0</v>
@@ -3163,7 +3216,7 @@
         <v>98</v>
       </c>
       <c r="B21" s="31">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="C21" s="32">
         <v>14.0</v>
@@ -7205,13 +7258,17 @@
       <c r="B9" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="43"/>
+      <c r="C9" s="42" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="13">
         <v>9.0</v>
       </c>
-      <c r="B10" s="41"/>
+      <c r="B10" s="41" t="s">
+        <v>63</v>
+      </c>
       <c r="C10" s="43"/>
       <c r="G10" s="14"/>
     </row>
@@ -12200,16 +12257,16 @@
         <v>104</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2">
@@ -12373,11 +12430,11 @@
       </c>
       <c r="D9" s="49" t="str">
         <f>'THURSDAY SINGLES'!J20</f>
-        <v/>
-      </c>
-      <c r="E9" s="48" t="str">
+        <v>JOHN KING</v>
+      </c>
+      <c r="E9" s="48">
         <f>'THURSDAY SINGLES'!J$21</f>
-        <v/>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
@@ -12386,15 +12443,15 @@
       </c>
       <c r="B10" s="48" t="str">
         <f>'SUNDAY SINGLES'!K24</f>
-        <v/>
-      </c>
-      <c r="C10" s="48" t="str">
+        <v>TONI SHIRLEY</v>
+      </c>
+      <c r="C10" s="48">
         <f>'SUNDAY SINGLES'!K25</f>
-        <v/>
+        <v>39</v>
       </c>
       <c r="D10" s="49"/>
       <c r="E10" s="48" t="str">
-        <f>'THURSDAY SINGLES'!J$21</f>
+        <f>'THURSDAY SINGLES'!K$21</f>
         <v/>
       </c>
     </row>
@@ -12412,7 +12469,7 @@
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="48" t="str">
-        <f>'THURSDAY SINGLES'!J$21</f>
+        <f>'THURSDAY SINGLES'!L$21</f>
         <v/>
       </c>
     </row>
@@ -12422,7 +12479,7 @@
       </c>
       <c r="D12" s="49"/>
       <c r="E12" s="48" t="str">
-        <f>'THURSDAY SINGLES'!J$21</f>
+        <f>'THURSDAY SINGLES'!M$21</f>
         <v/>
       </c>
     </row>
@@ -12432,7 +12489,7 @@
       </c>
       <c r="D13" s="49"/>
       <c r="E13" s="48" t="str">
-        <f>'THURSDAY SINGLES'!J$21</f>
+        <f>'THURSDAY SINGLES'!N$21</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
052 Week 10/9 update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="114">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -344,7 +344,7 @@
     <t>STEW LAWSON</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>N/A</t>
   </si>
   <si>
     <t>SUNDAY</t>
@@ -1200,7 +1200,9 @@
       <c r="K7" s="12">
         <v>26.0</v>
       </c>
-      <c r="L7" s="14"/>
+      <c r="L7" s="13">
+        <v>24.0</v>
+      </c>
       <c r="M7" s="15"/>
       <c r="N7" s="14"/>
       <c r="O7" s="15"/>
@@ -1217,7 +1219,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>211</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8">
@@ -1249,7 +1251,9 @@
         <v>30.0</v>
       </c>
       <c r="K8" s="15"/>
-      <c r="L8" s="14"/>
+      <c r="L8" s="13">
+        <v>39.0</v>
+      </c>
       <c r="M8" s="15"/>
       <c r="N8" s="14"/>
       <c r="O8" s="15"/>
@@ -1266,7 +1270,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>249</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9">
@@ -1425,7 +1429,9 @@
       <c r="K12" s="12">
         <v>31.0</v>
       </c>
-      <c r="L12" s="14"/>
+      <c r="L12" s="13">
+        <v>35.0</v>
+      </c>
       <c r="M12" s="15"/>
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
@@ -1442,7 +1448,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>258</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13">
@@ -1470,7 +1476,9 @@
       <c r="K13" s="12">
         <v>32.0</v>
       </c>
-      <c r="L13" s="14"/>
+      <c r="L13" s="13">
+        <v>25.0</v>
+      </c>
       <c r="M13" s="15"/>
       <c r="N13" s="14"/>
       <c r="O13" s="15"/>
@@ -1487,7 +1495,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14">
@@ -1650,7 +1658,9 @@
       <c r="K17" s="12">
         <v>35.0</v>
       </c>
-      <c r="L17" s="14"/>
+      <c r="L17" s="13">
+        <v>33.0</v>
+      </c>
       <c r="M17" s="15"/>
       <c r="N17" s="14"/>
       <c r="O17" s="15"/>
@@ -1667,7 +1677,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>287</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18">
@@ -1701,7 +1711,9 @@
       <c r="K18" s="12">
         <v>29.0</v>
       </c>
-      <c r="L18" s="14"/>
+      <c r="L18" s="13">
+        <v>24.0</v>
+      </c>
       <c r="M18" s="15"/>
       <c r="N18" s="14"/>
       <c r="O18" s="15"/>
@@ -1718,7 +1730,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>282</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19">
@@ -1748,7 +1760,9 @@
         <v>31.0</v>
       </c>
       <c r="K19" s="15"/>
-      <c r="L19" s="14"/>
+      <c r="L19" s="13">
+        <v>30.0</v>
+      </c>
       <c r="M19" s="15"/>
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
@@ -1765,7 +1779,7 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20">
@@ -1970,7 +1984,9 @@
       <c r="K24" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="L24" s="21"/>
+      <c r="L24" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
       <c r="O24" s="21"/>
@@ -2018,7 +2034,9 @@
       <c r="K25" s="24">
         <v>39.0</v>
       </c>
-      <c r="L25" s="24"/>
+      <c r="L25" s="24">
+        <v>39.0</v>
+      </c>
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
@@ -2653,7 +2671,9 @@
       <c r="J14" s="13">
         <v>28.0</v>
       </c>
-      <c r="K14" s="15"/>
+      <c r="K14" s="12">
+        <v>30.0</v>
+      </c>
       <c r="L14" s="14"/>
       <c r="M14" s="15"/>
       <c r="N14" s="14"/>
@@ -2671,7 +2691,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15">
@@ -2833,7 +2853,9 @@
         <v>39.0</v>
       </c>
       <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
+      <c r="K18" s="12">
+        <v>30.0</v>
+      </c>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
@@ -2851,7 +2873,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -2908,7 +2930,9 @@
       <c r="J20" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="K20" s="21"/>
+      <c r="K20" s="21" t="s">
+        <v>57</v>
+      </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
@@ -2954,7 +2978,9 @@
       <c r="J21" s="24">
         <v>32.0</v>
       </c>
-      <c r="K21" s="24"/>
+      <c r="K21" s="24">
+        <v>30.0</v>
+      </c>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
@@ -3040,7 +3066,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="31">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="C5" s="32">
         <v>14.0</v>
@@ -3051,10 +3077,10 @@
         <v>55</v>
       </c>
       <c r="B6" s="31">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
       <c r="C6" s="32">
-        <v>-1.0</v>
+        <v>-2.0</v>
       </c>
     </row>
     <row r="7">
@@ -3139,10 +3165,10 @@
         <v>63</v>
       </c>
       <c r="B14" s="31">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="C14" s="32">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="15">
@@ -3175,7 +3201,7 @@
         <v>9.0</v>
       </c>
       <c r="C17" s="32">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="18">
@@ -3194,10 +3220,10 @@
         <v>68</v>
       </c>
       <c r="B19" s="31">
+        <v>9.0</v>
+      </c>
+      <c r="C19" s="32">
         <v>8.0</v>
-      </c>
-      <c r="C19" s="32">
-        <v>7.0</v>
       </c>
     </row>
     <row r="20">
@@ -3238,10 +3264,10 @@
         <v>97</v>
       </c>
       <c r="B23" s="31">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="C23" s="32">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="24">
@@ -7269,14 +7295,18 @@
       <c r="B10" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="43"/>
+      <c r="C10" s="42" t="s">
+        <v>109</v>
+      </c>
       <c r="G10" s="14"/>
     </row>
     <row r="11">
       <c r="A11" s="13">
         <v>10.0</v>
       </c>
-      <c r="B11" s="44"/>
+      <c r="B11" s="41" t="s">
+        <v>109</v>
+      </c>
       <c r="C11" s="43"/>
     </row>
     <row r="12">
@@ -12449,10 +12479,13 @@
         <f>'SUNDAY SINGLES'!K25</f>
         <v>39</v>
       </c>
-      <c r="D10" s="49"/>
-      <c r="E10" s="48" t="str">
+      <c r="D10" s="49" t="str">
+        <f>'THURSDAY SINGLES'!K20</f>
+        <v>ALBIE GILLESPIE</v>
+      </c>
+      <c r="E10" s="48">
         <f>'THURSDAY SINGLES'!K$21</f>
-        <v/>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
@@ -12461,11 +12494,11 @@
       </c>
       <c r="B11" s="48" t="str">
         <f>'SUNDAY SINGLES'!L24</f>
-        <v/>
-      </c>
-      <c r="C11" s="48" t="str">
+        <v>JOHN ANTCLIFFE</v>
+      </c>
+      <c r="C11" s="48">
         <f>'SUNDAY SINGLES'!L25</f>
-        <v/>
+        <v>39</v>
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="48" t="str">

</xml_diff>

<commit_message>
053 Week 11/10 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>FRED HOLLINGWORTH</t>
   </si>
   <si>
     <t>SUNDAY</t>
@@ -1152,7 +1155,9 @@
         <v>30.0</v>
       </c>
       <c r="L6" s="14"/>
-      <c r="M6" s="15"/>
+      <c r="M6" s="12">
+        <v>31.0</v>
+      </c>
       <c r="N6" s="14"/>
       <c r="O6" s="15"/>
       <c r="P6" s="14"/>
@@ -1168,7 +1173,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>279</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7">
@@ -1203,7 +1208,9 @@
       <c r="L7" s="13">
         <v>24.0</v>
       </c>
-      <c r="M7" s="15"/>
+      <c r="M7" s="12">
+        <v>33.0</v>
+      </c>
       <c r="N7" s="14"/>
       <c r="O7" s="15"/>
       <c r="P7" s="14"/>
@@ -1219,7 +1226,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>235</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8">
@@ -1254,7 +1261,9 @@
       <c r="L8" s="13">
         <v>39.0</v>
       </c>
-      <c r="M8" s="15"/>
+      <c r="M8" s="12">
+        <v>41.0</v>
+      </c>
       <c r="N8" s="14"/>
       <c r="O8" s="15"/>
       <c r="P8" s="14"/>
@@ -1270,7 +1279,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>288</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9">
@@ -1299,7 +1308,9 @@
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
+      <c r="M9" s="12">
+        <v>31.0</v>
+      </c>
       <c r="N9" s="14"/>
       <c r="O9" s="15"/>
       <c r="P9" s="14"/>
@@ -1315,7 +1326,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>174</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10">
@@ -1344,7 +1355,9 @@
         <v>39.0</v>
       </c>
       <c r="L10" s="14"/>
-      <c r="M10" s="15"/>
+      <c r="M10" s="12">
+        <v>36.0</v>
+      </c>
       <c r="N10" s="14"/>
       <c r="O10" s="15"/>
       <c r="P10" s="14"/>
@@ -1360,7 +1373,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>206</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11">
@@ -1379,7 +1392,9 @@
         <v>32.0</v>
       </c>
       <c r="L11" s="14"/>
-      <c r="M11" s="15"/>
+      <c r="M11" s="12">
+        <v>39.0</v>
+      </c>
       <c r="N11" s="14"/>
       <c r="O11" s="15"/>
       <c r="P11" s="14"/>
@@ -1395,7 +1410,7 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12">
@@ -1432,7 +1447,9 @@
       <c r="L12" s="13">
         <v>35.0</v>
       </c>
-      <c r="M12" s="15"/>
+      <c r="M12" s="12">
+        <v>35.0</v>
+      </c>
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
       <c r="P12" s="14"/>
@@ -1448,7 +1465,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>293</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13">
@@ -1522,7 +1539,9 @@
         <v>36.0</v>
       </c>
       <c r="L14" s="14"/>
-      <c r="M14" s="15"/>
+      <c r="M14" s="12">
+        <v>36.0</v>
+      </c>
       <c r="N14" s="14"/>
       <c r="O14" s="15"/>
       <c r="P14" s="14"/>
@@ -1538,7 +1557,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>148</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15">
@@ -1661,7 +1680,9 @@
       <c r="L17" s="13">
         <v>33.0</v>
       </c>
-      <c r="M17" s="15"/>
+      <c r="M17" s="12">
+        <v>36.0</v>
+      </c>
       <c r="N17" s="14"/>
       <c r="O17" s="15"/>
       <c r="P17" s="14"/>
@@ -1677,7 +1698,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18">
@@ -1714,7 +1735,9 @@
       <c r="L18" s="13">
         <v>24.0</v>
       </c>
-      <c r="M18" s="15"/>
+      <c r="M18" s="12">
+        <v>40.0</v>
+      </c>
       <c r="N18" s="14"/>
       <c r="O18" s="15"/>
       <c r="P18" s="14"/>
@@ -1730,7 +1753,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>306</v>
+        <v>346</v>
       </c>
     </row>
     <row r="19">
@@ -1810,7 +1833,9 @@
         <v>32.0</v>
       </c>
       <c r="L20" s="14"/>
-      <c r="M20" s="15"/>
+      <c r="M20" s="12">
+        <v>35.0</v>
+      </c>
       <c r="N20" s="14"/>
       <c r="O20" s="15"/>
       <c r="P20" s="14"/>
@@ -1826,7 +1851,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21">
@@ -1908,7 +1933,9 @@
         <v>31.0</v>
       </c>
       <c r="L22" s="14"/>
-      <c r="M22" s="15"/>
+      <c r="M22" s="12">
+        <v>37.0</v>
+      </c>
       <c r="N22" s="14"/>
       <c r="O22" s="15"/>
       <c r="P22" s="14"/>
@@ -1924,7 +1951,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>275</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -1987,7 +2014,9 @@
       <c r="L24" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="M24" s="21"/>
+      <c r="M24" s="21" t="s">
+        <v>54</v>
+      </c>
       <c r="N24" s="21"/>
       <c r="O24" s="21"/>
       <c r="P24" s="21"/>
@@ -2037,7 +2066,9 @@
       <c r="L25" s="24">
         <v>39.0</v>
       </c>
-      <c r="M25" s="24"/>
+      <c r="M25" s="24">
+        <v>41.0</v>
+      </c>
       <c r="N25" s="24"/>
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
@@ -2310,7 +2341,9 @@
         <v>30.0</v>
       </c>
       <c r="K6" s="15"/>
-      <c r="L6" s="14"/>
+      <c r="L6" s="13">
+        <v>34.0</v>
+      </c>
       <c r="M6" s="15"/>
       <c r="N6" s="14"/>
       <c r="O6" s="15"/>
@@ -2327,7 +2360,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>225</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7">
@@ -2357,7 +2390,9 @@
         <v>32.0</v>
       </c>
       <c r="K7" s="15"/>
-      <c r="L7" s="14"/>
+      <c r="L7" s="13">
+        <v>33.0</v>
+      </c>
       <c r="M7" s="15"/>
       <c r="N7" s="14"/>
       <c r="O7" s="15"/>
@@ -2374,7 +2409,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>221</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8">
@@ -2451,7 +2486,9 @@
       <c r="I9" s="15"/>
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
-      <c r="L9" s="14"/>
+      <c r="L9" s="13">
+        <v>30.0</v>
+      </c>
       <c r="M9" s="15"/>
       <c r="N9" s="14"/>
       <c r="O9" s="15"/>
@@ -2468,7 +2505,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>178</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10">
@@ -2541,7 +2578,9 @@
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="15"/>
-      <c r="L11" s="14"/>
+      <c r="L11" s="13">
+        <v>26.0</v>
+      </c>
       <c r="M11" s="15"/>
       <c r="N11" s="14"/>
       <c r="O11" s="15"/>
@@ -2558,7 +2597,7 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>137</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12">
@@ -2590,7 +2629,9 @@
         <v>29.0</v>
       </c>
       <c r="K12" s="15"/>
-      <c r="L12" s="14"/>
+      <c r="L12" s="13">
+        <v>27.0</v>
+      </c>
       <c r="M12" s="15"/>
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
@@ -2607,7 +2648,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>249</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13">
@@ -2674,7 +2715,9 @@
       <c r="K14" s="12">
         <v>30.0</v>
       </c>
-      <c r="L14" s="14"/>
+      <c r="L14" s="13">
+        <v>31.0</v>
+      </c>
       <c r="M14" s="15"/>
       <c r="N14" s="14"/>
       <c r="O14" s="15"/>
@@ -2691,7 +2734,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15">
@@ -2719,7 +2762,9 @@
         <v>32.0</v>
       </c>
       <c r="K15" s="15"/>
-      <c r="L15" s="14"/>
+      <c r="L15" s="13">
+        <v>28.0</v>
+      </c>
       <c r="M15" s="15"/>
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
@@ -2736,7 +2781,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>180</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16">
@@ -2766,7 +2811,9 @@
         <v>32.0</v>
       </c>
       <c r="K16" s="15"/>
-      <c r="L16" s="14"/>
+      <c r="L16" s="13">
+        <v>30.0</v>
+      </c>
       <c r="M16" s="15"/>
       <c r="N16" s="14"/>
       <c r="O16" s="15"/>
@@ -2783,7 +2830,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>193</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17">
@@ -2856,7 +2903,9 @@
       <c r="K18" s="12">
         <v>30.0</v>
       </c>
-      <c r="L18" s="15"/>
+      <c r="L18" s="12">
+        <v>33.0</v>
+      </c>
       <c r="M18" s="15"/>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
@@ -2873,7 +2922,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>149</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -2933,7 +2982,9 @@
       <c r="K20" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="L20" s="21"/>
+      <c r="L20" s="21" t="s">
+        <v>63</v>
+      </c>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
       <c r="O20" s="21"/>
@@ -2981,7 +3032,9 @@
       <c r="K21" s="24">
         <v>30.0</v>
       </c>
-      <c r="L21" s="24"/>
+      <c r="L21" s="24">
+        <v>34.0</v>
+      </c>
       <c r="M21" s="24"/>
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
@@ -3069,7 +3122,7 @@
         <v>15.0</v>
       </c>
       <c r="C5" s="32">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="6">
@@ -3102,7 +3155,7 @@
         <v>8.0</v>
       </c>
       <c r="C8" s="32">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="9">
@@ -3176,10 +3229,10 @@
         <v>64</v>
       </c>
       <c r="B15" s="31">
-        <v>31.0</v>
+        <v>30.0</v>
       </c>
       <c r="C15" s="32">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="16">
@@ -7307,13 +7360,17 @@
       <c r="B11" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="43"/>
+      <c r="C11" s="42" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="13">
         <v>11.0</v>
       </c>
-      <c r="B12" s="41"/>
+      <c r="B12" s="41" t="s">
+        <v>110</v>
+      </c>
       <c r="C12" s="42"/>
     </row>
     <row r="13">
@@ -12287,16 +12344,16 @@
         <v>104</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2">
@@ -12500,19 +12557,33 @@
         <f>'SUNDAY SINGLES'!L25</f>
         <v>39</v>
       </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="48" t="str">
+      <c r="D11" s="49" t="str">
+        <f>'THURSDAY SINGLES'!L20</f>
+        <v>MAL JONES</v>
+      </c>
+      <c r="E11" s="48">
         <f>'THURSDAY SINGLES'!L$21</f>
-        <v/>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="13">
         <v>11.0</v>
       </c>
-      <c r="D12" s="49"/>
+      <c r="B12" s="48" t="str">
+        <f>'SUNDAY SINGLES'!M24</f>
+        <v>JOHN ANTCLIFFE</v>
+      </c>
+      <c r="C12" s="48">
+        <f>'SUNDAY SINGLES'!M25</f>
+        <v>41</v>
+      </c>
+      <c r="D12" s="49" t="str">
+        <f>'THURSDAY SINGLES'!M20</f>
+        <v/>
+      </c>
       <c r="E12" s="48" t="str">
-        <f>'THURSDAY SINGLES'!M$21</f>
+        <f>'THURSDAY SINGLES'!M21</f>
         <v/>
       </c>
     </row>
@@ -12520,7 +12591,18 @@
       <c r="A13" s="13">
         <v>12.0</v>
       </c>
-      <c r="D13" s="49"/>
+      <c r="B13" s="48" t="str">
+        <f>'SUNDAY SINGLES'!N24</f>
+        <v/>
+      </c>
+      <c r="C13" s="48" t="str">
+        <f>'SUNDAY SINGLES'!N25</f>
+        <v/>
+      </c>
+      <c r="D13" s="49" t="str">
+        <f>'THURSDAY SINGLES'!N20</f>
+        <v/>
+      </c>
       <c r="E13" s="48" t="str">
         <f>'THURSDAY SINGLES'!N$21</f>
         <v/>
@@ -12530,73 +12612,253 @@
       <c r="A14" s="13">
         <v>13.0</v>
       </c>
-      <c r="D14" s="49"/>
+      <c r="B14" s="48" t="str">
+        <f>'SUNDAY SINGLES'!O24</f>
+        <v/>
+      </c>
+      <c r="C14" s="48" t="str">
+        <f>'SUNDAY SINGLES'!O25</f>
+        <v/>
+      </c>
+      <c r="D14" s="49" t="str">
+        <f>'THURSDAY SINGLES'!O20</f>
+        <v/>
+      </c>
+      <c r="E14" s="48" t="str">
+        <f>'THURSDAY SINGLES'!O21</f>
+        <v/>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="13">
         <v>14.0</v>
       </c>
-      <c r="D15" s="49"/>
+      <c r="B15" s="48" t="str">
+        <f>'SUNDAY SINGLES'!P24</f>
+        <v/>
+      </c>
+      <c r="C15" s="48" t="str">
+        <f>'SUNDAY SINGLES'!P25</f>
+        <v/>
+      </c>
+      <c r="D15" s="49" t="str">
+        <f>'THURSDAY SINGLES'!P20</f>
+        <v/>
+      </c>
+      <c r="E15" s="48" t="str">
+        <f>'THURSDAY SINGLES'!P21</f>
+        <v/>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="13">
         <v>15.0</v>
       </c>
-      <c r="D16" s="49"/>
+      <c r="B16" s="48" t="str">
+        <f>'SUNDAY SINGLES'!Q24</f>
+        <v/>
+      </c>
+      <c r="C16" s="48" t="str">
+        <f>'SUNDAY SINGLES'!Q25</f>
+        <v/>
+      </c>
+      <c r="D16" s="49" t="str">
+        <f>'THURSDAY SINGLES'!Q20</f>
+        <v/>
+      </c>
+      <c r="E16" s="48" t="str">
+        <f>'THURSDAY SINGLES'!Q21</f>
+        <v/>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="13">
         <v>16.0</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="B17" s="48" t="str">
+        <f>'SUNDAY SINGLES'!R24</f>
+        <v/>
+      </c>
+      <c r="C17" s="48" t="str">
+        <f>'SUNDAY SINGLES'!R25</f>
+        <v/>
+      </c>
+      <c r="D17" s="49" t="str">
+        <f>'THURSDAY SINGLES'!R20</f>
+        <v/>
+      </c>
+      <c r="E17" s="48" t="str">
+        <f>'THURSDAY SINGLES'!R21</f>
+        <v/>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="13">
         <v>17.0</v>
       </c>
-      <c r="D18" s="49"/>
+      <c r="B18" s="48" t="str">
+        <f>'SUNDAY SINGLES'!S24</f>
+        <v/>
+      </c>
+      <c r="C18" s="48" t="str">
+        <f>'SUNDAY SINGLES'!S25</f>
+        <v/>
+      </c>
+      <c r="D18" s="49" t="str">
+        <f>'THURSDAY SINGLES'!S20</f>
+        <v/>
+      </c>
+      <c r="E18" s="48" t="str">
+        <f>'THURSDAY SINGLES'!S21</f>
+        <v/>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="13">
         <v>18.0</v>
       </c>
-      <c r="D19" s="49"/>
+      <c r="B19" s="48" t="str">
+        <f>'SUNDAY SINGLES'!T24</f>
+        <v/>
+      </c>
+      <c r="C19" s="48" t="str">
+        <f>'SUNDAY SINGLES'!T25</f>
+        <v/>
+      </c>
+      <c r="D19" s="49" t="str">
+        <f>'THURSDAY SINGLES'!T20</f>
+        <v/>
+      </c>
+      <c r="E19" s="48" t="str">
+        <f>'THURSDAY SINGLES'!T21</f>
+        <v/>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="13">
         <v>19.0</v>
       </c>
-      <c r="D20" s="49"/>
+      <c r="B20" s="48" t="str">
+        <f>'SUNDAY SINGLES'!U24</f>
+        <v/>
+      </c>
+      <c r="C20" s="48" t="str">
+        <f>'SUNDAY SINGLES'!U25</f>
+        <v/>
+      </c>
+      <c r="D20" s="49" t="str">
+        <f>'THURSDAY SINGLES'!U20</f>
+        <v/>
+      </c>
+      <c r="E20" s="48" t="str">
+        <f>'THURSDAY SINGLES'!U21</f>
+        <v/>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="13">
         <v>20.0</v>
       </c>
-      <c r="D21" s="49"/>
+      <c r="B21" s="48" t="str">
+        <f>'SUNDAY SINGLES'!V24</f>
+        <v/>
+      </c>
+      <c r="C21" s="48" t="str">
+        <f>'SUNDAY SINGLES'!V25</f>
+        <v/>
+      </c>
+      <c r="D21" s="49" t="str">
+        <f>'THURSDAY SINGLES'!V20</f>
+        <v/>
+      </c>
+      <c r="E21" s="48" t="str">
+        <f>'THURSDAY SINGLES'!V21</f>
+        <v/>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="13">
         <v>21.0</v>
       </c>
-      <c r="D22" s="49"/>
+      <c r="B22" s="48" t="str">
+        <f>'SUNDAY SINGLES'!W24</f>
+        <v/>
+      </c>
+      <c r="C22" s="48" t="str">
+        <f>'SUNDAY SINGLES'!W25</f>
+        <v/>
+      </c>
+      <c r="D22" s="49" t="str">
+        <f>'THURSDAY SINGLES'!W20</f>
+        <v/>
+      </c>
+      <c r="E22" s="48" t="str">
+        <f>'THURSDAY SINGLES'!W21</f>
+        <v/>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="13">
         <v>22.0</v>
       </c>
-      <c r="D23" s="49"/>
+      <c r="B23" s="48" t="str">
+        <f>'SUNDAY SINGLES'!X24</f>
+        <v/>
+      </c>
+      <c r="C23" s="48" t="str">
+        <f>'SUNDAY SINGLES'!X25</f>
+        <v/>
+      </c>
+      <c r="D23" s="49" t="str">
+        <f>'THURSDAY SINGLES'!X20</f>
+        <v/>
+      </c>
+      <c r="E23" s="48" t="str">
+        <f>'THURSDAY SINGLES'!X21</f>
+        <v/>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="13">
         <v>23.0</v>
       </c>
-      <c r="D24" s="49"/>
+      <c r="B24" s="48" t="str">
+        <f>'SUNDAY SINGLES'!Y24</f>
+        <v/>
+      </c>
+      <c r="C24" s="48" t="str">
+        <f>'SUNDAY SINGLES'!Y25</f>
+        <v/>
+      </c>
+      <c r="D24" s="49" t="str">
+        <f>'THURSDAY SINGLES'!Y20</f>
+        <v/>
+      </c>
+      <c r="E24" s="48" t="str">
+        <f>'THURSDAY SINGLES'!Y21</f>
+        <v/>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="13">
         <v>24.0</v>
       </c>
-      <c r="D25" s="49"/>
+      <c r="B25" s="48" t="str">
+        <f>'SUNDAY SINGLES'!Z24</f>
+        <v/>
+      </c>
+      <c r="C25" s="48" t="str">
+        <f>'SUNDAY SINGLES'!Z25</f>
+        <v/>
+      </c>
+      <c r="D25" s="49" t="str">
+        <f>'THURSDAY SINGLES'!Z20</f>
+        <v/>
+      </c>
+      <c r="E25" s="48" t="str">
+        <f>'THURSDAY SINGLES'!Z21</f>
+        <v/>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="14"/>

</xml_diff>

<commit_message>
054 Week 12/11 update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="115">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -1105,7 +1105,9 @@
       </c>
       <c r="L5" s="14"/>
       <c r="M5" s="15"/>
-      <c r="N5" s="14"/>
+      <c r="N5" s="13">
+        <v>28.0</v>
+      </c>
       <c r="O5" s="15"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="15"/>
@@ -1120,7 +1122,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>225</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6">
@@ -1158,7 +1160,9 @@
       <c r="M6" s="12">
         <v>31.0</v>
       </c>
-      <c r="N6" s="14"/>
+      <c r="N6" s="13">
+        <v>28.0</v>
+      </c>
       <c r="O6" s="15"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="15"/>
@@ -1173,7 +1177,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>310</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7">
@@ -1211,7 +1215,9 @@
       <c r="M7" s="12">
         <v>33.0</v>
       </c>
-      <c r="N7" s="14"/>
+      <c r="N7" s="13">
+        <v>25.0</v>
+      </c>
       <c r="O7" s="15"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="15"/>
@@ -1226,7 +1232,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>268</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8">
@@ -1264,7 +1270,9 @@
       <c r="M8" s="12">
         <v>41.0</v>
       </c>
-      <c r="N8" s="14"/>
+      <c r="N8" s="13">
+        <v>34.0</v>
+      </c>
       <c r="O8" s="15"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="15"/>
@@ -1279,7 +1287,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>329</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9">
@@ -1311,7 +1319,9 @@
       <c r="M9" s="12">
         <v>31.0</v>
       </c>
-      <c r="N9" s="14"/>
+      <c r="N9" s="13">
+        <v>25.0</v>
+      </c>
       <c r="O9" s="15"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="15"/>
@@ -1326,7 +1336,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>205</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10">
@@ -1358,7 +1368,9 @@
       <c r="M10" s="12">
         <v>36.0</v>
       </c>
-      <c r="N10" s="14"/>
+      <c r="N10" s="13">
+        <v>37.0</v>
+      </c>
       <c r="O10" s="15"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
@@ -1373,7 +1385,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>242</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11">
@@ -1450,7 +1462,9 @@
       <c r="M12" s="12">
         <v>35.0</v>
       </c>
-      <c r="N12" s="14"/>
+      <c r="N12" s="13">
+        <v>27.0</v>
+      </c>
       <c r="O12" s="15"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="15"/>
@@ -1465,7 +1479,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>328</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13">
@@ -1497,7 +1511,9 @@
         <v>25.0</v>
       </c>
       <c r="M13" s="15"/>
-      <c r="N13" s="14"/>
+      <c r="N13" s="13">
+        <v>34.0</v>
+      </c>
       <c r="O13" s="15"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="15"/>
@@ -1512,7 +1528,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14">
@@ -1542,7 +1558,9 @@
       <c r="M14" s="12">
         <v>36.0</v>
       </c>
-      <c r="N14" s="14"/>
+      <c r="N14" s="13">
+        <v>39.0</v>
+      </c>
       <c r="O14" s="15"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="15"/>
@@ -1557,7 +1575,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>184</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15">
@@ -1628,7 +1646,9 @@
       <c r="K16" s="15"/>
       <c r="L16" s="14"/>
       <c r="M16" s="15"/>
-      <c r="N16" s="14"/>
+      <c r="N16" s="13">
+        <v>33.0</v>
+      </c>
       <c r="O16" s="15"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="15"/>
@@ -1643,7 +1663,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>151</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17">
@@ -1683,7 +1703,9 @@
       <c r="M17" s="12">
         <v>36.0</v>
       </c>
-      <c r="N17" s="14"/>
+      <c r="N17" s="13">
+        <v>30.0</v>
+      </c>
       <c r="O17" s="15"/>
       <c r="P17" s="14"/>
       <c r="Q17" s="15"/>
@@ -1698,7 +1720,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>356</v>
+        <v>386</v>
       </c>
     </row>
     <row r="18">
@@ -1738,7 +1760,9 @@
       <c r="M18" s="12">
         <v>40.0</v>
       </c>
-      <c r="N18" s="14"/>
+      <c r="N18" s="13">
+        <v>33.0</v>
+      </c>
       <c r="O18" s="15"/>
       <c r="P18" s="14"/>
       <c r="Q18" s="15"/>
@@ -1753,7 +1777,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>346</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19">
@@ -1836,7 +1860,9 @@
       <c r="M20" s="12">
         <v>35.0</v>
       </c>
-      <c r="N20" s="14"/>
+      <c r="N20" s="13">
+        <v>33.0</v>
+      </c>
       <c r="O20" s="15"/>
       <c r="P20" s="14"/>
       <c r="Q20" s="15"/>
@@ -1851,7 +1877,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>275</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21">
@@ -1883,7 +1909,9 @@
       <c r="K21" s="15"/>
       <c r="L21" s="14"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="14"/>
+      <c r="N21" s="13">
+        <v>30.0</v>
+      </c>
       <c r="O21" s="15"/>
       <c r="P21" s="14"/>
       <c r="Q21" s="15"/>
@@ -1898,7 +1926,7 @@
       <c r="Z21" s="16"/>
       <c r="AA21" s="14">
         <f t="shared" si="1"/>
-        <v>224</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22">
@@ -1936,7 +1964,9 @@
       <c r="M22" s="12">
         <v>37.0</v>
       </c>
-      <c r="N22" s="14"/>
+      <c r="N22" s="13">
+        <v>30.0</v>
+      </c>
       <c r="O22" s="15"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="15"/>
@@ -1951,7 +1981,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>312</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2017,7 +2047,9 @@
       <c r="M24" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="N24" s="21"/>
+      <c r="N24" s="21" t="s">
+        <v>60</v>
+      </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
@@ -2069,7 +2101,9 @@
       <c r="M25" s="24">
         <v>41.0</v>
       </c>
-      <c r="N25" s="24"/>
+      <c r="N25" s="24">
+        <v>39.0</v>
+      </c>
       <c r="O25" s="24"/>
       <c r="P25" s="24"/>
       <c r="Q25" s="24"/>
@@ -2344,7 +2378,9 @@
       <c r="L6" s="13">
         <v>34.0</v>
       </c>
-      <c r="M6" s="15"/>
+      <c r="M6" s="12">
+        <v>32.0</v>
+      </c>
       <c r="N6" s="14"/>
       <c r="O6" s="15"/>
       <c r="P6" s="14"/>
@@ -2360,7 +2396,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>259</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7">
@@ -2393,7 +2429,9 @@
       <c r="L7" s="13">
         <v>33.0</v>
       </c>
-      <c r="M7" s="15"/>
+      <c r="M7" s="12">
+        <v>34.0</v>
+      </c>
       <c r="N7" s="14"/>
       <c r="O7" s="15"/>
       <c r="P7" s="14"/>
@@ -2409,7 +2447,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>254</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8">
@@ -2442,7 +2480,9 @@
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="15"/>
+      <c r="M8" s="12">
+        <v>35.0</v>
+      </c>
       <c r="N8" s="14"/>
       <c r="O8" s="15"/>
       <c r="P8" s="14"/>
@@ -2458,7 +2498,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>251</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9">
@@ -2489,7 +2529,9 @@
       <c r="L9" s="13">
         <v>30.0</v>
       </c>
-      <c r="M9" s="15"/>
+      <c r="M9" s="12">
+        <v>35.0</v>
+      </c>
       <c r="N9" s="14"/>
       <c r="O9" s="15"/>
       <c r="P9" s="14"/>
@@ -2505,7 +2547,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10">
@@ -2536,7 +2578,9 @@
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="15"/>
+      <c r="M10" s="12">
+        <v>28.0</v>
+      </c>
       <c r="N10" s="14"/>
       <c r="O10" s="15"/>
       <c r="P10" s="14"/>
@@ -2552,7 +2596,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>243</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11">
@@ -2632,7 +2676,9 @@
       <c r="L12" s="13">
         <v>27.0</v>
       </c>
-      <c r="M12" s="15"/>
+      <c r="M12" s="12">
+        <v>30.0</v>
+      </c>
       <c r="N12" s="14"/>
       <c r="O12" s="15"/>
       <c r="P12" s="14"/>
@@ -2648,7 +2694,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>276</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13">
@@ -2718,7 +2764,9 @@
       <c r="L14" s="13">
         <v>31.0</v>
       </c>
-      <c r="M14" s="15"/>
+      <c r="M14" s="12">
+        <v>28.0</v>
+      </c>
       <c r="N14" s="14"/>
       <c r="O14" s="15"/>
       <c r="P14" s="14"/>
@@ -2734,7 +2782,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15">
@@ -2765,7 +2813,9 @@
       <c r="L15" s="13">
         <v>28.0</v>
       </c>
-      <c r="M15" s="15"/>
+      <c r="M15" s="12">
+        <v>32.0</v>
+      </c>
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
       <c r="P15" s="14"/>
@@ -2781,7 +2831,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16">
@@ -2906,7 +2956,9 @@
       <c r="L18" s="12">
         <v>33.0</v>
       </c>
-      <c r="M18" s="15"/>
+      <c r="M18" s="12">
+        <v>26.0</v>
+      </c>
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
@@ -2922,7 +2974,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>182</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -2985,7 +3037,9 @@
       <c r="L20" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="M20" s="21"/>
+      <c r="M20" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="N20" s="21"/>
       <c r="O20" s="21"/>
       <c r="P20" s="21"/>
@@ -3035,7 +3089,9 @@
       <c r="L21" s="24">
         <v>34.0</v>
       </c>
-      <c r="M21" s="24"/>
+      <c r="M21" s="24">
+        <v>35.0</v>
+      </c>
       <c r="N21" s="24"/>
       <c r="O21" s="24"/>
       <c r="P21" s="24"/>
@@ -7371,13 +7427,17 @@
       <c r="B12" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="42"/>
+      <c r="C12" s="42" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="13">
         <v>12.0</v>
       </c>
-      <c r="B13" s="41"/>
+      <c r="B13" s="41" t="s">
+        <v>62</v>
+      </c>
       <c r="C13" s="42"/>
     </row>
     <row r="14">
@@ -12580,11 +12640,11 @@
       </c>
       <c r="D12" s="49" t="str">
         <f>'THURSDAY SINGLES'!M20</f>
-        <v/>
-      </c>
-      <c r="E12" s="48" t="str">
+        <v>LES DOBBINS</v>
+      </c>
+      <c r="E12" s="48">
         <f>'THURSDAY SINGLES'!M21</f>
-        <v/>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -12593,11 +12653,11 @@
       </c>
       <c r="B13" s="48" t="str">
         <f>'SUNDAY SINGLES'!N24</f>
-        <v/>
-      </c>
-      <c r="C13" s="48" t="str">
+        <v>TONY SLATER</v>
+      </c>
+      <c r="C13" s="48">
         <f>'SUNDAY SINGLES'!N25</f>
-        <v/>
+        <v>39</v>
       </c>
       <c r="D13" s="49" t="str">
         <f>'THURSDAY SINGLES'!N20</f>

</xml_diff>

<commit_message>
055 Week 13/12 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="115">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -230,6 +230,9 @@
     <t>FRED HOLINGWORTH</t>
   </si>
   <si>
+    <t>FRED HOLLINGWORTH</t>
+  </si>
+  <si>
     <t>WINNERS SCORE</t>
   </si>
   <si>
@@ -345,9 +348,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>FRED HOLLINGWORTH</t>
   </si>
   <si>
     <t>SUNDAY</t>
@@ -1163,7 +1163,9 @@
       <c r="N6" s="13">
         <v>28.0</v>
       </c>
-      <c r="O6" s="15"/>
+      <c r="O6" s="12">
+        <v>37.0</v>
+      </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="14"/>
@@ -1177,7 +1179,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>338</v>
+        <v>375</v>
       </c>
     </row>
     <row r="7">
@@ -1273,7 +1275,9 @@
       <c r="N8" s="13">
         <v>34.0</v>
       </c>
-      <c r="O8" s="15"/>
+      <c r="O8" s="12">
+        <v>28.0</v>
+      </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="14"/>
@@ -1287,7 +1291,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>363</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9">
@@ -1322,7 +1326,9 @@
       <c r="N9" s="13">
         <v>25.0</v>
       </c>
-      <c r="O9" s="15"/>
+      <c r="O9" s="12">
+        <v>30.0</v>
+      </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="15"/>
       <c r="R9" s="14"/>
@@ -1336,7 +1342,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10">
@@ -1371,7 +1377,9 @@
       <c r="N10" s="13">
         <v>37.0</v>
       </c>
-      <c r="O10" s="15"/>
+      <c r="O10" s="12">
+        <v>41.0</v>
+      </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
       <c r="R10" s="14"/>
@@ -1385,7 +1393,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>279</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11">
@@ -1408,7 +1416,9 @@
         <v>39.0</v>
       </c>
       <c r="N11" s="14"/>
-      <c r="O11" s="15"/>
+      <c r="O11" s="12">
+        <v>32.0</v>
+      </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="14"/>
@@ -1422,7 +1432,7 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12">
@@ -1514,7 +1524,9 @@
       <c r="N13" s="13">
         <v>34.0</v>
       </c>
-      <c r="O13" s="15"/>
+      <c r="O13" s="12">
+        <v>38.0</v>
+      </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="15"/>
       <c r="R13" s="14"/>
@@ -1528,7 +1540,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>232</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14">
@@ -1561,7 +1573,9 @@
       <c r="N14" s="13">
         <v>39.0</v>
       </c>
-      <c r="O14" s="15"/>
+      <c r="O14" s="12">
+        <v>33.0</v>
+      </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="14"/>
@@ -1575,7 +1589,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>223</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15">
@@ -1649,7 +1663,9 @@
       <c r="N16" s="13">
         <v>33.0</v>
       </c>
-      <c r="O16" s="15"/>
+      <c r="O16" s="12">
+        <v>34.0</v>
+      </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="14"/>
@@ -1663,7 +1679,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>184</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17">
@@ -1706,7 +1722,9 @@
       <c r="N17" s="13">
         <v>30.0</v>
       </c>
-      <c r="O17" s="15"/>
+      <c r="O17" s="12">
+        <v>37.0</v>
+      </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="14"/>
@@ -1720,7 +1738,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>386</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18">
@@ -1763,7 +1781,9 @@
       <c r="N18" s="13">
         <v>33.0</v>
       </c>
-      <c r="O18" s="15"/>
+      <c r="O18" s="12">
+        <v>39.0</v>
+      </c>
       <c r="P18" s="14"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="14"/>
@@ -1777,7 +1797,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>379</v>
+        <v>418</v>
       </c>
     </row>
     <row r="19">
@@ -1863,7 +1883,9 @@
       <c r="N20" s="13">
         <v>33.0</v>
       </c>
-      <c r="O20" s="15"/>
+      <c r="O20" s="12">
+        <v>41.0</v>
+      </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="15"/>
       <c r="R20" s="14"/>
@@ -1877,7 +1899,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>308</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21">
@@ -1967,7 +1989,9 @@
       <c r="N22" s="13">
         <v>30.0</v>
       </c>
-      <c r="O22" s="15"/>
+      <c r="O22" s="12">
+        <v>37.0</v>
+      </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="15"/>
       <c r="R22" s="14"/>
@@ -1981,7 +2005,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>342</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2050,7 +2074,9 @@
       <c r="N24" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="O24" s="21"/>
+      <c r="O24" s="21" t="s">
+        <v>71</v>
+      </c>
       <c r="P24" s="21"/>
       <c r="Q24" s="21"/>
       <c r="R24" s="21"/>
@@ -2066,7 +2092,7 @@
     </row>
     <row r="25">
       <c r="B25" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="24">
         <v>35.0</v>
@@ -2104,7 +2130,9 @@
       <c r="N25" s="24">
         <v>39.0</v>
       </c>
-      <c r="O25" s="24"/>
+      <c r="O25" s="24">
+        <v>41.0</v>
+      </c>
       <c r="P25" s="24"/>
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
@@ -2141,83 +2169,83 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AA3" s="6"/>
     </row>
@@ -2381,7 +2409,9 @@
       <c r="M6" s="12">
         <v>32.0</v>
       </c>
-      <c r="N6" s="14"/>
+      <c r="N6" s="13">
+        <v>33.0</v>
+      </c>
       <c r="O6" s="15"/>
       <c r="P6" s="14"/>
       <c r="Q6" s="15"/>
@@ -2396,7 +2426,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>291</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7">
@@ -2432,7 +2462,9 @@
       <c r="M7" s="12">
         <v>34.0</v>
       </c>
-      <c r="N7" s="14"/>
+      <c r="N7" s="13">
+        <v>35.0</v>
+      </c>
       <c r="O7" s="15"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="15"/>
@@ -2447,7 +2479,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>288</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8">
@@ -2483,7 +2515,9 @@
       <c r="M8" s="12">
         <v>35.0</v>
       </c>
-      <c r="N8" s="14"/>
+      <c r="N8" s="13">
+        <v>41.0</v>
+      </c>
       <c r="O8" s="15"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="15"/>
@@ -2498,7 +2532,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>286</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9">
@@ -2532,7 +2566,9 @@
       <c r="M9" s="12">
         <v>35.0</v>
       </c>
-      <c r="N9" s="14"/>
+      <c r="N9" s="13">
+        <v>32.0</v>
+      </c>
       <c r="O9" s="15"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="15"/>
@@ -2547,7 +2583,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>243</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10">
@@ -2581,7 +2617,9 @@
       <c r="M10" s="12">
         <v>28.0</v>
       </c>
-      <c r="N10" s="14"/>
+      <c r="N10" s="13">
+        <v>37.0</v>
+      </c>
       <c r="O10" s="15"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
@@ -2596,12 +2634,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>271</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C11" s="12">
         <v>22.0</v>
@@ -2646,7 +2684,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C12" s="12">
         <v>28.0</v>
@@ -2699,7 +2737,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" s="12">
         <v>31.0</v>
@@ -2767,7 +2805,9 @@
       <c r="M14" s="12">
         <v>28.0</v>
       </c>
-      <c r="N14" s="14"/>
+      <c r="N14" s="13">
+        <v>34.0</v>
+      </c>
       <c r="O14" s="15"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="15"/>
@@ -2782,7 +2822,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15">
@@ -2816,7 +2856,9 @@
       <c r="M15" s="12">
         <v>32.0</v>
       </c>
-      <c r="N15" s="14"/>
+      <c r="N15" s="13">
+        <v>34.0</v>
+      </c>
       <c r="O15" s="15"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="15"/>
@@ -2831,12 +2873,12 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C16" s="12">
         <v>32.0</v>
@@ -2932,7 +2974,7 @@
     </row>
     <row r="18">
       <c r="B18" s="26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C18" s="12">
         <v>27.0</v>
@@ -2959,7 +3001,9 @@
       <c r="M18" s="12">
         <v>26.0</v>
       </c>
-      <c r="N18" s="15"/>
+      <c r="N18" s="12">
+        <v>26.0</v>
+      </c>
       <c r="O18" s="15"/>
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
@@ -2974,7 +3018,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -3014,10 +3058,10 @@
         <v>56</v>
       </c>
       <c r="E20" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>99</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>64</v>
@@ -3029,7 +3073,7 @@
         <v>64</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>57</v>
@@ -3040,7 +3084,9 @@
       <c r="M20" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="N20" s="21"/>
+      <c r="N20" s="21" t="s">
+        <v>60</v>
+      </c>
       <c r="O20" s="21"/>
       <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
@@ -3057,7 +3103,7 @@
     </row>
     <row r="21">
       <c r="B21" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C21" s="24">
         <v>40.0</v>
@@ -3092,7 +3138,9 @@
       <c r="M21" s="24">
         <v>35.0</v>
       </c>
-      <c r="N21" s="24"/>
+      <c r="N21" s="24">
+        <v>41.0</v>
+      </c>
       <c r="O21" s="24"/>
       <c r="P21" s="24"/>
       <c r="Q21" s="24"/>
@@ -3131,10 +3179,10 @@
         <v>25</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
@@ -3145,7 +3193,7 @@
         <v>14.0</v>
       </c>
       <c r="C2" s="32">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="3">
@@ -3164,10 +3212,10 @@
         <v>53</v>
       </c>
       <c r="B4" s="31">
+        <v>23.0</v>
+      </c>
+      <c r="C4" s="32">
         <v>21.0</v>
-      </c>
-      <c r="C4" s="32">
-        <v>19.0</v>
       </c>
     </row>
     <row r="5">
@@ -3175,7 +3223,7 @@
         <v>54</v>
       </c>
       <c r="B5" s="31">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C5" s="32">
         <v>13.0</v>
@@ -3197,10 +3245,10 @@
         <v>56</v>
       </c>
       <c r="B7" s="31">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="C7" s="32">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="8">
@@ -3208,7 +3256,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="31">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="C8" s="32">
         <v>6.0</v>
@@ -3230,7 +3278,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="31">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="C10" s="32">
         <v>7.0</v>
@@ -3241,10 +3289,10 @@
         <v>60</v>
       </c>
       <c r="B11" s="31">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="C11" s="32">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="12">
@@ -3274,10 +3322,10 @@
         <v>63</v>
       </c>
       <c r="B14" s="31">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="C14" s="32">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="15">
@@ -3285,10 +3333,10 @@
         <v>64</v>
       </c>
       <c r="B15" s="31">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
       <c r="C15" s="32">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="16">
@@ -3307,10 +3355,10 @@
         <v>66</v>
       </c>
       <c r="B17" s="31">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="C17" s="32">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="18">
@@ -3337,29 +3385,29 @@
     </row>
     <row r="20">
       <c r="A20" s="33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B20" s="31">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="C20" s="32">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B21" s="31">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="C21" s="32">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B22" s="31">
         <v>15.0</v>
@@ -3370,7 +3418,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B23" s="31">
         <v>30.0</v>
@@ -3381,7 +3429,7 @@
     </row>
     <row r="24">
       <c r="A24" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B24" s="34">
         <v>27.0</v>
@@ -7300,13 +7348,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
@@ -7350,7 +7398,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -7361,7 +7409,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
@@ -7380,7 +7428,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>67</v>
@@ -7394,7 +7442,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10">
@@ -7405,7 +7453,7 @@
         <v>63</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7414,10 +7462,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12">
@@ -7425,10 +7473,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13">
@@ -7438,13 +7486,17 @@
       <c r="B13" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="42" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="13">
         <v>13.0</v>
       </c>
-      <c r="B14" s="41"/>
+      <c r="B14" s="41" t="s">
+        <v>60</v>
+      </c>
       <c r="C14" s="43"/>
     </row>
     <row r="15">
@@ -12401,7 +12453,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>111</v>
@@ -12661,11 +12713,11 @@
       </c>
       <c r="D13" s="49" t="str">
         <f>'THURSDAY SINGLES'!N20</f>
-        <v/>
-      </c>
-      <c r="E13" s="48" t="str">
+        <v>TONY SLATER</v>
+      </c>
+      <c r="E13" s="48">
         <f>'THURSDAY SINGLES'!N$21</f>
-        <v/>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
@@ -12674,11 +12726,11 @@
       </c>
       <c r="B14" s="48" t="str">
         <f>'SUNDAY SINGLES'!O24</f>
-        <v/>
-      </c>
-      <c r="C14" s="48" t="str">
+        <v>FRED HOLLINGWORTH</v>
+      </c>
+      <c r="C14" s="48">
         <f>'SUNDAY SINGLES'!O25</f>
-        <v/>
+        <v>41</v>
       </c>
       <c r="D14" s="49" t="str">
         <f>'THURSDAY SINGLES'!O20</f>

</xml_diff>

<commit_message>
056 Week 14/13 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="115">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -1109,7 +1109,9 @@
         <v>28.0</v>
       </c>
       <c r="O5" s="15"/>
-      <c r="P5" s="14"/>
+      <c r="P5" s="13">
+        <v>25.0</v>
+      </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="14"/>
       <c r="S5" s="15"/>
@@ -1122,7 +1124,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>253</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6">
@@ -1221,7 +1223,9 @@
         <v>25.0</v>
       </c>
       <c r="O7" s="15"/>
-      <c r="P7" s="14"/>
+      <c r="P7" s="13">
+        <v>37.0</v>
+      </c>
       <c r="Q7" s="15"/>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
@@ -1234,7 +1238,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>293</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8">
@@ -1278,7 +1282,9 @@
       <c r="O8" s="12">
         <v>28.0</v>
       </c>
-      <c r="P8" s="14"/>
+      <c r="P8" s="13">
+        <v>29.0</v>
+      </c>
       <c r="Q8" s="15"/>
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
@@ -1291,7 +1297,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>391</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9">
@@ -1419,7 +1425,9 @@
       <c r="O11" s="12">
         <v>32.0</v>
       </c>
-      <c r="P11" s="14"/>
+      <c r="P11" s="13">
+        <v>32.0</v>
+      </c>
       <c r="Q11" s="15"/>
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
@@ -1432,7 +1440,7 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12">
@@ -1476,7 +1484,9 @@
         <v>27.0</v>
       </c>
       <c r="O12" s="15"/>
-      <c r="P12" s="14"/>
+      <c r="P12" s="13">
+        <v>32.0</v>
+      </c>
       <c r="Q12" s="15"/>
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
@@ -1489,7 +1499,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>355</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13">
@@ -1576,7 +1586,9 @@
       <c r="O14" s="12">
         <v>33.0</v>
       </c>
-      <c r="P14" s="14"/>
+      <c r="P14" s="13">
+        <v>33.0</v>
+      </c>
       <c r="Q14" s="15"/>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
@@ -1589,7 +1601,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>256</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15">
@@ -1666,7 +1678,9 @@
       <c r="O16" s="12">
         <v>34.0</v>
       </c>
-      <c r="P16" s="14"/>
+      <c r="P16" s="13">
+        <v>39.0</v>
+      </c>
       <c r="Q16" s="15"/>
       <c r="R16" s="14"/>
       <c r="S16" s="15"/>
@@ -1679,7 +1693,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>218</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17">
@@ -1784,7 +1798,9 @@
       <c r="O18" s="12">
         <v>39.0</v>
       </c>
-      <c r="P18" s="14"/>
+      <c r="P18" s="13">
+        <v>25.0</v>
+      </c>
       <c r="Q18" s="15"/>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
@@ -1797,7 +1813,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>418</v>
+        <v>443</v>
       </c>
     </row>
     <row r="19">
@@ -2077,7 +2093,9 @@
       <c r="O24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="P24" s="21"/>
+      <c r="P24" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="Q24" s="21"/>
       <c r="R24" s="21"/>
       <c r="S24" s="21"/>
@@ -2133,7 +2151,9 @@
       <c r="O25" s="24">
         <v>41.0</v>
       </c>
-      <c r="P25" s="24"/>
+      <c r="P25" s="24">
+        <v>39.0</v>
+      </c>
       <c r="Q25" s="24"/>
       <c r="R25" s="24"/>
       <c r="S25" s="24"/>
@@ -2359,7 +2379,9 @@
       <c r="L5" s="14"/>
       <c r="M5" s="15"/>
       <c r="N5" s="14"/>
-      <c r="O5" s="15"/>
+      <c r="O5" s="12">
+        <v>42.0</v>
+      </c>
       <c r="P5" s="14"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="14"/>
@@ -2373,7 +2395,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>211</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6">
@@ -2465,7 +2487,9 @@
       <c r="N7" s="13">
         <v>35.0</v>
       </c>
-      <c r="O7" s="15"/>
+      <c r="O7" s="12">
+        <v>31.0</v>
+      </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="15"/>
       <c r="R7" s="14"/>
@@ -2479,7 +2503,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8">
@@ -2518,7 +2542,9 @@
       <c r="N8" s="13">
         <v>41.0</v>
       </c>
-      <c r="O8" s="15"/>
+      <c r="O8" s="12">
+        <v>31.0</v>
+      </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="15"/>
       <c r="R8" s="14"/>
@@ -2532,7 +2558,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>327</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9">
@@ -2569,7 +2595,9 @@
       <c r="N9" s="13">
         <v>32.0</v>
       </c>
-      <c r="O9" s="15"/>
+      <c r="O9" s="12">
+        <v>34.0</v>
+      </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="15"/>
       <c r="R9" s="14"/>
@@ -2583,7 +2611,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>275</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10">
@@ -2718,7 +2746,9 @@
         <v>30.0</v>
       </c>
       <c r="N12" s="14"/>
-      <c r="O12" s="15"/>
+      <c r="O12" s="12">
+        <v>24.0</v>
+      </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="14"/>
@@ -2732,7 +2762,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>306</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13">
@@ -2808,7 +2838,9 @@
       <c r="N14" s="13">
         <v>34.0</v>
       </c>
-      <c r="O14" s="15"/>
+      <c r="O14" s="12">
+        <v>28.0</v>
+      </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="15"/>
       <c r="R14" s="14"/>
@@ -2822,7 +2854,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>178</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15">
@@ -2859,7 +2891,9 @@
       <c r="N15" s="13">
         <v>34.0</v>
       </c>
-      <c r="O15" s="15"/>
+      <c r="O15" s="12">
+        <v>30.0</v>
+      </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="15"/>
       <c r="R15" s="14"/>
@@ -2873,7 +2907,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>274</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16">
@@ -2908,7 +2942,9 @@
       </c>
       <c r="M16" s="15"/>
       <c r="N16" s="14"/>
-      <c r="O16" s="15"/>
+      <c r="O16" s="12">
+        <v>37.0</v>
+      </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="15"/>
       <c r="R16" s="14"/>
@@ -2922,7 +2958,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>223</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17">
@@ -2955,7 +2991,9 @@
       <c r="L17" s="14"/>
       <c r="M17" s="15"/>
       <c r="N17" s="14"/>
-      <c r="O17" s="15"/>
+      <c r="O17" s="12">
+        <v>37.0</v>
+      </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="15"/>
       <c r="R17" s="14"/>
@@ -2969,7 +3007,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>232</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18">
@@ -3004,7 +3042,9 @@
       <c r="N18" s="12">
         <v>26.0</v>
       </c>
-      <c r="O18" s="15"/>
+      <c r="O18" s="12">
+        <v>29.0</v>
+      </c>
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
@@ -3018,7 +3058,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>234</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -3087,7 +3127,9 @@
       <c r="N20" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="21"/>
+      <c r="O20" s="21" t="s">
+        <v>51</v>
+      </c>
       <c r="P20" s="21"/>
       <c r="Q20" s="21"/>
       <c r="R20" s="21"/>
@@ -3141,7 +3183,9 @@
       <c r="N21" s="24">
         <v>41.0</v>
       </c>
-      <c r="O21" s="24"/>
+      <c r="O21" s="24">
+        <v>42.0</v>
+      </c>
       <c r="P21" s="24"/>
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
@@ -3311,10 +3355,10 @@
         <v>62</v>
       </c>
       <c r="B13" s="31">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="C13" s="32">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="14">
@@ -7497,13 +7541,17 @@
       <c r="B14" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="43"/>
+      <c r="C14" s="42" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="13">
         <v>14.0</v>
       </c>
-      <c r="B15" s="41"/>
+      <c r="B15" s="41" t="s">
+        <v>110</v>
+      </c>
       <c r="C15" s="43"/>
     </row>
     <row r="16">
@@ -12734,11 +12782,11 @@
       </c>
       <c r="D14" s="49" t="str">
         <f>'THURSDAY SINGLES'!O20</f>
-        <v/>
-      </c>
-      <c r="E14" s="48" t="str">
+        <v>BAZ MASON</v>
+      </c>
+      <c r="E14" s="48">
         <f>'THURSDAY SINGLES'!O21</f>
-        <v/>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
@@ -12747,11 +12795,11 @@
       </c>
       <c r="B15" s="48" t="str">
         <f>'SUNDAY SINGLES'!P24</f>
-        <v/>
-      </c>
-      <c r="C15" s="48" t="str">
+        <v>STEVE FELLOWS</v>
+      </c>
+      <c r="C15" s="48">
         <f>'SUNDAY SINGLES'!P25</f>
-        <v/>
+        <v>39</v>
       </c>
       <c r="D15" s="49" t="str">
         <f>'THURSDAY SINGLES'!P20</f>

</xml_diff>

<commit_message>
057 Name data normalization
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="114">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -215,7 +215,7 @@
     <t>PAUL HANCOX</t>
   </si>
   <si>
-    <t>FRED HOLLIWORTH</t>
+    <t>FRED HOLLINGWORTH</t>
   </si>
   <si>
     <t>SCOTT LEONARDE</t>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>FRED HOLINGWORTH</t>
-  </si>
-  <si>
-    <t>FRED HOLLINGWORTH</t>
   </si>
   <si>
     <t>WINNERS SCORE</t>
@@ -2091,7 +2088,7 @@
         <v>60</v>
       </c>
       <c r="O24" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P24" s="21" t="s">
         <v>62</v>
@@ -2110,7 +2107,7 @@
     </row>
     <row r="25">
       <c r="B25" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="24">
         <v>35.0</v>
@@ -2189,83 +2186,83 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="V3" s="4" t="s">
+      <c r="W3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="Y3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="AA3" s="6"/>
     </row>
@@ -2667,7 +2664,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="12">
         <v>22.0</v>
@@ -2712,7 +2709,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="12">
         <v>28.0</v>
@@ -2767,7 +2764,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="12">
         <v>31.0</v>
@@ -2912,7 +2909,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="12">
         <v>32.0</v>
@@ -3012,7 +3009,7 @@
     </row>
     <row r="18">
       <c r="B18" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="12">
         <v>27.0</v>
@@ -3098,10 +3095,10 @@
         <v>56</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>64</v>
@@ -3113,7 +3110,7 @@
         <v>64</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>57</v>
@@ -3145,7 +3142,7 @@
     </row>
     <row r="21">
       <c r="B21" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="24">
         <v>40.0</v>
@@ -3223,10 +3220,10 @@
         <v>25</v>
       </c>
       <c r="B1" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>103</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2">
@@ -3429,7 +3426,7 @@
     </row>
     <row r="20">
       <c r="A20" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="31">
         <v>19.0</v>
@@ -3440,7 +3437,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B21" s="31">
         <v>18.0</v>
@@ -3451,7 +3448,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B22" s="31">
         <v>15.0</v>
@@ -3462,7 +3459,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="31">
         <v>30.0</v>
@@ -3473,7 +3470,7 @@
     </row>
     <row r="24">
       <c r="A24" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B24" s="34">
         <v>27.0</v>
@@ -7392,13 +7389,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2">
@@ -7442,7 +7439,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6">
@@ -7453,7 +7450,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7">
@@ -7472,7 +7469,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>67</v>
@@ -7486,7 +7483,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
@@ -7497,7 +7494,7 @@
         <v>63</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7506,10 +7503,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12">
@@ -7517,10 +7514,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
@@ -7531,7 +7528,7 @@
         <v>62</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
@@ -7550,7 +7547,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="43"/>
     </row>
@@ -12501,19 +12498,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="E1" s="23" t="s">
         <v>113</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
058 Week 15/14 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="114">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -1109,7 +1109,9 @@
       <c r="P5" s="13">
         <v>25.0</v>
       </c>
-      <c r="Q5" s="15"/>
+      <c r="Q5" s="12">
+        <v>36.0</v>
+      </c>
       <c r="R5" s="14"/>
       <c r="S5" s="15"/>
       <c r="T5" s="14"/>
@@ -1121,7 +1123,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>278</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6">
@@ -1223,7 +1225,9 @@
       <c r="P7" s="13">
         <v>37.0</v>
       </c>
-      <c r="Q7" s="15"/>
+      <c r="Q7" s="12">
+        <v>28.0</v>
+      </c>
       <c r="R7" s="14"/>
       <c r="S7" s="15"/>
       <c r="T7" s="14"/>
@@ -1235,7 +1239,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>330</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8">
@@ -1282,7 +1286,9 @@
       <c r="P8" s="13">
         <v>29.0</v>
       </c>
-      <c r="Q8" s="15"/>
+      <c r="Q8" s="12">
+        <v>33.0</v>
+      </c>
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
       <c r="T8" s="14"/>
@@ -1294,7 +1300,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>420</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9">
@@ -1384,7 +1390,9 @@
         <v>41.0</v>
       </c>
       <c r="P10" s="14"/>
-      <c r="Q10" s="15"/>
+      <c r="Q10" s="12">
+        <v>37.0</v>
+      </c>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
       <c r="T10" s="14"/>
@@ -1396,7 +1404,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11">
@@ -1586,7 +1594,9 @@
       <c r="P14" s="13">
         <v>33.0</v>
       </c>
-      <c r="Q14" s="15"/>
+      <c r="Q14" s="12">
+        <v>31.0</v>
+      </c>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
       <c r="T14" s="14"/>
@@ -1598,7 +1608,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>289</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15">
@@ -1627,7 +1637,9 @@
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
       <c r="P15" s="14"/>
-      <c r="Q15" s="15"/>
+      <c r="Q15" s="12">
+        <v>36.0</v>
+      </c>
       <c r="R15" s="14"/>
       <c r="S15" s="15"/>
       <c r="T15" s="14"/>
@@ -1639,7 +1651,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>124</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16">
@@ -1678,7 +1690,9 @@
       <c r="P16" s="13">
         <v>39.0</v>
       </c>
-      <c r="Q16" s="15"/>
+      <c r="Q16" s="12">
+        <v>28.0</v>
+      </c>
       <c r="R16" s="14"/>
       <c r="S16" s="15"/>
       <c r="T16" s="14"/>
@@ -1690,7 +1704,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>257</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17">
@@ -1737,7 +1751,9 @@
         <v>37.0</v>
       </c>
       <c r="P17" s="14"/>
-      <c r="Q17" s="15"/>
+      <c r="Q17" s="12">
+        <v>29.0</v>
+      </c>
       <c r="R17" s="14"/>
       <c r="S17" s="15"/>
       <c r="T17" s="14"/>
@@ -1749,7 +1765,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>423</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18">
@@ -1900,7 +1916,9 @@
         <v>41.0</v>
       </c>
       <c r="P20" s="14"/>
-      <c r="Q20" s="15"/>
+      <c r="Q20" s="12">
+        <v>32.0</v>
+      </c>
       <c r="R20" s="14"/>
       <c r="S20" s="15"/>
       <c r="T20" s="14"/>
@@ -1912,7 +1930,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>349</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21">
@@ -1949,7 +1967,9 @@
       </c>
       <c r="O21" s="15"/>
       <c r="P21" s="14"/>
-      <c r="Q21" s="15"/>
+      <c r="Q21" s="12">
+        <v>25.0</v>
+      </c>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
       <c r="T21" s="14"/>
@@ -1961,7 +1981,7 @@
       <c r="Z21" s="16"/>
       <c r="AA21" s="14">
         <f t="shared" si="1"/>
-        <v>254</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22">
@@ -2006,7 +2026,9 @@
         <v>37.0</v>
       </c>
       <c r="P22" s="14"/>
-      <c r="Q22" s="15"/>
+      <c r="Q22" s="12">
+        <v>37.0</v>
+      </c>
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
       <c r="T22" s="14"/>
@@ -2018,7 +2040,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>379</v>
+        <v>416</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2093,7 +2115,9 @@
       <c r="P24" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="Q24" s="21"/>
+      <c r="Q24" s="21" t="s">
+        <v>68</v>
+      </c>
       <c r="R24" s="21"/>
       <c r="S24" s="21"/>
       <c r="T24" s="21"/>
@@ -2151,7 +2175,9 @@
       <c r="P25" s="24">
         <v>39.0</v>
       </c>
-      <c r="Q25" s="24"/>
+      <c r="Q25" s="24">
+        <v>37.0</v>
+      </c>
       <c r="R25" s="24"/>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
@@ -2379,7 +2405,9 @@
       <c r="O5" s="12">
         <v>42.0</v>
       </c>
-      <c r="P5" s="14"/>
+      <c r="P5" s="13">
+        <v>37.0</v>
+      </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="14"/>
       <c r="S5" s="15"/>
@@ -2392,7 +2420,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>253</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6">
@@ -2542,7 +2570,9 @@
       <c r="O8" s="12">
         <v>31.0</v>
       </c>
-      <c r="P8" s="14"/>
+      <c r="P8" s="13">
+        <v>39.0</v>
+      </c>
       <c r="Q8" s="15"/>
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
@@ -2555,7 +2585,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>358</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9">
@@ -2595,7 +2625,9 @@
       <c r="O9" s="12">
         <v>34.0</v>
       </c>
-      <c r="P9" s="14"/>
+      <c r="P9" s="13">
+        <v>30.0</v>
+      </c>
       <c r="Q9" s="15"/>
       <c r="R9" s="14"/>
       <c r="S9" s="15"/>
@@ -2608,7 +2640,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>309</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10">
@@ -2646,7 +2678,9 @@
         <v>37.0</v>
       </c>
       <c r="O10" s="15"/>
-      <c r="P10" s="14"/>
+      <c r="P10" s="13">
+        <v>30.0</v>
+      </c>
       <c r="Q10" s="15"/>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
@@ -2659,7 +2693,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>308</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11">
@@ -2746,7 +2780,9 @@
       <c r="O12" s="12">
         <v>24.0</v>
       </c>
-      <c r="P12" s="14"/>
+      <c r="P12" s="13">
+        <v>40.0</v>
+      </c>
       <c r="Q12" s="15"/>
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
@@ -2759,7 +2795,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>330</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13">
@@ -2791,7 +2827,9 @@
       <c r="M13" s="15"/>
       <c r="N13" s="14"/>
       <c r="O13" s="15"/>
-      <c r="P13" s="14"/>
+      <c r="P13" s="13">
+        <v>34.0</v>
+      </c>
       <c r="Q13" s="15"/>
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
@@ -2804,7 +2842,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>196</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14">
@@ -2838,7 +2876,9 @@
       <c r="O14" s="12">
         <v>28.0</v>
       </c>
-      <c r="P14" s="14"/>
+      <c r="P14" s="13">
+        <v>34.0</v>
+      </c>
       <c r="Q14" s="15"/>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
@@ -2851,7 +2891,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>206</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15">
@@ -2891,7 +2931,9 @@
       <c r="O15" s="12">
         <v>30.0</v>
       </c>
-      <c r="P15" s="14"/>
+      <c r="P15" s="13">
+        <v>38.0</v>
+      </c>
       <c r="Q15" s="15"/>
       <c r="R15" s="14"/>
       <c r="S15" s="15"/>
@@ -2904,7 +2946,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>304</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16">
@@ -2942,7 +2984,9 @@
       <c r="O16" s="12">
         <v>37.0</v>
       </c>
-      <c r="P16" s="14"/>
+      <c r="P16" s="13">
+        <v>34.0</v>
+      </c>
       <c r="Q16" s="15"/>
       <c r="R16" s="14"/>
       <c r="S16" s="15"/>
@@ -2955,7 +2999,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>260</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17">
@@ -2991,7 +3035,9 @@
       <c r="O17" s="12">
         <v>37.0</v>
       </c>
-      <c r="P17" s="14"/>
+      <c r="P17" s="13">
+        <v>33.0</v>
+      </c>
       <c r="Q17" s="15"/>
       <c r="R17" s="14"/>
       <c r="S17" s="15"/>
@@ -3004,7 +3050,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>269</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18">
@@ -3127,7 +3173,9 @@
       <c r="O20" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="P20" s="21"/>
+      <c r="P20" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="Q20" s="21"/>
       <c r="R20" s="21"/>
       <c r="S20" s="21"/>
@@ -3183,7 +3231,9 @@
       <c r="O21" s="24">
         <v>42.0</v>
       </c>
-      <c r="P21" s="24"/>
+      <c r="P21" s="24">
+        <v>40.0</v>
+      </c>
       <c r="Q21" s="24"/>
       <c r="R21" s="24"/>
       <c r="S21" s="24"/>
@@ -3231,7 +3281,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="31">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="C2" s="32">
         <v>13.0</v>
@@ -3253,7 +3303,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="31">
-        <v>23.0</v>
+        <v>22.0</v>
       </c>
       <c r="C4" s="32">
         <v>21.0</v>
@@ -3267,7 +3317,7 @@
         <v>14.0</v>
       </c>
       <c r="C5" s="32">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="6">
@@ -3330,10 +3380,10 @@
         <v>60</v>
       </c>
       <c r="B11" s="31">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="C11" s="32">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="12">
@@ -3344,7 +3394,7 @@
         <v>18.0</v>
       </c>
       <c r="C12" s="32">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="13">
@@ -3352,7 +3402,7 @@
         <v>62</v>
       </c>
       <c r="B13" s="31">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="C13" s="32">
         <v>19.0</v>
@@ -3377,7 +3427,7 @@
         <v>29.0</v>
       </c>
       <c r="C15" s="32">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="16">
@@ -3418,10 +3468,10 @@
         <v>68</v>
       </c>
       <c r="B19" s="31">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="C19" s="32">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="20">
@@ -3440,10 +3490,10 @@
         <v>98</v>
       </c>
       <c r="B21" s="31">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="C21" s="32">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="22">
@@ -3462,10 +3512,10 @@
         <v>97</v>
       </c>
       <c r="B23" s="31">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="C23" s="32">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="24">
@@ -3473,10 +3523,10 @@
         <v>100</v>
       </c>
       <c r="B24" s="34">
+        <v>28.0</v>
+      </c>
+      <c r="C24" s="35">
         <v>27.0</v>
-      </c>
-      <c r="C24" s="35">
-        <v>25.0</v>
       </c>
     </row>
     <row r="25">
@@ -7549,13 +7599,17 @@
       <c r="B15" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="43"/>
+      <c r="C15" s="42" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="13">
         <v>15.0</v>
       </c>
-      <c r="B16" s="41"/>
+      <c r="B16" s="41" t="s">
+        <v>62</v>
+      </c>
       <c r="C16" s="42"/>
     </row>
     <row r="17">
@@ -12800,11 +12854,11 @@
       </c>
       <c r="D15" s="49" t="str">
         <f>'THURSDAY SINGLES'!P20</f>
-        <v/>
-      </c>
-      <c r="E15" s="48" t="str">
+        <v>DAVE BARNETT</v>
+      </c>
+      <c r="E15" s="48">
         <f>'THURSDAY SINGLES'!P21</f>
-        <v/>
+        <v>40</v>
       </c>
     </row>
     <row r="16">
@@ -12813,11 +12867,11 @@
       </c>
       <c r="B16" s="48" t="str">
         <f>'SUNDAY SINGLES'!Q24</f>
-        <v/>
-      </c>
-      <c r="C16" s="48" t="str">
+        <v>ANDY THOMPSON</v>
+      </c>
+      <c r="C16" s="48">
         <f>'SUNDAY SINGLES'!Q25</f>
-        <v/>
+        <v>37</v>
       </c>
       <c r="D16" s="49" t="str">
         <f>'THURSDAY SINGLES'!Q20</f>

</xml_diff>

<commit_message>
059 Week 16/15 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="114">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -1393,7 +1393,9 @@
       <c r="Q10" s="12">
         <v>37.0</v>
       </c>
-      <c r="R10" s="14"/>
+      <c r="R10" s="13">
+        <v>39.0</v>
+      </c>
       <c r="S10" s="15"/>
       <c r="T10" s="14"/>
       <c r="U10" s="15"/>
@@ -1404,7 +1406,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>357</v>
+        <v>396</v>
       </c>
     </row>
     <row r="11">
@@ -2118,7 +2120,9 @@
       <c r="Q24" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="R24" s="21"/>
+      <c r="R24" s="21" t="s">
+        <v>56</v>
+      </c>
       <c r="S24" s="21"/>
       <c r="T24" s="21"/>
       <c r="U24" s="21"/>
@@ -2178,7 +2182,9 @@
       <c r="Q25" s="24">
         <v>37.0</v>
       </c>
-      <c r="R25" s="24"/>
+      <c r="R25" s="24">
+        <v>39.0</v>
+      </c>
       <c r="S25" s="24"/>
       <c r="T25" s="24"/>
       <c r="U25" s="24"/>
@@ -2461,7 +2467,9 @@
       </c>
       <c r="O6" s="15"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="15"/>
+      <c r="Q6" s="12">
+        <v>35.0</v>
+      </c>
       <c r="R6" s="14"/>
       <c r="S6" s="15"/>
       <c r="T6" s="14"/>
@@ -2473,7 +2481,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>324</v>
+        <v>359</v>
       </c>
     </row>
     <row r="7">
@@ -2573,7 +2581,9 @@
       <c r="P8" s="13">
         <v>39.0</v>
       </c>
-      <c r="Q8" s="15"/>
+      <c r="Q8" s="12">
+        <v>35.0</v>
+      </c>
       <c r="R8" s="14"/>
       <c r="S8" s="15"/>
       <c r="T8" s="14"/>
@@ -2585,7 +2595,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>397</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9">
@@ -2628,7 +2638,9 @@
       <c r="P9" s="13">
         <v>30.0</v>
       </c>
-      <c r="Q9" s="15"/>
+      <c r="Q9" s="12">
+        <v>29.0</v>
+      </c>
       <c r="R9" s="14"/>
       <c r="S9" s="15"/>
       <c r="T9" s="14"/>
@@ -2640,7 +2652,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>339</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10">
@@ -2681,7 +2693,9 @@
       <c r="P10" s="13">
         <v>30.0</v>
       </c>
-      <c r="Q10" s="15"/>
+      <c r="Q10" s="12">
+        <v>35.0</v>
+      </c>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
       <c r="T10" s="14"/>
@@ -2693,7 +2707,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>338</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11">
@@ -2783,7 +2797,9 @@
       <c r="P12" s="13">
         <v>40.0</v>
       </c>
-      <c r="Q12" s="15"/>
+      <c r="Q12" s="12">
+        <v>39.0</v>
+      </c>
       <c r="R12" s="14"/>
       <c r="S12" s="15"/>
       <c r="T12" s="14"/>
@@ -2795,7 +2811,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>370</v>
+        <v>409</v>
       </c>
     </row>
     <row r="13">
@@ -2830,7 +2846,9 @@
       <c r="P13" s="13">
         <v>34.0</v>
       </c>
-      <c r="Q13" s="15"/>
+      <c r="Q13" s="12">
+        <v>28.0</v>
+      </c>
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
       <c r="T13" s="14"/>
@@ -2842,7 +2860,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>230</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14">
@@ -2879,7 +2897,9 @@
       <c r="P14" s="13">
         <v>34.0</v>
       </c>
-      <c r="Q14" s="15"/>
+      <c r="Q14" s="12">
+        <v>30.0</v>
+      </c>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
       <c r="T14" s="14"/>
@@ -2891,7 +2911,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15">
@@ -2934,7 +2954,9 @@
       <c r="P15" s="13">
         <v>38.0</v>
       </c>
-      <c r="Q15" s="15"/>
+      <c r="Q15" s="12">
+        <v>28.0</v>
+      </c>
       <c r="R15" s="14"/>
       <c r="S15" s="15"/>
       <c r="T15" s="14"/>
@@ -2946,7 +2968,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>342</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16">
@@ -3089,7 +3111,9 @@
         <v>29.0</v>
       </c>
       <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
+      <c r="Q18" s="12">
+        <v>23.0</v>
+      </c>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
       <c r="T18" s="15"/>
@@ -3101,7 +3125,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>263</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -3176,7 +3200,9 @@
       <c r="P20" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="Q20" s="21"/>
+      <c r="Q20" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="R20" s="21"/>
       <c r="S20" s="21"/>
       <c r="T20" s="21"/>
@@ -3234,7 +3260,9 @@
       <c r="P21" s="24">
         <v>40.0</v>
       </c>
-      <c r="Q21" s="24"/>
+      <c r="Q21" s="24">
+        <v>39.0</v>
+      </c>
       <c r="R21" s="24"/>
       <c r="S21" s="24"/>
       <c r="T21" s="24"/>
@@ -3303,7 +3331,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="31">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="C4" s="32">
         <v>21.0</v>
@@ -3317,7 +3345,7 @@
         <v>14.0</v>
       </c>
       <c r="C5" s="32">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="6">
@@ -3391,10 +3419,10 @@
         <v>61</v>
       </c>
       <c r="B12" s="31">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="C12" s="32">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="13">
@@ -7610,13 +7638,17 @@
       <c r="B16" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="42" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="13">
         <v>16.0</v>
       </c>
-      <c r="B17" s="41"/>
+      <c r="B17" s="41" t="s">
+        <v>109</v>
+      </c>
       <c r="C17" s="42"/>
     </row>
     <row r="18">
@@ -12875,11 +12907,11 @@
       </c>
       <c r="D16" s="49" t="str">
         <f>'THURSDAY SINGLES'!Q20</f>
-        <v/>
-      </c>
-      <c r="E16" s="48" t="str">
+        <v>DAVE BARNETT</v>
+      </c>
+      <c r="E16" s="48">
         <f>'THURSDAY SINGLES'!Q21</f>
-        <v/>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
@@ -12888,11 +12920,11 @@
       </c>
       <c r="B17" s="48" t="str">
         <f>'SUNDAY SINGLES'!R24</f>
-        <v/>
-      </c>
-      <c r="C17" s="48" t="str">
+        <v>TONI SHIRLEY</v>
+      </c>
+      <c r="C17" s="48">
         <f>'SUNDAY SINGLES'!R25</f>
-        <v/>
+        <v>39</v>
       </c>
       <c r="D17" s="49" t="str">
         <f>'THURSDAY SINGLES'!R20</f>

</xml_diff>

<commit_message>
060 Week 16/16 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="114">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -2415,7 +2415,9 @@
         <v>37.0</v>
       </c>
       <c r="Q5" s="15"/>
-      <c r="R5" s="14"/>
+      <c r="R5" s="13">
+        <v>32.0</v>
+      </c>
       <c r="S5" s="15"/>
       <c r="T5" s="14"/>
       <c r="U5" s="15"/>
@@ -2426,7 +2428,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>290</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6">
@@ -2470,7 +2472,9 @@
       <c r="Q6" s="12">
         <v>35.0</v>
       </c>
-      <c r="R6" s="14"/>
+      <c r="R6" s="13">
+        <v>31.0</v>
+      </c>
       <c r="S6" s="15"/>
       <c r="T6" s="14"/>
       <c r="U6" s="15"/>
@@ -2481,7 +2485,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>359</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7">
@@ -2525,7 +2529,9 @@
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="15"/>
-      <c r="R7" s="14"/>
+      <c r="R7" s="13">
+        <v>35.0</v>
+      </c>
       <c r="S7" s="15"/>
       <c r="T7" s="14"/>
       <c r="U7" s="15"/>
@@ -2536,7 +2542,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>354</v>
+        <v>389</v>
       </c>
     </row>
     <row r="8">
@@ -2584,7 +2590,9 @@
       <c r="Q8" s="12">
         <v>35.0</v>
       </c>
-      <c r="R8" s="14"/>
+      <c r="R8" s="13">
+        <v>29.0</v>
+      </c>
       <c r="S8" s="15"/>
       <c r="T8" s="14"/>
       <c r="U8" s="15"/>
@@ -2595,7 +2603,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>432</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9">
@@ -2641,7 +2649,9 @@
       <c r="Q9" s="12">
         <v>29.0</v>
       </c>
-      <c r="R9" s="14"/>
+      <c r="R9" s="13">
+        <v>27.0</v>
+      </c>
       <c r="S9" s="15"/>
       <c r="T9" s="14"/>
       <c r="U9" s="15"/>
@@ -2652,7 +2662,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>368</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10">
@@ -2741,7 +2751,9 @@
       <c r="O11" s="15"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="15"/>
-      <c r="R11" s="14"/>
+      <c r="R11" s="13">
+        <v>27.0</v>
+      </c>
       <c r="S11" s="15"/>
       <c r="T11" s="14"/>
       <c r="U11" s="15"/>
@@ -2752,7 +2764,7 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>163</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12">
@@ -2800,7 +2812,9 @@
       <c r="Q12" s="12">
         <v>39.0</v>
       </c>
-      <c r="R12" s="14"/>
+      <c r="R12" s="13">
+        <v>36.0</v>
+      </c>
       <c r="S12" s="15"/>
       <c r="T12" s="14"/>
       <c r="U12" s="15"/>
@@ -2811,7 +2825,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>409</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13">
@@ -2849,7 +2863,9 @@
       <c r="Q13" s="12">
         <v>28.0</v>
       </c>
-      <c r="R13" s="14"/>
+      <c r="R13" s="13">
+        <v>39.0</v>
+      </c>
       <c r="S13" s="15"/>
       <c r="T13" s="14"/>
       <c r="U13" s="15"/>
@@ -2860,7 +2876,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>258</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14">
@@ -2900,7 +2916,9 @@
       <c r="Q14" s="12">
         <v>30.0</v>
       </c>
-      <c r="R14" s="14"/>
+      <c r="R14" s="13">
+        <v>31.0</v>
+      </c>
       <c r="S14" s="15"/>
       <c r="T14" s="14"/>
       <c r="U14" s="15"/>
@@ -2911,7 +2929,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>270</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15">
@@ -2957,7 +2975,9 @@
       <c r="Q15" s="12">
         <v>28.0</v>
       </c>
-      <c r="R15" s="14"/>
+      <c r="R15" s="13">
+        <v>24.0</v>
+      </c>
       <c r="S15" s="15"/>
       <c r="T15" s="14"/>
       <c r="U15" s="15"/>
@@ -2968,7 +2988,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>370</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16">
@@ -3061,7 +3081,9 @@
         <v>33.0</v>
       </c>
       <c r="Q17" s="15"/>
-      <c r="R17" s="14"/>
+      <c r="R17" s="13">
+        <v>30.0</v>
+      </c>
       <c r="S17" s="15"/>
       <c r="T17" s="14"/>
       <c r="U17" s="15"/>
@@ -3072,7 +3094,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>302</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18">
@@ -3203,7 +3225,9 @@
       <c r="Q20" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="R20" s="21"/>
+      <c r="R20" s="21" t="s">
+        <v>99</v>
+      </c>
       <c r="S20" s="21"/>
       <c r="T20" s="21"/>
       <c r="U20" s="21"/>
@@ -3263,7 +3287,9 @@
       <c r="Q21" s="24">
         <v>39.0</v>
       </c>
-      <c r="R21" s="24"/>
+      <c r="R21" s="24">
+        <v>39.0</v>
+      </c>
       <c r="S21" s="24"/>
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
@@ -3312,7 +3338,7 @@
         <v>15.0</v>
       </c>
       <c r="C2" s="32">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="3">
@@ -3375,10 +3401,10 @@
         <v>57</v>
       </c>
       <c r="B8" s="31">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="C8" s="32">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="9">
@@ -3400,7 +3426,7 @@
         <v>9.0</v>
       </c>
       <c r="C10" s="32">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="11">
@@ -3518,7 +3544,7 @@
         <v>98</v>
       </c>
       <c r="B21" s="31">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="C21" s="32">
         <v>15.0</v>
@@ -3529,7 +3555,7 @@
         <v>99</v>
       </c>
       <c r="B22" s="31">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C22" s="32">
         <v>13.0</v>
@@ -3540,10 +3566,10 @@
         <v>97</v>
       </c>
       <c r="B23" s="31">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="C23" s="32">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="24">
@@ -7649,7 +7675,9 @@
       <c r="B17" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="42"/>
+      <c r="C17" s="42" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="13">
@@ -12928,11 +12956,11 @@
       </c>
       <c r="D17" s="49" t="str">
         <f>'THURSDAY SINGLES'!R20</f>
-        <v/>
-      </c>
-      <c r="E17" s="48" t="str">
+        <v>MARTIN BROCK</v>
+      </c>
+      <c r="E17" s="48">
         <f>'THURSDAY SINGLES'!R21</f>
-        <v/>
+        <v>39</v>
       </c>
     </row>
     <row r="18">

</xml_diff>

<commit_message>
061 Week 17/17 update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="114">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -654,10 +654,10 @@
     <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1112,8 +1112,10 @@
       <c r="Q5" s="12">
         <v>36.0</v>
       </c>
-      <c r="R5" s="14"/>
-      <c r="S5" s="15"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="12">
+        <v>29.0</v>
+      </c>
       <c r="T5" s="14"/>
       <c r="U5" s="15"/>
       <c r="V5" s="14"/>
@@ -1123,7 +1125,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>314</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6">
@@ -1169,8 +1171,10 @@
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="15"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="15"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="12">
+        <v>31.0</v>
+      </c>
       <c r="T6" s="14"/>
       <c r="U6" s="15"/>
       <c r="V6" s="14"/>
@@ -1180,7 +1184,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>375</v>
+        <v>406</v>
       </c>
     </row>
     <row r="7">
@@ -1228,8 +1232,10 @@
       <c r="Q7" s="12">
         <v>28.0</v>
       </c>
-      <c r="R7" s="14"/>
-      <c r="S7" s="15"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="12">
+        <v>33.0</v>
+      </c>
       <c r="T7" s="14"/>
       <c r="U7" s="15"/>
       <c r="V7" s="14"/>
@@ -1239,7 +1245,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>358</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8">
@@ -1289,8 +1295,10 @@
       <c r="Q8" s="12">
         <v>33.0</v>
       </c>
-      <c r="R8" s="14"/>
-      <c r="S8" s="15"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="12">
+        <v>35.0</v>
+      </c>
       <c r="T8" s="14"/>
       <c r="U8" s="15"/>
       <c r="V8" s="14"/>
@@ -1300,7 +1308,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>453</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9">
@@ -1496,7 +1504,9 @@
       </c>
       <c r="Q12" s="15"/>
       <c r="R12" s="14"/>
-      <c r="S12" s="15"/>
+      <c r="S12" s="12">
+        <v>33.0</v>
+      </c>
       <c r="T12" s="14"/>
       <c r="U12" s="15"/>
       <c r="V12" s="14"/>
@@ -1506,7 +1516,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>387</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13">
@@ -1643,7 +1653,9 @@
         <v>36.0</v>
       </c>
       <c r="R15" s="14"/>
-      <c r="S15" s="15"/>
+      <c r="S15" s="12">
+        <v>39.0</v>
+      </c>
       <c r="T15" s="14"/>
       <c r="U15" s="15"/>
       <c r="V15" s="14"/>
@@ -1653,7 +1665,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16">
@@ -1696,7 +1708,9 @@
         <v>28.0</v>
       </c>
       <c r="R16" s="14"/>
-      <c r="S16" s="15"/>
+      <c r="S16" s="12">
+        <v>32.0</v>
+      </c>
       <c r="T16" s="14"/>
       <c r="U16" s="15"/>
       <c r="V16" s="14"/>
@@ -1706,7 +1720,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>285</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17">
@@ -1757,7 +1771,9 @@
         <v>29.0</v>
       </c>
       <c r="R17" s="14"/>
-      <c r="S17" s="15"/>
+      <c r="S17" s="12">
+        <v>34.0</v>
+      </c>
       <c r="T17" s="14"/>
       <c r="U17" s="15"/>
       <c r="V17" s="14"/>
@@ -1767,7 +1783,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>452</v>
+        <v>486</v>
       </c>
     </row>
     <row r="18">
@@ -1867,7 +1883,9 @@
       <c r="P19" s="14"/>
       <c r="Q19" s="15"/>
       <c r="R19" s="14"/>
-      <c r="S19" s="15"/>
+      <c r="S19" s="12">
+        <v>33.0</v>
+      </c>
       <c r="T19" s="14"/>
       <c r="U19" s="15"/>
       <c r="V19" s="14"/>
@@ -1877,7 +1895,7 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20">
@@ -1922,7 +1940,9 @@
         <v>32.0</v>
       </c>
       <c r="R20" s="14"/>
-      <c r="S20" s="15"/>
+      <c r="S20" s="12">
+        <v>35.0</v>
+      </c>
       <c r="T20" s="14"/>
       <c r="U20" s="15"/>
       <c r="V20" s="14"/>
@@ -1932,7 +1952,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>381</v>
+        <v>416</v>
       </c>
     </row>
     <row r="21">
@@ -2123,7 +2143,9 @@
       <c r="R24" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="S24" s="21"/>
+      <c r="S24" s="21" t="s">
+        <v>61</v>
+      </c>
       <c r="T24" s="21"/>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
@@ -2185,7 +2207,9 @@
       <c r="R25" s="24">
         <v>39.0</v>
       </c>
-      <c r="S25" s="24"/>
+      <c r="S25" s="24">
+        <v>39.0</v>
+      </c>
       <c r="T25" s="24"/>
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
@@ -2418,7 +2442,9 @@
       <c r="R5" s="13">
         <v>32.0</v>
       </c>
-      <c r="S5" s="15"/>
+      <c r="S5" s="12">
+        <v>26.0</v>
+      </c>
       <c r="T5" s="14"/>
       <c r="U5" s="15"/>
       <c r="V5" s="14"/>
@@ -2428,7 +2454,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>322</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6">
@@ -2475,7 +2501,9 @@
       <c r="R6" s="13">
         <v>31.0</v>
       </c>
-      <c r="S6" s="15"/>
+      <c r="S6" s="12">
+        <v>35.0</v>
+      </c>
       <c r="T6" s="14"/>
       <c r="U6" s="15"/>
       <c r="V6" s="14"/>
@@ -2485,7 +2513,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>390</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7">
@@ -2532,7 +2560,9 @@
       <c r="R7" s="13">
         <v>35.0</v>
       </c>
-      <c r="S7" s="15"/>
+      <c r="S7" s="12">
+        <v>40.0</v>
+      </c>
       <c r="T7" s="14"/>
       <c r="U7" s="15"/>
       <c r="V7" s="14"/>
@@ -2542,7 +2572,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>389</v>
+        <v>429</v>
       </c>
     </row>
     <row r="8">
@@ -2593,7 +2623,9 @@
       <c r="R8" s="13">
         <v>29.0</v>
       </c>
-      <c r="S8" s="15"/>
+      <c r="S8" s="12">
+        <v>33.0</v>
+      </c>
       <c r="T8" s="14"/>
       <c r="U8" s="15"/>
       <c r="V8" s="14"/>
@@ -2603,7 +2635,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>461</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9">
@@ -2652,7 +2684,9 @@
       <c r="R9" s="13">
         <v>27.0</v>
       </c>
-      <c r="S9" s="15"/>
+      <c r="S9" s="12">
+        <v>30.0</v>
+      </c>
       <c r="T9" s="14"/>
       <c r="U9" s="15"/>
       <c r="V9" s="14"/>
@@ -2662,7 +2696,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>395</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10">
@@ -2754,7 +2788,9 @@
       <c r="R11" s="13">
         <v>27.0</v>
       </c>
-      <c r="S11" s="15"/>
+      <c r="S11" s="12">
+        <v>34.0</v>
+      </c>
       <c r="T11" s="14"/>
       <c r="U11" s="15"/>
       <c r="V11" s="14"/>
@@ -2764,7 +2800,7 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>190</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12">
@@ -2815,7 +2851,9 @@
       <c r="R12" s="13">
         <v>36.0</v>
       </c>
-      <c r="S12" s="15"/>
+      <c r="S12" s="12">
+        <v>32.0</v>
+      </c>
       <c r="T12" s="14"/>
       <c r="U12" s="15"/>
       <c r="V12" s="14"/>
@@ -2825,7 +2863,7 @@
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>445</v>
+        <v>477</v>
       </c>
     </row>
     <row r="13">
@@ -2919,7 +2957,9 @@
       <c r="R14" s="13">
         <v>31.0</v>
       </c>
-      <c r="S14" s="15"/>
+      <c r="S14" s="12">
+        <v>40.0</v>
+      </c>
       <c r="T14" s="14"/>
       <c r="U14" s="15"/>
       <c r="V14" s="14"/>
@@ -2929,7 +2969,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>301</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15">
@@ -2978,7 +3018,9 @@
       <c r="R15" s="13">
         <v>24.0</v>
       </c>
-      <c r="S15" s="15"/>
+      <c r="S15" s="12">
+        <v>35.0</v>
+      </c>
       <c r="T15" s="14"/>
       <c r="U15" s="15"/>
       <c r="V15" s="14"/>
@@ -2988,7 +3030,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>394</v>
+        <v>429</v>
       </c>
     </row>
     <row r="16">
@@ -3031,7 +3073,9 @@
       </c>
       <c r="Q16" s="15"/>
       <c r="R16" s="14"/>
-      <c r="S16" s="15"/>
+      <c r="S16" s="12">
+        <v>29.0</v>
+      </c>
       <c r="T16" s="14"/>
       <c r="U16" s="15"/>
       <c r="V16" s="14"/>
@@ -3041,7 +3085,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>294</v>
+        <v>323</v>
       </c>
     </row>
     <row r="17">
@@ -3228,7 +3272,9 @@
       <c r="R20" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="S20" s="21"/>
+      <c r="S20" s="21" t="s">
+        <v>57</v>
+      </c>
       <c r="T20" s="21"/>
       <c r="U20" s="21"/>
       <c r="V20" s="21"/>
@@ -3290,7 +3336,9 @@
       <c r="R21" s="24">
         <v>39.0</v>
       </c>
-      <c r="S21" s="24"/>
+      <c r="S21" s="24">
+        <v>40.0</v>
+      </c>
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
@@ -3335,10 +3383,10 @@
         <v>51</v>
       </c>
       <c r="B2" s="31">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C2" s="32">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="3">
@@ -3368,10 +3416,10 @@
         <v>54</v>
       </c>
       <c r="B5" s="31">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="C5" s="32">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="6">
@@ -3423,10 +3471,10 @@
         <v>59</v>
       </c>
       <c r="B10" s="31">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="C10" s="32">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="11">
@@ -3434,10 +3482,10 @@
         <v>60</v>
       </c>
       <c r="B11" s="31">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="C11" s="32">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="12">
@@ -3456,10 +3504,10 @@
         <v>62</v>
       </c>
       <c r="B13" s="31">
+        <v>22.0</v>
+      </c>
+      <c r="C13" s="32">
         <v>21.0</v>
-      </c>
-      <c r="C13" s="32">
-        <v>19.0</v>
       </c>
     </row>
     <row r="14">
@@ -3467,7 +3515,7 @@
         <v>63</v>
       </c>
       <c r="B14" s="31">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C14" s="32">
         <v>13.0</v>
@@ -3555,7 +3603,7 @@
         <v>99</v>
       </c>
       <c r="B22" s="31">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="C22" s="32">
         <v>13.0</v>
@@ -3566,10 +3614,10 @@
         <v>97</v>
       </c>
       <c r="B23" s="31">
-        <v>32.0</v>
+        <v>29.0</v>
       </c>
       <c r="C23" s="32">
-        <v>30.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="24">
@@ -3577,7 +3625,7 @@
         <v>100</v>
       </c>
       <c r="B24" s="34">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="C24" s="35">
         <v>27.0</v>
@@ -7683,15 +7731,19 @@
       <c r="A18" s="13">
         <v>17.0</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="43"/>
+      <c r="B18" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="13">
         <v>18.0</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="43"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
     </row>
     <row r="20">
       <c r="A20" s="13">
@@ -7704,28 +7756,28 @@
       <c r="A21" s="13">
         <v>20.0</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
     </row>
     <row r="22">
       <c r="A22" s="13">
         <v>21.0</v>
       </c>
-      <c r="B22" s="44"/>
+      <c r="B22" s="43"/>
       <c r="C22" s="42"/>
     </row>
     <row r="23">
       <c r="A23" s="13">
         <v>22.0</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
     </row>
     <row r="24">
       <c r="A24" s="13">
         <v>23.0</v>
       </c>
-      <c r="B24" s="44"/>
+      <c r="B24" s="43"/>
       <c r="C24" s="42"/>
     </row>
     <row r="25">
@@ -12969,19 +13021,19 @@
       </c>
       <c r="B18" s="48" t="str">
         <f>'SUNDAY SINGLES'!S24</f>
-        <v/>
-      </c>
-      <c r="C18" s="48" t="str">
+        <v>ADY STEANE</v>
+      </c>
+      <c r="C18" s="48">
         <f>'SUNDAY SINGLES'!S25</f>
-        <v/>
+        <v>39</v>
       </c>
       <c r="D18" s="49" t="str">
         <f>'THURSDAY SINGLES'!S20</f>
-        <v/>
-      </c>
-      <c r="E18" s="48" t="str">
+        <v>ALBIE GILLESPIE</v>
+      </c>
+      <c r="E18" s="48">
         <f>'THURSDAY SINGLES'!S21</f>
-        <v/>
+        <v>40</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
062 Week 18/18 update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="116">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -230,6 +230,9 @@
     <t>FRED HOLINGWORTH</t>
   </si>
   <si>
+    <t>HELEN RIGG</t>
+  </si>
+  <si>
     <t>WINNERS SCORE</t>
   </si>
   <si>
@@ -345,6 +348,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>ARTHUR YOUNG</t>
   </si>
   <si>
     <t>SUNDAY</t>
@@ -1116,7 +1122,9 @@
       <c r="S5" s="12">
         <v>29.0</v>
       </c>
-      <c r="T5" s="14"/>
+      <c r="T5" s="13">
+        <v>33.0</v>
+      </c>
       <c r="U5" s="15"/>
       <c r="V5" s="14"/>
       <c r="W5" s="15"/>
@@ -1125,7 +1133,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>343</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6">
@@ -1175,7 +1183,9 @@
       <c r="S6" s="12">
         <v>31.0</v>
       </c>
-      <c r="T6" s="14"/>
+      <c r="T6" s="13">
+        <v>35.0</v>
+      </c>
       <c r="U6" s="15"/>
       <c r="V6" s="14"/>
       <c r="W6" s="15"/>
@@ -1184,7 +1194,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>406</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7">
@@ -1236,7 +1246,9 @@
       <c r="S7" s="12">
         <v>33.0</v>
       </c>
-      <c r="T7" s="14"/>
+      <c r="T7" s="13">
+        <v>36.0</v>
+      </c>
       <c r="U7" s="15"/>
       <c r="V7" s="14"/>
       <c r="W7" s="15"/>
@@ -1245,7 +1257,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>391</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8">
@@ -1405,7 +1417,9 @@
         <v>39.0</v>
       </c>
       <c r="S10" s="15"/>
-      <c r="T10" s="14"/>
+      <c r="T10" s="13">
+        <v>33.0</v>
+      </c>
       <c r="U10" s="15"/>
       <c r="V10" s="14"/>
       <c r="W10" s="15"/>
@@ -1414,7 +1428,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>396</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11">
@@ -1558,7 +1572,9 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
-      <c r="T13" s="14"/>
+      <c r="T13" s="13">
+        <v>30.0</v>
+      </c>
       <c r="U13" s="15"/>
       <c r="V13" s="14"/>
       <c r="W13" s="15"/>
@@ -1567,7 +1583,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>270</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14">
@@ -1774,7 +1790,9 @@
       <c r="S17" s="12">
         <v>34.0</v>
       </c>
-      <c r="T17" s="14"/>
+      <c r="T17" s="13">
+        <v>35.0</v>
+      </c>
       <c r="U17" s="15"/>
       <c r="V17" s="14"/>
       <c r="W17" s="15"/>
@@ -1783,7 +1801,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>486</v>
+        <v>521</v>
       </c>
     </row>
     <row r="18">
@@ -1835,7 +1853,9 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
-      <c r="T18" s="14"/>
+      <c r="T18" s="13">
+        <v>31.0</v>
+      </c>
       <c r="U18" s="15"/>
       <c r="V18" s="14"/>
       <c r="W18" s="15"/>
@@ -1844,7 +1864,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>443</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19">
@@ -1943,7 +1963,9 @@
       <c r="S20" s="12">
         <v>35.0</v>
       </c>
-      <c r="T20" s="14"/>
+      <c r="T20" s="13">
+        <v>33.0</v>
+      </c>
       <c r="U20" s="15"/>
       <c r="V20" s="14"/>
       <c r="W20" s="15"/>
@@ -1952,7 +1974,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>416</v>
+        <v>449</v>
       </c>
     </row>
     <row r="21">
@@ -1994,7 +2016,9 @@
       </c>
       <c r="R21" s="14"/>
       <c r="S21" s="15"/>
-      <c r="T21" s="14"/>
+      <c r="T21" s="13">
+        <v>37.0</v>
+      </c>
       <c r="U21" s="15"/>
       <c r="V21" s="14"/>
       <c r="W21" s="15"/>
@@ -2003,7 +2027,7 @@
       <c r="Z21" s="16"/>
       <c r="AA21" s="14">
         <f t="shared" si="1"/>
-        <v>279</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22">
@@ -2053,7 +2077,9 @@
       </c>
       <c r="R22" s="14"/>
       <c r="S22" s="15"/>
-      <c r="T22" s="14"/>
+      <c r="T22" s="13">
+        <v>28.0</v>
+      </c>
       <c r="U22" s="15"/>
       <c r="V22" s="14"/>
       <c r="W22" s="15"/>
@@ -2062,7 +2088,7 @@
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>416</v>
+        <v>444</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2146,7 +2172,9 @@
       <c r="S24" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="T24" s="21"/>
+      <c r="T24" s="21" t="s">
+        <v>71</v>
+      </c>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
@@ -2157,7 +2185,7 @@
     </row>
     <row r="25">
       <c r="B25" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="24">
         <v>35.0</v>
@@ -2210,7 +2238,9 @@
       <c r="S25" s="24">
         <v>39.0</v>
       </c>
-      <c r="T25" s="24"/>
+      <c r="T25" s="24">
+        <v>44.0</v>
+      </c>
       <c r="U25" s="24"/>
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
@@ -2242,83 +2272,83 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AA3" s="6"/>
     </row>
@@ -2445,7 +2475,9 @@
       <c r="S5" s="12">
         <v>26.0</v>
       </c>
-      <c r="T5" s="14"/>
+      <c r="T5" s="13">
+        <v>29.0</v>
+      </c>
       <c r="U5" s="15"/>
       <c r="V5" s="14"/>
       <c r="W5" s="15"/>
@@ -2454,7 +2486,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>348</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6">
@@ -2504,7 +2536,9 @@
       <c r="S6" s="12">
         <v>35.0</v>
       </c>
-      <c r="T6" s="14"/>
+      <c r="T6" s="13">
+        <v>28.0</v>
+      </c>
       <c r="U6" s="15"/>
       <c r="V6" s="14"/>
       <c r="W6" s="15"/>
@@ -2513,7 +2547,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>425</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7">
@@ -2563,7 +2597,9 @@
       <c r="S7" s="12">
         <v>40.0</v>
       </c>
-      <c r="T7" s="14"/>
+      <c r="T7" s="13">
+        <v>35.0</v>
+      </c>
       <c r="U7" s="15"/>
       <c r="V7" s="14"/>
       <c r="W7" s="15"/>
@@ -2572,7 +2608,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>429</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8">
@@ -2626,7 +2662,9 @@
       <c r="S8" s="12">
         <v>33.0</v>
       </c>
-      <c r="T8" s="14"/>
+      <c r="T8" s="13">
+        <v>27.0</v>
+      </c>
       <c r="U8" s="15"/>
       <c r="V8" s="14"/>
       <c r="W8" s="15"/>
@@ -2635,7 +2673,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>494</v>
+        <v>521</v>
       </c>
     </row>
     <row r="9">
@@ -2687,7 +2725,9 @@
       <c r="S9" s="12">
         <v>30.0</v>
       </c>
-      <c r="T9" s="14"/>
+      <c r="T9" s="13">
+        <v>34.0</v>
+      </c>
       <c r="U9" s="15"/>
       <c r="V9" s="14"/>
       <c r="W9" s="15"/>
@@ -2696,7 +2736,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>425</v>
+        <v>459</v>
       </c>
     </row>
     <row r="10">
@@ -2742,7 +2782,9 @@
       </c>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
-      <c r="T10" s="14"/>
+      <c r="T10" s="13">
+        <v>38.0</v>
+      </c>
       <c r="U10" s="15"/>
       <c r="V10" s="14"/>
       <c r="W10" s="15"/>
@@ -2751,12 +2793,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>373</v>
+        <v>411</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C11" s="12">
         <v>22.0</v>
@@ -2791,7 +2833,9 @@
       <c r="S11" s="12">
         <v>34.0</v>
       </c>
-      <c r="T11" s="14"/>
+      <c r="T11" s="13">
+        <v>28.0</v>
+      </c>
       <c r="U11" s="15"/>
       <c r="V11" s="14"/>
       <c r="W11" s="15"/>
@@ -2800,12 +2844,12 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>224</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C12" s="12">
         <v>28.0</v>
@@ -2868,7 +2912,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" s="12">
         <v>31.0</v>
@@ -2905,7 +2949,9 @@
         <v>39.0</v>
       </c>
       <c r="S13" s="15"/>
-      <c r="T13" s="14"/>
+      <c r="T13" s="13">
+        <v>31.0</v>
+      </c>
       <c r="U13" s="15"/>
       <c r="V13" s="14"/>
       <c r="W13" s="15"/>
@@ -2914,7 +2960,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>297</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14">
@@ -3035,7 +3081,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C16" s="12">
         <v>32.0</v>
@@ -3076,7 +3122,9 @@
       <c r="S16" s="12">
         <v>29.0</v>
       </c>
-      <c r="T16" s="14"/>
+      <c r="T16" s="13">
+        <v>29.0</v>
+      </c>
       <c r="U16" s="15"/>
       <c r="V16" s="14"/>
       <c r="W16" s="15"/>
@@ -3085,7 +3133,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>323</v>
+        <v>352</v>
       </c>
     </row>
     <row r="17">
@@ -3129,7 +3177,9 @@
         <v>30.0</v>
       </c>
       <c r="S17" s="15"/>
-      <c r="T17" s="14"/>
+      <c r="T17" s="13">
+        <v>36.0</v>
+      </c>
       <c r="U17" s="15"/>
       <c r="V17" s="14"/>
       <c r="W17" s="15"/>
@@ -3138,12 +3188,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>332</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C18" s="12">
         <v>27.0</v>
@@ -3182,7 +3232,9 @@
       </c>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
+      <c r="T18" s="12">
+        <v>35.0</v>
+      </c>
       <c r="U18" s="15"/>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
@@ -3191,7 +3243,7 @@
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>286</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -3231,10 +3283,10 @@
         <v>56</v>
       </c>
       <c r="E20" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="21" t="s">
         <v>99</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="G20" s="21" t="s">
         <v>64</v>
@@ -3246,7 +3298,7 @@
         <v>64</v>
       </c>
       <c r="J20" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K20" s="21" t="s">
         <v>57</v>
@@ -3264,18 +3316,20 @@
         <v>51</v>
       </c>
       <c r="P20" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Q20" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R20" s="21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="S20" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="T20" s="21"/>
+      <c r="T20" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="U20" s="21"/>
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
@@ -3286,7 +3340,7 @@
     </row>
     <row r="21">
       <c r="B21" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C21" s="24">
         <v>40.0</v>
@@ -3339,7 +3393,9 @@
       <c r="S21" s="24">
         <v>40.0</v>
       </c>
-      <c r="T21" s="24"/>
+      <c r="T21" s="24">
+        <v>38.0</v>
+      </c>
       <c r="U21" s="24"/>
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
@@ -3372,10 +3428,10 @@
         <v>25</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
@@ -3578,7 +3634,7 @@
     </row>
     <row r="20">
       <c r="A20" s="33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B20" s="31">
         <v>19.0</v>
@@ -3589,7 +3645,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B21" s="31">
         <v>16.0</v>
@@ -3600,7 +3656,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B22" s="31">
         <v>15.0</v>
@@ -3611,7 +3667,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B23" s="31">
         <v>29.0</v>
@@ -3622,7 +3678,7 @@
     </row>
     <row r="24">
       <c r="A24" s="18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B24" s="34">
         <v>29.0</v>
@@ -7541,13 +7597,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
@@ -7591,7 +7647,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6">
@@ -7602,7 +7658,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
@@ -7621,7 +7677,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>67</v>
@@ -7635,7 +7691,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10">
@@ -7646,7 +7702,7 @@
         <v>63</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7655,10 +7711,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12">
@@ -7669,7 +7725,7 @@
         <v>66</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13">
@@ -7680,7 +7736,7 @@
         <v>62</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14">
@@ -7699,7 +7755,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>57</v>
@@ -7721,7 +7777,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>59</v>
@@ -7742,8 +7798,12 @@
       <c r="A19" s="13">
         <v>18.0</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="44"/>
+      <c r="B19" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="13">
@@ -12664,19 +12724,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -13042,19 +13102,19 @@
       </c>
       <c r="B19" s="48" t="str">
         <f>'SUNDAY SINGLES'!T24</f>
-        <v/>
-      </c>
-      <c r="C19" s="48" t="str">
+        <v>HELEN RIGG</v>
+      </c>
+      <c r="C19" s="48">
         <f>'SUNDAY SINGLES'!T25</f>
-        <v/>
+        <v>44</v>
       </c>
       <c r="D19" s="49" t="str">
         <f>'THURSDAY SINGLES'!T20</f>
-        <v/>
-      </c>
-      <c r="E19" s="48" t="str">
+        <v>KEN PEEL</v>
+      </c>
+      <c r="E19" s="48">
         <f>'THURSDAY SINGLES'!T21</f>
-        <v/>
+        <v>38</v>
       </c>
     </row>
     <row r="20">

</xml_diff>

<commit_message>
063 Week 19/19 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="116">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -1186,7 +1186,9 @@
       <c r="T6" s="13">
         <v>35.0</v>
       </c>
-      <c r="U6" s="15"/>
+      <c r="U6" s="12">
+        <v>37.0</v>
+      </c>
       <c r="V6" s="14"/>
       <c r="W6" s="15"/>
       <c r="X6" s="14"/>
@@ -1194,7 +1196,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>441</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7">
@@ -1312,7 +1314,9 @@
         <v>35.0</v>
       </c>
       <c r="T8" s="14"/>
-      <c r="U8" s="15"/>
+      <c r="U8" s="12">
+        <v>39.0</v>
+      </c>
       <c r="V8" s="14"/>
       <c r="W8" s="15"/>
       <c r="X8" s="14"/>
@@ -1320,7 +1324,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>488</v>
+        <v>527</v>
       </c>
     </row>
     <row r="9">
@@ -1363,7 +1367,9 @@
       <c r="R9" s="14"/>
       <c r="S9" s="15"/>
       <c r="T9" s="14"/>
-      <c r="U9" s="15"/>
+      <c r="U9" s="12">
+        <v>34.0</v>
+      </c>
       <c r="V9" s="14"/>
       <c r="W9" s="15"/>
       <c r="X9" s="14"/>
@@ -1371,7 +1377,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>260</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10">
@@ -1420,7 +1426,9 @@
       <c r="T10" s="13">
         <v>33.0</v>
       </c>
-      <c r="U10" s="15"/>
+      <c r="U10" s="12">
+        <v>40.0</v>
+      </c>
       <c r="V10" s="14"/>
       <c r="W10" s="15"/>
       <c r="X10" s="14"/>
@@ -1428,7 +1436,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>429</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11">
@@ -1575,7 +1583,9 @@
       <c r="T13" s="13">
         <v>30.0</v>
       </c>
-      <c r="U13" s="15"/>
+      <c r="U13" s="12">
+        <v>40.0</v>
+      </c>
       <c r="V13" s="14"/>
       <c r="W13" s="15"/>
       <c r="X13" s="14"/>
@@ -1583,7 +1593,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14">
@@ -1628,7 +1638,9 @@
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
       <c r="T14" s="14"/>
-      <c r="U14" s="15"/>
+      <c r="U14" s="12">
+        <v>34.0</v>
+      </c>
       <c r="V14" s="14"/>
       <c r="W14" s="15"/>
       <c r="X14" s="14"/>
@@ -1636,7 +1648,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>320</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15">
@@ -1728,7 +1740,9 @@
         <v>32.0</v>
       </c>
       <c r="T16" s="14"/>
-      <c r="U16" s="15"/>
+      <c r="U16" s="12">
+        <v>36.0</v>
+      </c>
       <c r="V16" s="14"/>
       <c r="W16" s="15"/>
       <c r="X16" s="14"/>
@@ -1736,7 +1750,7 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>317</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17">
@@ -1793,7 +1807,9 @@
       <c r="T17" s="13">
         <v>35.0</v>
       </c>
-      <c r="U17" s="15"/>
+      <c r="U17" s="12">
+        <v>34.0</v>
+      </c>
       <c r="V17" s="14"/>
       <c r="W17" s="15"/>
       <c r="X17" s="14"/>
@@ -1801,7 +1817,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>521</v>
+        <v>555</v>
       </c>
     </row>
     <row r="18">
@@ -1856,7 +1872,9 @@
       <c r="T18" s="13">
         <v>31.0</v>
       </c>
-      <c r="U18" s="15"/>
+      <c r="U18" s="12">
+        <v>36.0</v>
+      </c>
       <c r="V18" s="14"/>
       <c r="W18" s="15"/>
       <c r="X18" s="14"/>
@@ -1864,7 +1882,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>474</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19">
@@ -1907,7 +1925,9 @@
         <v>33.0</v>
       </c>
       <c r="T19" s="14"/>
-      <c r="U19" s="15"/>
+      <c r="U19" s="12">
+        <v>34.0</v>
+      </c>
       <c r="V19" s="14"/>
       <c r="W19" s="15"/>
       <c r="X19" s="14"/>
@@ -1915,7 +1935,7 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>273</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20">
@@ -2175,7 +2195,9 @@
       <c r="T24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="U24" s="21"/>
+      <c r="U24" s="21" t="s">
+        <v>71</v>
+      </c>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
       <c r="X24" s="21"/>
@@ -2241,7 +2263,9 @@
       <c r="T25" s="24">
         <v>44.0</v>
       </c>
-      <c r="U25" s="24"/>
+      <c r="U25" s="24">
+        <v>47.0</v>
+      </c>
       <c r="V25" s="24"/>
       <c r="W25" s="24"/>
       <c r="X25" s="24"/>
@@ -2478,7 +2502,9 @@
       <c r="T5" s="13">
         <v>29.0</v>
       </c>
-      <c r="U5" s="15"/>
+      <c r="U5" s="12">
+        <v>35.0</v>
+      </c>
       <c r="V5" s="14"/>
       <c r="W5" s="15"/>
       <c r="X5" s="14"/>
@@ -2486,7 +2512,7 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>377</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6">
@@ -2539,7 +2565,9 @@
       <c r="T6" s="13">
         <v>28.0</v>
       </c>
-      <c r="U6" s="15"/>
+      <c r="U6" s="12">
+        <v>37.0</v>
+      </c>
       <c r="V6" s="14"/>
       <c r="W6" s="15"/>
       <c r="X6" s="14"/>
@@ -2547,7 +2575,7 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>453</v>
+        <v>490</v>
       </c>
     </row>
     <row r="7">
@@ -2600,7 +2628,9 @@
       <c r="T7" s="13">
         <v>35.0</v>
       </c>
-      <c r="U7" s="15"/>
+      <c r="U7" s="12">
+        <v>34.0</v>
+      </c>
       <c r="V7" s="14"/>
       <c r="W7" s="15"/>
       <c r="X7" s="14"/>
@@ -2608,7 +2638,7 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>464</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8">
@@ -2665,7 +2695,9 @@
       <c r="T8" s="13">
         <v>27.0</v>
       </c>
-      <c r="U8" s="15"/>
+      <c r="U8" s="12">
+        <v>32.0</v>
+      </c>
       <c r="V8" s="14"/>
       <c r="W8" s="15"/>
       <c r="X8" s="14"/>
@@ -2673,7 +2705,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>521</v>
+        <v>553</v>
       </c>
     </row>
     <row r="9">
@@ -2728,7 +2760,9 @@
       <c r="T9" s="13">
         <v>34.0</v>
       </c>
-      <c r="U9" s="15"/>
+      <c r="U9" s="12">
+        <v>34.0</v>
+      </c>
       <c r="V9" s="14"/>
       <c r="W9" s="15"/>
       <c r="X9" s="14"/>
@@ -2736,7 +2770,7 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>459</v>
+        <v>493</v>
       </c>
     </row>
     <row r="10">
@@ -2785,7 +2819,9 @@
       <c r="T10" s="13">
         <v>38.0</v>
       </c>
-      <c r="U10" s="15"/>
+      <c r="U10" s="12">
+        <v>33.0</v>
+      </c>
       <c r="V10" s="14"/>
       <c r="W10" s="15"/>
       <c r="X10" s="14"/>
@@ -2793,7 +2829,7 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>411</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11">
@@ -2952,7 +2988,9 @@
       <c r="T13" s="13">
         <v>31.0</v>
       </c>
-      <c r="U13" s="15"/>
+      <c r="U13" s="12">
+        <v>33.0</v>
+      </c>
       <c r="V13" s="14"/>
       <c r="W13" s="15"/>
       <c r="X13" s="14"/>
@@ -2960,7 +2998,7 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>328</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14">
@@ -3068,7 +3106,9 @@
         <v>35.0</v>
       </c>
       <c r="T15" s="14"/>
-      <c r="U15" s="15"/>
+      <c r="U15" s="12">
+        <v>27.0</v>
+      </c>
       <c r="V15" s="14"/>
       <c r="W15" s="15"/>
       <c r="X15" s="14"/>
@@ -3076,7 +3116,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>429</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16">
@@ -3180,7 +3220,9 @@
       <c r="T17" s="13">
         <v>36.0</v>
       </c>
-      <c r="U17" s="15"/>
+      <c r="U17" s="12">
+        <v>38.0</v>
+      </c>
       <c r="V17" s="14"/>
       <c r="W17" s="15"/>
       <c r="X17" s="14"/>
@@ -3188,7 +3230,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>368</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18">
@@ -3330,7 +3372,9 @@
       <c r="T20" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="U20" s="21"/>
+      <c r="U20" s="21" t="s">
+        <v>61</v>
+      </c>
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
       <c r="X20" s="21"/>
@@ -3396,7 +3440,9 @@
       <c r="T21" s="24">
         <v>38.0</v>
       </c>
-      <c r="U21" s="24"/>
+      <c r="U21" s="24">
+        <v>39.0</v>
+      </c>
       <c r="V21" s="24"/>
       <c r="W21" s="24"/>
       <c r="X21" s="24"/>
@@ -3472,10 +3518,10 @@
         <v>54</v>
       </c>
       <c r="B5" s="31">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="C5" s="32">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="6">
@@ -3494,10 +3540,10 @@
         <v>56</v>
       </c>
       <c r="B7" s="31">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="C7" s="32">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="8">
@@ -3505,10 +3551,10 @@
         <v>57</v>
       </c>
       <c r="B8" s="31">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="C8" s="32">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="9">
@@ -3516,7 +3562,7 @@
         <v>58</v>
       </c>
       <c r="B9" s="31">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="C9" s="32">
         <v>18.0</v>
@@ -3549,10 +3595,10 @@
         <v>61</v>
       </c>
       <c r="B12" s="31">
-        <v>19.0</v>
+        <v>17.0</v>
       </c>
       <c r="C12" s="32">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="13">
@@ -3563,7 +3609,7 @@
         <v>22.0</v>
       </c>
       <c r="C13" s="32">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="14">
@@ -3571,10 +3617,10 @@
         <v>63</v>
       </c>
       <c r="B14" s="31">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="C14" s="32">
-        <v>13.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="15">
@@ -3582,10 +3628,10 @@
         <v>64</v>
       </c>
       <c r="B15" s="31">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="C15" s="32">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="16">
@@ -3593,7 +3639,7 @@
         <v>65</v>
       </c>
       <c r="B16" s="31">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="C16" s="32">
         <v>12.0</v>
@@ -3640,7 +3686,7 @@
         <v>19.0</v>
       </c>
       <c r="C20" s="32">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="21">
@@ -3651,7 +3697,7 @@
         <v>16.0</v>
       </c>
       <c r="C21" s="32">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="22">
@@ -3681,10 +3727,10 @@
         <v>101</v>
       </c>
       <c r="B24" s="34">
-        <v>29.0</v>
+        <v>28.0</v>
       </c>
       <c r="C24" s="35">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="25">
@@ -7809,8 +7855,12 @@
       <c r="A20" s="13">
         <v>19.0</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
+      <c r="B20" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="13">
@@ -13123,19 +13173,19 @@
       </c>
       <c r="B20" s="48" t="str">
         <f>'SUNDAY SINGLES'!U24</f>
-        <v/>
-      </c>
-      <c r="C20" s="48" t="str">
+        <v>HELEN RIGG</v>
+      </c>
+      <c r="C20" s="48">
         <f>'SUNDAY SINGLES'!U25</f>
-        <v/>
+        <v>47</v>
       </c>
       <c r="D20" s="49" t="str">
         <f>'THURSDAY SINGLES'!U20</f>
-        <v/>
-      </c>
-      <c r="E20" s="48" t="str">
+        <v>ADY STEANE</v>
+      </c>
+      <c r="E20" s="48">
         <f>'THURSDAY SINGLES'!U21</f>
-        <v/>
+        <v>39</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
064 Week 20/20 update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="117">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>JODAN HOWARD</t>
+  </si>
+  <si>
+    <t>SIMON EDWARDS</t>
   </si>
   <si>
     <t>WHITE TEES</t>
@@ -1126,14 +1129,16 @@
         <v>33.0</v>
       </c>
       <c r="U5" s="15"/>
-      <c r="V5" s="14"/>
+      <c r="V5" s="13">
+        <v>31.0</v>
+      </c>
       <c r="W5" s="15"/>
       <c r="X5" s="14"/>
       <c r="Y5" s="15"/>
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>376</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6">
@@ -1189,14 +1194,16 @@
       <c r="U6" s="12">
         <v>37.0</v>
       </c>
-      <c r="V6" s="14"/>
+      <c r="V6" s="13">
+        <v>32.0</v>
+      </c>
       <c r="W6" s="15"/>
       <c r="X6" s="14"/>
       <c r="Y6" s="15"/>
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>478</v>
+        <v>510</v>
       </c>
     </row>
     <row r="7">
@@ -1317,14 +1324,16 @@
       <c r="U8" s="12">
         <v>39.0</v>
       </c>
-      <c r="V8" s="14"/>
+      <c r="V8" s="13">
+        <v>30.0</v>
+      </c>
       <c r="W8" s="15"/>
       <c r="X8" s="14"/>
       <c r="Y8" s="15"/>
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>527</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9">
@@ -1370,14 +1379,16 @@
       <c r="U9" s="12">
         <v>34.0</v>
       </c>
-      <c r="V9" s="14"/>
+      <c r="V9" s="13">
+        <v>29.0</v>
+      </c>
       <c r="W9" s="15"/>
       <c r="X9" s="14"/>
       <c r="Y9" s="15"/>
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>294</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10">
@@ -1429,14 +1440,16 @@
       <c r="U10" s="12">
         <v>40.0</v>
       </c>
-      <c r="V10" s="14"/>
+      <c r="V10" s="13">
+        <v>26.0</v>
+      </c>
       <c r="W10" s="15"/>
       <c r="X10" s="14"/>
       <c r="Y10" s="15"/>
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>469</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11">
@@ -1586,14 +1599,16 @@
       <c r="U13" s="12">
         <v>40.0</v>
       </c>
-      <c r="V13" s="14"/>
+      <c r="V13" s="13">
+        <v>29.0</v>
+      </c>
       <c r="W13" s="15"/>
       <c r="X13" s="14"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>340</v>
+        <v>369</v>
       </c>
     </row>
     <row r="14">
@@ -1641,14 +1656,16 @@
       <c r="U14" s="12">
         <v>34.0</v>
       </c>
-      <c r="V14" s="14"/>
+      <c r="V14" s="13">
+        <v>29.0</v>
+      </c>
       <c r="W14" s="15"/>
       <c r="X14" s="14"/>
       <c r="Y14" s="15"/>
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>354</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15">
@@ -1686,14 +1703,16 @@
       </c>
       <c r="T15" s="14"/>
       <c r="U15" s="15"/>
-      <c r="V15" s="14"/>
+      <c r="V15" s="13">
+        <v>28.0</v>
+      </c>
       <c r="W15" s="15"/>
       <c r="X15" s="14"/>
       <c r="Y15" s="15"/>
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>199</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16">
@@ -1743,14 +1762,16 @@
       <c r="U16" s="12">
         <v>36.0</v>
       </c>
-      <c r="V16" s="14"/>
+      <c r="V16" s="13">
+        <v>38.0</v>
+      </c>
       <c r="W16" s="15"/>
       <c r="X16" s="14"/>
       <c r="Y16" s="15"/>
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>353</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17">
@@ -1810,14 +1831,16 @@
       <c r="U17" s="12">
         <v>34.0</v>
       </c>
-      <c r="V17" s="14"/>
+      <c r="V17" s="13">
+        <v>33.0</v>
+      </c>
       <c r="W17" s="15"/>
       <c r="X17" s="14"/>
       <c r="Y17" s="15"/>
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>555</v>
+        <v>588</v>
       </c>
     </row>
     <row r="18">
@@ -1875,14 +1898,16 @@
       <c r="U18" s="12">
         <v>36.0</v>
       </c>
-      <c r="V18" s="14"/>
+      <c r="V18" s="13">
+        <v>25.0</v>
+      </c>
       <c r="W18" s="15"/>
       <c r="X18" s="14"/>
       <c r="Y18" s="15"/>
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>510</v>
+        <v>535</v>
       </c>
     </row>
     <row r="19">
@@ -1928,14 +1953,16 @@
       <c r="U19" s="12">
         <v>34.0</v>
       </c>
-      <c r="V19" s="14"/>
+      <c r="V19" s="13">
+        <v>34.0</v>
+      </c>
       <c r="W19" s="15"/>
       <c r="X19" s="14"/>
       <c r="Y19" s="15"/>
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>307</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20">
@@ -1987,14 +2014,16 @@
         <v>33.0</v>
       </c>
       <c r="U20" s="15"/>
-      <c r="V20" s="14"/>
+      <c r="V20" s="13">
+        <v>32.0</v>
+      </c>
       <c r="W20" s="15"/>
       <c r="X20" s="14"/>
       <c r="Y20" s="15"/>
       <c r="Z20" s="16"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>449</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21">
@@ -2101,14 +2130,16 @@
         <v>28.0</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="14"/>
+      <c r="V22" s="13">
+        <v>32.0</v>
+      </c>
       <c r="W22" s="15"/>
       <c r="X22" s="14"/>
       <c r="Y22" s="15"/>
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>444</v>
+        <v>476</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2198,7 +2229,9 @@
       <c r="U24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="V24" s="21"/>
+      <c r="V24" s="21" t="s">
+        <v>62</v>
+      </c>
       <c r="W24" s="21"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="21"/>
@@ -2266,7 +2299,9 @@
       <c r="U25" s="24">
         <v>47.0</v>
       </c>
-      <c r="V25" s="24"/>
+      <c r="V25" s="24">
+        <v>38.0</v>
+      </c>
       <c r="W25" s="24"/>
       <c r="X25" s="24"/>
       <c r="Y25" s="24"/>
@@ -2568,14 +2603,16 @@
       <c r="U6" s="12">
         <v>37.0</v>
       </c>
-      <c r="V6" s="14"/>
+      <c r="V6" s="13">
+        <v>35.0</v>
+      </c>
       <c r="W6" s="15"/>
       <c r="X6" s="14"/>
       <c r="Y6" s="15"/>
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>490</v>
+        <v>525</v>
       </c>
     </row>
     <row r="7">
@@ -2822,14 +2859,16 @@
       <c r="U10" s="12">
         <v>33.0</v>
       </c>
-      <c r="V10" s="14"/>
+      <c r="V10" s="13">
+        <v>35.0</v>
+      </c>
       <c r="W10" s="15"/>
       <c r="X10" s="14"/>
       <c r="Y10" s="15"/>
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>444</v>
+        <v>479</v>
       </c>
     </row>
     <row r="11">
@@ -2936,14 +2975,16 @@
       </c>
       <c r="T12" s="14"/>
       <c r="U12" s="15"/>
-      <c r="V12" s="14"/>
+      <c r="V12" s="13">
+        <v>37.0</v>
+      </c>
       <c r="W12" s="15"/>
       <c r="X12" s="14"/>
       <c r="Y12" s="15"/>
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>477</v>
+        <v>514</v>
       </c>
     </row>
     <row r="13">
@@ -2991,14 +3032,16 @@
       <c r="U13" s="12">
         <v>33.0</v>
       </c>
-      <c r="V13" s="14"/>
+      <c r="V13" s="13">
+        <v>38.0</v>
+      </c>
       <c r="W13" s="15"/>
       <c r="X13" s="14"/>
       <c r="Y13" s="15"/>
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>361</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14">
@@ -3046,14 +3089,16 @@
       </c>
       <c r="T14" s="14"/>
       <c r="U14" s="15"/>
-      <c r="V14" s="14"/>
+      <c r="V14" s="13">
+        <v>32.0</v>
+      </c>
       <c r="W14" s="15"/>
       <c r="X14" s="14"/>
       <c r="Y14" s="15"/>
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>341</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15">
@@ -3109,14 +3154,16 @@
       <c r="U15" s="12">
         <v>27.0</v>
       </c>
-      <c r="V15" s="14"/>
+      <c r="V15" s="13">
+        <v>34.0</v>
+      </c>
       <c r="W15" s="15"/>
       <c r="X15" s="14"/>
       <c r="Y15" s="15"/>
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>456</v>
+        <v>490</v>
       </c>
     </row>
     <row r="16">
@@ -3375,7 +3422,9 @@
       <c r="U20" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="V20" s="21"/>
+      <c r="V20" s="21" t="s">
+        <v>103</v>
+      </c>
       <c r="W20" s="21"/>
       <c r="X20" s="21"/>
       <c r="Y20" s="21"/>
@@ -3443,7 +3492,9 @@
       <c r="U21" s="24">
         <v>39.0</v>
       </c>
-      <c r="V21" s="24"/>
+      <c r="V21" s="24">
+        <v>39.0</v>
+      </c>
       <c r="W21" s="24"/>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
@@ -3474,10 +3525,10 @@
         <v>25</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2">
@@ -7643,13 +7694,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2">
@@ -7693,7 +7744,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6">
@@ -7723,7 +7774,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>67</v>
@@ -7737,7 +7788,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10">
@@ -7748,7 +7799,7 @@
         <v>63</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7757,10 +7808,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12">
@@ -7782,7 +7833,7 @@
         <v>62</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14">
@@ -7801,7 +7852,7 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>57</v>
@@ -7823,7 +7874,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>59</v>
@@ -7845,7 +7896,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C19" s="42" t="s">
         <v>51</v>
@@ -7866,8 +7917,12 @@
       <c r="A21" s="13">
         <v>20.0</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="44"/>
+      <c r="B21" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="13">
@@ -12774,19 +12829,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
@@ -13194,19 +13249,19 @@
       </c>
       <c r="B21" s="48" t="str">
         <f>'SUNDAY SINGLES'!V24</f>
-        <v/>
-      </c>
-      <c r="C21" s="48" t="str">
+        <v>STEVE FELLOWS</v>
+      </c>
+      <c r="C21" s="48">
         <f>'SUNDAY SINGLES'!V25</f>
-        <v/>
+        <v>38</v>
       </c>
       <c r="D21" s="49" t="str">
         <f>'THURSDAY SINGLES'!V20</f>
-        <v/>
-      </c>
-      <c r="E21" s="48" t="str">
+        <v>SIMON EDWARDS</v>
+      </c>
+      <c r="E21" s="48">
         <f>'THURSDAY SINGLES'!V21</f>
-        <v/>
+        <v>39</v>
       </c>
     </row>
     <row r="22">

</xml_diff>

<commit_message>
067 Week 22/22 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="117">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -1198,12 +1198,14 @@
       <c r="W6" s="12">
         <v>36.0</v>
       </c>
-      <c r="X6" s="14"/>
+      <c r="X6" s="13">
+        <v>34.0</v>
+      </c>
       <c r="Y6" s="15"/>
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>546</v>
+        <v>580</v>
       </c>
     </row>
     <row r="7">
@@ -1387,12 +1389,14 @@
       <c r="W9" s="12">
         <v>33.0</v>
       </c>
-      <c r="X9" s="14"/>
+      <c r="X9" s="13">
+        <v>33.0</v>
+      </c>
       <c r="Y9" s="15"/>
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>356</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10">
@@ -1450,12 +1454,14 @@
       <c r="W10" s="12">
         <v>32.0</v>
       </c>
-      <c r="X10" s="14"/>
+      <c r="X10" s="13">
+        <v>35.0</v>
+      </c>
       <c r="Y10" s="15"/>
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>527</v>
+        <v>562</v>
       </c>
     </row>
     <row r="11">
@@ -1493,12 +1499,14 @@
       <c r="W11" s="12">
         <v>36.0</v>
       </c>
-      <c r="X11" s="14"/>
+      <c r="X11" s="13">
+        <v>37.0</v>
+      </c>
       <c r="Y11" s="15"/>
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>171</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12">
@@ -1556,12 +1564,14 @@
       <c r="W12" s="12">
         <v>38.0</v>
       </c>
-      <c r="X12" s="14"/>
+      <c r="X12" s="13">
+        <v>35.0</v>
+      </c>
       <c r="Y12" s="15"/>
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>458</v>
+        <v>493</v>
       </c>
     </row>
     <row r="13">
@@ -1674,12 +1684,14 @@
       <c r="W14" s="12">
         <v>31.0</v>
       </c>
-      <c r="X14" s="14"/>
+      <c r="X14" s="13">
+        <v>35.0</v>
+      </c>
       <c r="Y14" s="15"/>
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>414</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15">
@@ -1723,12 +1735,14 @@
       <c r="W15" s="12">
         <v>31.0</v>
       </c>
-      <c r="X15" s="14"/>
+      <c r="X15" s="13">
+        <v>33.0</v>
+      </c>
       <c r="Y15" s="15"/>
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>258</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16">
@@ -1784,12 +1798,14 @@
       <c r="W16" s="12">
         <v>24.0</v>
       </c>
-      <c r="X16" s="14"/>
+      <c r="X16" s="13">
+        <v>29.0</v>
+      </c>
       <c r="Y16" s="15"/>
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>415</v>
+        <v>444</v>
       </c>
     </row>
     <row r="17">
@@ -1855,12 +1871,14 @@
       <c r="W17" s="12">
         <v>33.0</v>
       </c>
-      <c r="X17" s="14"/>
+      <c r="X17" s="13">
+        <v>26.0</v>
+      </c>
       <c r="Y17" s="15"/>
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>621</v>
+        <v>647</v>
       </c>
     </row>
     <row r="18">
@@ -1924,12 +1942,14 @@
       <c r="W18" s="12">
         <v>32.0</v>
       </c>
-      <c r="X18" s="14"/>
+      <c r="X18" s="13">
+        <v>22.0</v>
+      </c>
       <c r="Y18" s="15"/>
       <c r="Z18" s="16"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>567</v>
+        <v>589</v>
       </c>
     </row>
     <row r="19">
@@ -1979,12 +1999,14 @@
         <v>34.0</v>
       </c>
       <c r="W19" s="15"/>
-      <c r="X19" s="14"/>
+      <c r="X19" s="13">
+        <v>35.0</v>
+      </c>
       <c r="Y19" s="15"/>
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>341</v>
+        <v>376</v>
       </c>
     </row>
     <row r="20">
@@ -2160,12 +2182,14 @@
       <c r="W22" s="12">
         <v>37.0</v>
       </c>
-      <c r="X22" s="14"/>
+      <c r="X22" s="13">
+        <v>37.0</v>
+      </c>
       <c r="Y22" s="15"/>
       <c r="Z22" s="16"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>513</v>
+        <v>550</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2261,7 +2285,9 @@
       <c r="W24" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="X24" s="21"/>
+      <c r="X24" s="21" t="s">
+        <v>68</v>
+      </c>
       <c r="Y24" s="21"/>
       <c r="Z24" s="21"/>
       <c r="AA24" s="22"/>
@@ -2333,7 +2359,9 @@
       <c r="W25" s="24">
         <v>38.0</v>
       </c>
-      <c r="X25" s="24"/>
+      <c r="X25" s="24">
+        <v>37.0</v>
+      </c>
       <c r="Y25" s="24"/>
       <c r="Z25" s="24"/>
       <c r="AA25" s="14"/>
@@ -8009,7 +8037,9 @@
       <c r="A23" s="13">
         <v>22.0</v>
       </c>
-      <c r="B23" s="44"/>
+      <c r="B23" s="42" t="s">
+        <v>68</v>
+      </c>
       <c r="C23" s="43" t="s">
         <v>111</v>
       </c>
@@ -13367,11 +13397,11 @@
       </c>
       <c r="B23" s="48" t="str">
         <f>'SUNDAY SINGLES'!X24</f>
-        <v/>
-      </c>
-      <c r="C23" s="48" t="str">
+        <v>ANDY THOMPSON</v>
+      </c>
+      <c r="C23" s="48">
         <f>'SUNDAY SINGLES'!X25</f>
-        <v/>
+        <v>37</v>
       </c>
       <c r="D23" s="49" t="str">
         <f>'THURSDAY SINGLES'!X20</f>

</xml_diff>

<commit_message>
068 Week 22/23 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="117">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -2670,11 +2670,13 @@
       <c r="X6" s="13">
         <v>36.0</v>
       </c>
-      <c r="Y6" s="15"/>
+      <c r="Y6" s="12">
+        <v>37.0</v>
+      </c>
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>596</v>
+        <v>633</v>
       </c>
     </row>
     <row r="7">
@@ -2735,11 +2737,13 @@
         <v>39.0</v>
       </c>
       <c r="X7" s="14"/>
-      <c r="Y7" s="15"/>
+      <c r="Y7" s="12">
+        <v>32.0</v>
+      </c>
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>537</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8">
@@ -2804,11 +2808,13 @@
       <c r="X8" s="13">
         <v>37.0</v>
       </c>
-      <c r="Y8" s="15"/>
+      <c r="Y8" s="12">
+        <v>35.0</v>
+      </c>
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>590</v>
+        <v>625</v>
       </c>
     </row>
     <row r="9">
@@ -2934,11 +2940,13 @@
       <c r="X10" s="13">
         <v>31.0</v>
       </c>
-      <c r="Y10" s="15"/>
+      <c r="Y10" s="12">
+        <v>30.0</v>
+      </c>
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>536</v>
+        <v>566</v>
       </c>
     </row>
     <row r="11">
@@ -2987,11 +2995,13 @@
       <c r="X11" s="13">
         <v>28.0</v>
       </c>
-      <c r="Y11" s="15"/>
+      <c r="Y11" s="12">
+        <v>28.0</v>
+      </c>
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>280</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12">
@@ -3056,11 +3066,13 @@
       <c r="X12" s="13">
         <v>28.0</v>
       </c>
-      <c r="Y12" s="15"/>
+      <c r="Y12" s="12">
+        <v>38.0</v>
+      </c>
       <c r="Z12" s="16"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>570</v>
+        <v>608</v>
       </c>
     </row>
     <row r="13">
@@ -3115,11 +3127,13 @@
         <v>34.0</v>
       </c>
       <c r="X13" s="14"/>
-      <c r="Y13" s="15"/>
+      <c r="Y13" s="12">
+        <v>36.0</v>
+      </c>
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>433</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14">
@@ -3174,11 +3188,13 @@
       <c r="X14" s="13">
         <v>39.0</v>
       </c>
-      <c r="Y14" s="15"/>
+      <c r="Y14" s="12">
+        <v>35.0</v>
+      </c>
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>412</v>
+        <v>447</v>
       </c>
     </row>
     <row r="15">
@@ -3241,11 +3257,13 @@
         <v>30.0</v>
       </c>
       <c r="X15" s="14"/>
-      <c r="Y15" s="15"/>
+      <c r="Y15" s="12">
+        <v>29.0</v>
+      </c>
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>520</v>
+        <v>549</v>
       </c>
     </row>
     <row r="16">
@@ -3302,11 +3320,13 @@
       <c r="X16" s="13">
         <v>30.0</v>
       </c>
-      <c r="Y16" s="15"/>
+      <c r="Y16" s="12">
+        <v>36.0</v>
+      </c>
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>413</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17">
@@ -3418,11 +3438,13 @@
       <c r="X18" s="12">
         <v>30.0</v>
       </c>
-      <c r="Y18" s="15"/>
+      <c r="Y18" s="12">
+        <v>33.0</v>
+      </c>
       <c r="Z18" s="15"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>371</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -3521,7 +3543,9 @@
       <c r="X20" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="Y20" s="21"/>
+      <c r="Y20" s="21" t="s">
+        <v>99</v>
+      </c>
       <c r="Z20" s="21"/>
       <c r="AA20" s="28"/>
     </row>
@@ -3595,7 +3619,9 @@
       <c r="X21" s="24">
         <v>39.0</v>
       </c>
-      <c r="Y21" s="24"/>
+      <c r="Y21" s="24">
+        <v>38.0</v>
+      </c>
       <c r="Z21" s="24"/>
     </row>
   </sheetData>
@@ -3700,10 +3726,10 @@
         <v>57</v>
       </c>
       <c r="B8" s="32">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="C8" s="33">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="9">
@@ -3714,7 +3740,7 @@
         <v>20.0</v>
       </c>
       <c r="C9" s="33">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="10">
@@ -3722,10 +3748,10 @@
         <v>59</v>
       </c>
       <c r="B10" s="32">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="C10" s="33">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="11">
@@ -3736,7 +3762,7 @@
         <v>10.0</v>
       </c>
       <c r="C11" s="33">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="12">
@@ -3744,7 +3770,7 @@
         <v>61</v>
       </c>
       <c r="B12" s="32">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="C12" s="33">
         <v>15.0</v>
@@ -3777,10 +3803,10 @@
         <v>64</v>
       </c>
       <c r="B15" s="32">
+        <v>30.0</v>
+      </c>
+      <c r="C15" s="33">
         <v>29.0</v>
-      </c>
-      <c r="C15" s="33">
-        <v>28.0</v>
       </c>
     </row>
     <row r="16">
@@ -3835,7 +3861,7 @@
         <v>20.0</v>
       </c>
       <c r="C20" s="33">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="21">
@@ -3846,7 +3872,7 @@
         <v>15.0</v>
       </c>
       <c r="C21" s="33">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="22">
@@ -3876,7 +3902,7 @@
         <v>101</v>
       </c>
       <c r="B24" s="35">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
       <c r="C24" s="36">
         <v>28.0</v>
@@ -8049,7 +8075,9 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="44"/>
-      <c r="C24" s="43"/>
+      <c r="C24" s="43" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="13">
@@ -13426,11 +13454,11 @@
       </c>
       <c r="D24" s="49" t="str">
         <f>'THURSDAY SINGLES'!Y20</f>
-        <v/>
-      </c>
-      <c r="E24" s="48" t="str">
+        <v>DAVE BARNETT</v>
+      </c>
+      <c r="E24" s="48">
         <f>'THURSDAY SINGLES'!Y21</f>
-        <v/>
+        <v>38</v>
       </c>
     </row>
     <row r="25">

</xml_diff>

<commit_message>
070 Week 23/24 data update
</commit_message>
<xml_diff>
--- a/data/SUMMER GOLF 2025.xlsx
+++ b/data/SUMMER GOLF 2025.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="117">
   <si>
     <t>SUMMER GOLF - SUNDAY SINGLES</t>
   </si>
@@ -611,6 +611,9 @@
     <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -665,9 +668,6 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="9" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2698,10 +2698,12 @@
       <c r="Y6" s="12">
         <v>37.0</v>
       </c>
-      <c r="Z6" s="16"/>
+      <c r="Z6" s="25">
+        <v>30.0</v>
+      </c>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>633</v>
+        <v>663</v>
       </c>
     </row>
     <row r="7">
@@ -2765,10 +2767,12 @@
       <c r="Y7" s="12">
         <v>32.0</v>
       </c>
-      <c r="Z7" s="16"/>
+      <c r="Z7" s="25">
+        <v>28.0</v>
+      </c>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>569</v>
+        <v>597</v>
       </c>
     </row>
     <row r="8">
@@ -3094,10 +3098,12 @@
       <c r="Y12" s="12">
         <v>38.0</v>
       </c>
-      <c r="Z12" s="16"/>
+      <c r="Z12" s="25">
+        <v>32.0</v>
+      </c>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>608</v>
+        <v>640</v>
       </c>
     </row>
     <row r="13">
@@ -3216,10 +3222,12 @@
       <c r="Y14" s="12">
         <v>35.0</v>
       </c>
-      <c r="Z14" s="16"/>
+      <c r="Z14" s="25">
+        <v>31.0</v>
+      </c>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>447</v>
+        <v>478</v>
       </c>
     </row>
     <row r="15">
@@ -3285,10 +3293,12 @@
       <c r="Y15" s="12">
         <v>29.0</v>
       </c>
-      <c r="Z15" s="16"/>
+      <c r="Z15" s="25">
+        <v>29.0</v>
+      </c>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>549</v>
+        <v>578</v>
       </c>
     </row>
     <row r="16">
@@ -3348,14 +3358,16 @@
       <c r="Y16" s="12">
         <v>36.0</v>
       </c>
-      <c r="Z16" s="16"/>
+      <c r="Z16" s="25">
+        <v>27.0</v>
+      </c>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>449</v>
+        <v>476</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>67</v>
       </c>
       <c r="C17" s="16"/>
@@ -3402,7 +3414,7 @@
         <v>38.0</v>
       </c>
       <c r="V17" s="14"/>
-      <c r="W17" s="26"/>
+      <c r="W17" s="27"/>
       <c r="X17" s="14"/>
       <c r="Y17" s="15"/>
       <c r="Z17" s="16"/>
@@ -3412,7 +3424,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="28" t="s">
         <v>102</v>
       </c>
       <c r="C18" s="12">
@@ -3466,10 +3478,12 @@
       <c r="Y18" s="12">
         <v>33.0</v>
       </c>
-      <c r="Z18" s="15"/>
+      <c r="Z18" s="12">
+        <v>32.0</v>
+      </c>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>404</v>
+        <v>436</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -3571,8 +3585,10 @@
       <c r="Y20" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="Z20" s="21"/>
-      <c r="AA20" s="28"/>
+      <c r="Z20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA20" s="29"/>
     </row>
     <row r="21">
       <c r="B21" s="23" t="s">
@@ -3647,7 +3663,9 @@
       <c r="Y21" s="24">
         <v>38.0</v>
       </c>
-      <c r="Z21" s="24"/>
+      <c r="Z21" s="24">
+        <v>35.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -3670,13 +3688,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3684,10 +3702,10 @@
       <c r="A2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="33">
         <v>14.0</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="34">
         <v>13.0</v>
       </c>
     </row>
@@ -3695,10 +3713,10 @@
       <c r="A3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="33">
         <v>7.0</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="34">
         <v>6.0</v>
       </c>
     </row>
@@ -3706,10 +3724,10 @@
       <c r="A4" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="33">
         <v>23.0</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="34">
         <v>21.0</v>
       </c>
     </row>
@@ -3717,10 +3735,10 @@
       <c r="A5" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="33">
         <v>13.0</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="34">
         <v>12.0</v>
       </c>
     </row>
@@ -3728,10 +3746,10 @@
       <c r="A6" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="33">
         <v>-1.0</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="34">
         <v>-2.0</v>
       </c>
     </row>
@@ -3739,10 +3757,10 @@
       <c r="A7" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="33">
         <v>11.0</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="34">
         <v>11.0</v>
       </c>
     </row>
@@ -3750,10 +3768,10 @@
       <c r="A8" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="33">
         <v>8.0</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="34">
         <v>7.0</v>
       </c>
     </row>
@@ -3761,10 +3779,10 @@
       <c r="A9" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="33">
         <v>20.0</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="34">
         <v>19.0</v>
       </c>
     </row>
@@ -3772,10 +3790,10 @@
       <c r="A10" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="33">
         <v>6.0</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="34">
         <v>5.0</v>
       </c>
     </row>
@@ -3783,10 +3801,10 @@
       <c r="A11" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="33">
         <v>10.0</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="34">
         <v>8.0</v>
       </c>
     </row>
@@ -3794,10 +3812,10 @@
       <c r="A12" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="33">
         <v>17.0</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="34">
         <v>15.0</v>
       </c>
     </row>
@@ -3805,10 +3823,10 @@
       <c r="A13" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="33">
         <v>22.0</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="34">
         <v>21.0</v>
       </c>
     </row>
@@ -3816,10 +3834,10 @@
       <c r="A14" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="33">
         <v>11.0</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="34">
         <v>10.0</v>
       </c>
     </row>
@@ -3827,10 +3845,10 @@
       <c r="A15" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="33">
         <v>30.0</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="34">
         <v>29.0</v>
       </c>
     </row>
@@ -3838,10 +3856,10 @@
       <c r="A16" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="33">
         <v>14.0</v>
       </c>
-      <c r="C16" s="33">
+      <c r="C16" s="34">
         <v>12.0</v>
       </c>
     </row>
@@ -3849,10 +3867,10 @@
       <c r="A17" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="33">
         <v>7.0</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="34">
         <v>6.0</v>
       </c>
     </row>
@@ -3860,10 +3878,10 @@
       <c r="A18" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="33">
         <v>8.0</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="34">
         <v>7.0</v>
       </c>
     </row>
@@ -3871,21 +3889,21 @@
       <c r="A19" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="33">
         <v>8.0</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="34">
         <v>7.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="33">
         <v>20.0</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="34">
         <v>19.0</v>
       </c>
     </row>
@@ -3893,10 +3911,10 @@
       <c r="A21" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="33">
         <v>15.0</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="34">
         <v>13.0</v>
       </c>
     </row>
@@ -3904,10 +3922,10 @@
       <c r="A22" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B22" s="33">
         <v>15.0</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C22" s="34">
         <v>13.0</v>
       </c>
     </row>
@@ -3915,10 +3933,10 @@
       <c r="A23" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="33">
         <v>29.0</v>
       </c>
-      <c r="C23" s="33">
+      <c r="C23" s="34">
         <v>28.0</v>
       </c>
     </row>
@@ -3926,10 +3944,10 @@
       <c r="A24" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B24" s="36">
         <v>29.0</v>
       </c>
-      <c r="C24" s="36">
+      <c r="C24" s="37">
         <v>28.0</v>
       </c>
     </row>
@@ -7845,21 +7863,21 @@
       <c r="A1" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="39">
+      <c r="A2" s="40">
         <v>1.0</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="42" t="s">
         <v>60</v>
       </c>
     </row>
@@ -7867,10 +7885,10 @@
       <c r="A3" s="13">
         <v>2.0</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="44" t="s">
         <v>54</v>
       </c>
     </row>
@@ -7878,10 +7896,10 @@
       <c r="A4" s="13">
         <v>3.0</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="44" t="s">
         <v>51</v>
       </c>
     </row>
@@ -7889,10 +7907,10 @@
       <c r="A5" s="13">
         <v>4.0</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="44" t="s">
         <v>109</v>
       </c>
     </row>
@@ -7900,10 +7918,10 @@
       <c r="A6" s="13">
         <v>5.0</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="44" t="s">
         <v>99</v>
       </c>
     </row>
@@ -7911,10 +7929,10 @@
       <c r="A7" s="13">
         <v>6.0</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="44" t="s">
         <v>53</v>
       </c>
     </row>
@@ -7922,10 +7940,10 @@
       <c r="A8" s="13">
         <v>7.0</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>67</v>
       </c>
     </row>
@@ -7933,10 +7951,10 @@
       <c r="A9" s="13">
         <v>8.0</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="44" t="s">
         <v>111</v>
       </c>
     </row>
@@ -7944,10 +7962,10 @@
       <c r="A10" s="13">
         <v>9.0</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="44" t="s">
         <v>111</v>
       </c>
       <c r="G10" s="14"/>
@@ -7956,10 +7974,10 @@
       <c r="A11" s="13">
         <v>10.0</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="44" t="s">
         <v>111</v>
       </c>
     </row>
@@ -7967,10 +7985,10 @@
       <c r="A12" s="13">
         <v>11.0</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="44" t="s">
         <v>99</v>
       </c>
     </row>
@@ -7978,10 +7996,10 @@
       <c r="A13" s="13">
         <v>12.0</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="44" t="s">
         <v>111</v>
       </c>
     </row>
@@ -7989,10 +8007,10 @@
       <c r="A14" s="13">
         <v>13.0</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="44" t="s">
         <v>60</v>
       </c>
     </row>
@@ -8000,10 +8018,10 @@
       <c r="A15" s="13">
         <v>14.0</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="44" t="s">
         <v>57</v>
       </c>
     </row>
@@ -8011,10 +8029,10 @@
       <c r="A16" s="13">
         <v>15.0</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="44" t="s">
         <v>63</v>
       </c>
     </row>
@@ -8022,10 +8040,10 @@
       <c r="A17" s="13">
         <v>16.0</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="44" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8033,10 +8051,10 @@
       <c r="A18" s="13">
         <v>17.0</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="44" t="s">
         <v>57</v>
       </c>
     </row>
@@ -8044,10 +8062,10 @@
       <c r="A19" s="13">
         <v>18.0</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="44" t="s">
         <v>51</v>
       </c>
     </row>
@@ -8055,10 +8073,10 @@
       <c r="A20" s="13">
         <v>19.0</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="44" t="s">
         <v>60</v>
       </c>
     </row>
@@ -8066,10 +8084,10 @@
       <c r="A21" s="13">
         <v>20.0</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="44" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8077,10 +8095,10 @@
       <c r="A22" s="13">
         <v>21.0</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="44" t="s">
         <v>59</v>
       </c>
     </row>
@@ -8088,10 +8106,10 @@
       <c r="A23" s="13">
         <v>22.0</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="44" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8099,10 +8117,10 @@
       <c r="A24" s="13">
         <v>23.0</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="44" t="s">
         <v>101</v>
       </c>
     </row>
@@ -8110,8 +8128,10 @@
       <c r="A25" s="13">
         <v>24.0</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="44" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="14"/>
@@ -13502,11 +13522,11 @@
       </c>
       <c r="D25" s="48" t="str">
         <f>'THURSDAY SINGLES'!Z20</f>
-        <v/>
-      </c>
-      <c r="E25" s="47" t="str">
+        <v>ADY STEANE</v>
+      </c>
+      <c r="E25" s="47">
         <f>'THURSDAY SINGLES'!Z21</f>
-        <v/>
+        <v>35</v>
       </c>
     </row>
     <row r="26">

</xml_diff>